<commit_message>
updated page-data.xlsx file with new data
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -1350,12 +1350,12 @@
       <c r="H3" s="12">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="I3" s="12">
         <f>COUNTIF(B:B,"NOT INDEXED")
 </f>
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="J3" s="12">
         <f>COUNTIF(B:B,"INDEXED")
@@ -1464,12 +1464,12 @@
       <c r="H7" s="12">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="I7" s="12">
         <f>COUNTIF(C:C,"NOT INDEXED")
 </f>
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="J7" s="12">
         <f>COUNTIF(C:C,"INDEXED")
@@ -1692,7 +1692,7 @@
       <c r="H15" s="12">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="I15" s="12">
         <f>COUNTIF(E:E,"INVALID")
@@ -1702,7 +1702,7 @@
       <c r="J15" s="12">
         <f>COUNTIF(E:E,"VALID")
 </f>
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16">
@@ -1939,7 +1939,7 @@
         <v>9</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1983,7 +1983,7 @@
         <v>9</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -2018,10 +2018,10 @@
         <v>46</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>9</v>
@@ -2049,7 +2049,7 @@
         <v>9</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -2062,10 +2062,10 @@
         <v>48</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>9</v>
@@ -2093,7 +2093,7 @@
         <v>9</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -2401,7 +2401,7 @@
         <v>14</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -2414,10 +2414,10 @@
         <v>64</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>9</v>
@@ -2436,10 +2436,10 @@
         <v>65</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>9</v>
@@ -2458,10 +2458,10 @@
         <v>66</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>9</v>
@@ -3140,10 +3140,10 @@
         <v>97</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>9</v>
@@ -3162,10 +3162,10 @@
         <v>98</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>9</v>
@@ -3206,10 +3206,10 @@
         <v>100</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>9</v>
@@ -3228,10 +3228,10 @@
         <v>101</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>9</v>
@@ -3250,10 +3250,10 @@
         <v>102</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>9</v>
@@ -3272,10 +3272,10 @@
         <v>103</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D87" s="7" t="s">
         <v>9</v>
@@ -3932,10 +3932,10 @@
         <v>133</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D117" s="7" t="s">
         <v>9</v>
@@ -5657,7 +5657,7 @@
         <v>9</v>
       </c>
       <c r="E195" s="7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F195" s="2"/>
       <c r="G195" s="2"/>
@@ -5679,7 +5679,7 @@
         <v>9</v>
       </c>
       <c r="E196" s="7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F196" s="2"/>
       <c r="G196" s="2"/>

</xml_diff>

<commit_message>
updated page data JSON and XLSX files
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -51,13 +51,13 @@
     <t>https://changelog.heatlabs.net</t>
   </si>
   <si>
-    <t>https://heatlabs.net/</t>
-  </si>
-  <si>
     <t>HTTPS</t>
   </si>
   <si>
     <t>VALID</t>
+  </si>
+  <si>
+    <t>https://heatlabs.net</t>
   </si>
   <si>
     <t>https://heatlabs.net/agents</t>
@@ -1298,10 +1298,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="10">
@@ -1322,7 +1322,7 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>7</v>
@@ -1331,10 +1331,10 @@
         <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1352,7 +1352,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>9</v>
@@ -1375,10 +1375,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="7" t="s">
@@ -1402,16 +1402,16 @@
         <v>8</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -1421,7 +1421,7 @@
       <c r="I7" s="10">
         <f>COUNTIF(C:C,"INDEXED")
 </f>
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
@@ -1435,10 +1435,10 @@
         <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1456,10 +1456,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="3" t="s">
@@ -1479,10 +1479,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="11" t="s">
@@ -1492,7 +1492,7 @@
         <v>23</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -1506,16 +1506,16 @@
         <v>8</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1525,7 +1525,7 @@
       <c r="I11" s="10">
         <f>COUNTIF(D:D,"HTTPS")
 </f>
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12">
@@ -1539,10 +1539,10 @@
         <v>8</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1560,10 +1560,10 @@
         <v>8</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="3" t="s">
@@ -1596,7 +1596,7 @@
         <v>29</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -1610,16 +1610,16 @@
         <v>8</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -1629,7 +1629,7 @@
       <c r="I15" s="10">
         <f>COUNTIF(E:E,"VALID")
 </f>
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16">
@@ -1643,10 +1643,10 @@
         <v>8</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1664,10 +1664,10 @@
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1703,13 +1703,13 @@
         <v>7</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1727,10 +1727,10 @@
         <v>8</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1748,10 +1748,10 @@
         <v>8</v>
       </c>
       <c r="D21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1769,10 +1769,10 @@
         <v>8</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1790,10 +1790,10 @@
         <v>8</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1811,10 +1811,10 @@
         <v>8</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1832,10 +1832,10 @@
         <v>8</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1874,10 +1874,10 @@
         <v>8</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1895,10 +1895,10 @@
         <v>8</v>
       </c>
       <c r="D28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1916,10 +1916,10 @@
         <v>8</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -1937,10 +1937,10 @@
         <v>8</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1958,10 +1958,10 @@
         <v>8</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1979,10 +1979,10 @@
         <v>8</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -2000,10 +2000,10 @@
         <v>7</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -2021,10 +2021,10 @@
         <v>7</v>
       </c>
       <c r="D34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -2042,10 +2042,10 @@
         <v>7</v>
       </c>
       <c r="D35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2084,10 +2084,10 @@
         <v>7</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -2126,10 +2126,10 @@
         <v>7</v>
       </c>
       <c r="D39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -2189,10 +2189,10 @@
         <v>7</v>
       </c>
       <c r="D42" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -2210,10 +2210,10 @@
         <v>8</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -2252,10 +2252,10 @@
         <v>8</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -2273,10 +2273,10 @@
         <v>7</v>
       </c>
       <c r="D46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -2294,10 +2294,10 @@
         <v>8</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -2315,10 +2315,10 @@
         <v>8</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -2336,10 +2336,10 @@
         <v>8</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -2651,10 +2651,10 @@
         <v>8</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -2672,10 +2672,10 @@
         <v>7</v>
       </c>
       <c r="D65" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
@@ -2693,10 +2693,10 @@
         <v>8</v>
       </c>
       <c r="D66" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -2714,10 +2714,10 @@
         <v>8</v>
       </c>
       <c r="D67" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E67" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -2735,10 +2735,10 @@
         <v>8</v>
       </c>
       <c r="D68" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E68" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
@@ -2777,10 +2777,10 @@
         <v>8</v>
       </c>
       <c r="D70" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
@@ -2798,10 +2798,10 @@
         <v>8</v>
       </c>
       <c r="D71" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
@@ -2840,10 +2840,10 @@
         <v>8</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -2882,10 +2882,10 @@
         <v>8</v>
       </c>
       <c r="D75" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E75" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
@@ -2903,10 +2903,10 @@
         <v>8</v>
       </c>
       <c r="D76" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
@@ -2945,10 +2945,10 @@
         <v>8</v>
       </c>
       <c r="D78" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
@@ -2966,10 +2966,10 @@
         <v>8</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
@@ -2987,10 +2987,10 @@
         <v>8</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
@@ -3029,10 +3029,10 @@
         <v>8</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -3092,10 +3092,10 @@
         <v>8</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
@@ -3533,10 +3533,10 @@
         <v>8</v>
       </c>
       <c r="D106" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E106" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
@@ -3722,10 +3722,10 @@
         <v>8</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
@@ -3911,7 +3911,7 @@
         <v>10</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E124" s="6" t="s">
         <v>9</v>
@@ -4163,10 +4163,10 @@
         <v>10</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
@@ -5360,10 +5360,10 @@
         <v>8</v>
       </c>
       <c r="D193" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E193" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F193" s="2"/>
       <c r="G193" s="2"/>
@@ -5381,10 +5381,10 @@
         <v>8</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E194" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F194" s="2"/>
       <c r="G194" s="2"/>
@@ -5402,10 +5402,10 @@
         <v>8</v>
       </c>
       <c r="D195" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E195" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E195" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="F195" s="2"/>
       <c r="G195" s="2"/>
@@ -5423,10 +5423,10 @@
         <v>7</v>
       </c>
       <c r="D196" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E196" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E196" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F196" s="2"/>
       <c r="G196" s="2"/>
@@ -5444,10 +5444,10 @@
         <v>7</v>
       </c>
       <c r="D197" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E197" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F197" s="2"/>
       <c r="G197" s="2"/>
@@ -5486,10 +5486,10 @@
         <v>7</v>
       </c>
       <c r="D199" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E199" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E199" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F199" s="2"/>
       <c r="G199" s="2"/>
@@ -5507,10 +5507,10 @@
         <v>8</v>
       </c>
       <c r="D200" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E200" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F200" s="2"/>
       <c r="G200" s="2"/>
@@ -5528,10 +5528,10 @@
         <v>7</v>
       </c>
       <c r="D201" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E201" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E201" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F201" s="2"/>
       <c r="G201" s="2"/>
@@ -5570,10 +5570,10 @@
         <v>8</v>
       </c>
       <c r="D203" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E203" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E203" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F203" s="2"/>
       <c r="G203" s="2"/>
@@ -5591,10 +5591,10 @@
         <v>7</v>
       </c>
       <c r="D204" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E204" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E204" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F204" s="2"/>
       <c r="G204" s="2"/>
@@ -5633,10 +5633,10 @@
         <v>8</v>
       </c>
       <c r="D206" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E206" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E206" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F206" s="2"/>
       <c r="G206" s="2"/>
@@ -5654,10 +5654,10 @@
         <v>7</v>
       </c>
       <c r="D207" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E207" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E207" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F207" s="2"/>
       <c r="G207" s="2"/>
@@ -5780,10 +5780,10 @@
         <v>7</v>
       </c>
       <c r="D213" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E213" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E213" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="F213" s="2"/>
       <c r="G213" s="2"/>
@@ -5801,10 +5801,10 @@
         <v>7</v>
       </c>
       <c r="D214" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E214" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F214" s="2"/>
       <c r="G214" s="2"/>
@@ -5822,10 +5822,10 @@
         <v>7</v>
       </c>
       <c r="D215" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E215" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F215" s="2"/>
       <c r="G215" s="2"/>
@@ -5843,10 +5843,10 @@
         <v>7</v>
       </c>
       <c r="D216" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E216" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F216" s="2"/>
       <c r="G216" s="2"/>
@@ -5864,10 +5864,10 @@
         <v>7</v>
       </c>
       <c r="D217" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E217" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F217" s="2"/>
       <c r="G217" s="2"/>
@@ -5885,10 +5885,10 @@
         <v>7</v>
       </c>
       <c r="D218" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E218" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F218" s="2"/>
       <c r="G218" s="2"/>
@@ -5927,10 +5927,10 @@
         <v>8</v>
       </c>
       <c r="D220" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E220" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E220" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F220" s="2"/>
       <c r="G220" s="2"/>
@@ -5948,10 +5948,10 @@
         <v>7</v>
       </c>
       <c r="D221" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E221" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E221" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F221" s="2"/>
       <c r="G221" s="2"/>
@@ -5969,10 +5969,10 @@
         <v>7</v>
       </c>
       <c r="D222" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E222" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E222" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F222" s="2"/>
       <c r="G222" s="2"/>
@@ -5990,10 +5990,10 @@
         <v>7</v>
       </c>
       <c r="D223" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E223" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F223" s="2"/>
       <c r="G223" s="2"/>
@@ -6011,10 +6011,10 @@
         <v>7</v>
       </c>
       <c r="D224" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E224" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F224" s="2"/>
       <c r="G224" s="2"/>
@@ -6032,10 +6032,10 @@
         <v>7</v>
       </c>
       <c r="D225" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E225" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E225" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F225" s="2"/>
       <c r="G225" s="2"/>
@@ -6053,10 +6053,10 @@
         <v>8</v>
       </c>
       <c r="D226" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E226" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E226" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F226" s="2"/>
       <c r="G226" s="2"/>
@@ -6074,10 +6074,10 @@
         <v>7</v>
       </c>
       <c r="D227" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E227" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E227" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F227" s="2"/>
       <c r="G227" s="2"/>
@@ -6095,10 +6095,10 @@
         <v>7</v>
       </c>
       <c r="D228" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E228" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E228" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F228" s="2"/>
       <c r="G228" s="2"/>
@@ -6116,10 +6116,10 @@
         <v>7</v>
       </c>
       <c r="D229" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E229" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F229" s="2"/>
       <c r="G229" s="2"/>
@@ -6137,10 +6137,10 @@
         <v>8</v>
       </c>
       <c r="D230" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F230" s="2"/>
       <c r="G230" s="2"/>
@@ -6155,13 +6155,13 @@
         <v>7</v>
       </c>
       <c r="C231" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D231" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E231" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F231" s="2"/>
       <c r="G231" s="2"/>
@@ -6179,10 +6179,10 @@
         <v>8</v>
       </c>
       <c r="D232" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E232" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F232" s="2"/>
       <c r="G232" s="2"/>
@@ -6200,10 +6200,10 @@
         <v>8</v>
       </c>
       <c r="D233" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E233" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E233" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F233" s="2"/>
       <c r="G233" s="2"/>
@@ -6263,10 +6263,10 @@
         <v>7</v>
       </c>
       <c r="D236" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E236" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E236" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F236" s="2"/>
       <c r="G236" s="2"/>
@@ -6284,10 +6284,10 @@
         <v>7</v>
       </c>
       <c r="D237" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E237" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F237" s="2"/>
       <c r="G237" s="2"/>
@@ -6305,10 +6305,10 @@
         <v>7</v>
       </c>
       <c r="D238" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E238" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E238" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F238" s="2"/>
       <c r="G238" s="2"/>
@@ -6326,10 +6326,10 @@
         <v>8</v>
       </c>
       <c r="D239" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F239" s="2"/>
       <c r="G239" s="2"/>
@@ -6347,10 +6347,10 @@
         <v>7</v>
       </c>
       <c r="D240" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F240" s="2"/>
       <c r="G240" s="2"/>
@@ -6368,10 +6368,10 @@
         <v>8</v>
       </c>
       <c r="D241" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E241" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F241" s="2"/>
       <c r="G241" s="2"/>
@@ -6389,10 +6389,10 @@
         <v>8</v>
       </c>
       <c r="D242" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E242" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E242" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F242" s="2"/>
       <c r="G242" s="2"/>
@@ -6410,7 +6410,7 @@
         <v>7</v>
       </c>
       <c r="D243" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E243" s="6" t="s">
         <v>9</v>
@@ -6431,10 +6431,10 @@
         <v>7</v>
       </c>
       <c r="D244" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E244" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E244" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F244" s="2"/>
       <c r="G244" s="2"/>
@@ -6452,10 +6452,10 @@
         <v>7</v>
       </c>
       <c r="D245" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E245" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E245" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="F245" s="2"/>
       <c r="G245" s="2"/>

</xml_diff>

<commit_message>
updated page data files
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -240,7 +240,7 @@
     <t>https://heatlabs.net/bug-hunting/titan-dummies-respawn-glitch</t>
   </si>
   <si>
-    <t>https://heatlabs.net/bug-hunting/unlocking_the_camera</t>
+    <t>https://heatlabs.net/bug-hunting/unlocking-the-camera</t>
   </si>
   <si>
     <t>https://heatlabs.net/bug-hunting/who-is-pcw-bug-hunters</t>
@@ -1307,17 +1307,17 @@
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
 </f>
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="I3" s="10">
         <f>COUNTIF(B:B,"INDEXED")
 </f>
-        <v>74</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4">
@@ -1399,7 +1399,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>12</v>
@@ -1411,17 +1411,17 @@
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
 </f>
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="I7" s="10">
         <f>COUNTIF(C:C,"INDEXED")
 </f>
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8">
@@ -1453,7 +1453,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>12</v>
@@ -1503,7 +1503,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>12</v>
@@ -1515,7 +1515,7 @@
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1525,7 +1525,7 @@
       <c r="I11" s="10">
         <f>COUNTIF(D:D,"HTTPS")
 </f>
-        <v>82</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12">
@@ -1640,7 +1640,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>12</v>
@@ -1724,7 +1724,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>12</v>
@@ -1763,7 +1763,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>8</v>
@@ -1784,7 +1784,7 @@
         <v>38</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>8</v>
@@ -1805,7 +1805,7 @@
         <v>39</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>8</v>
@@ -1826,10 +1826,10 @@
         <v>40</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>12</v>
@@ -1868,7 +1868,7 @@
         <v>42</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>8</v>
@@ -1910,7 +1910,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>8</v>
@@ -1931,7 +1931,7 @@
         <v>45</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>8</v>
@@ -1952,7 +1952,7 @@
         <v>46</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>8</v>
@@ -1973,7 +1973,7 @@
         <v>47</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>8</v>
@@ -2204,7 +2204,7 @@
         <v>58</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>8</v>
@@ -2246,7 +2246,7 @@
         <v>60</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>8</v>
@@ -2288,7 +2288,7 @@
         <v>62</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>8</v>
@@ -2309,7 +2309,7 @@
         <v>63</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>8</v>
@@ -2330,7 +2330,7 @@
         <v>64</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>8</v>
@@ -2357,7 +2357,7 @@
         <v>8</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>9</v>
@@ -2378,7 +2378,7 @@
         <v>8</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>9</v>
@@ -2399,7 +2399,7 @@
         <v>8</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>9</v>
@@ -2420,7 +2420,7 @@
         <v>8</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>9</v>
@@ -2441,7 +2441,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>9</v>
@@ -2462,7 +2462,7 @@
         <v>8</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>9</v>
@@ -2483,7 +2483,7 @@
         <v>8</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>9</v>
@@ -2504,7 +2504,7 @@
         <v>8</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>9</v>
@@ -2525,7 +2525,7 @@
         <v>8</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>9</v>
@@ -2546,7 +2546,7 @@
         <v>8</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>9</v>
@@ -2582,10 +2582,10 @@
         <v>76</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>9</v>
@@ -2603,10 +2603,10 @@
         <v>77</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>9</v>
@@ -2774,7 +2774,7 @@
         <v>7</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>12</v>
@@ -2834,7 +2834,7 @@
         <v>88</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>8</v>
@@ -2960,7 +2960,7 @@
         <v>94</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>8</v>
@@ -2981,7 +2981,7 @@
         <v>95</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>8</v>
@@ -3023,7 +3023,7 @@
         <v>97</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>8</v>
@@ -3065,7 +3065,7 @@
         <v>99</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>8</v>
@@ -3086,7 +3086,7 @@
         <v>100</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>8</v>
@@ -3530,7 +3530,7 @@
         <v>7</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>12</v>
@@ -3716,7 +3716,7 @@
         <v>130</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>8</v>
@@ -3806,7 +3806,7 @@
         <v>8</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E119" s="6" t="s">
         <v>9</v>
@@ -4373,7 +4373,7 @@
         <v>10</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E146" s="6" t="s">
         <v>9</v>
@@ -4415,7 +4415,7 @@
         <v>10</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E148" s="6" t="s">
         <v>9</v>
@@ -4598,10 +4598,10 @@
         <v>172</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D157" s="6" t="s">
         <v>9</v>
@@ -4619,10 +4619,10 @@
         <v>173</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D158" s="6" t="s">
         <v>9</v>
@@ -4640,10 +4640,10 @@
         <v>174</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D159" s="6" t="s">
         <v>9</v>
@@ -4913,10 +4913,10 @@
         <v>187</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D172" s="6" t="s">
         <v>9</v>
@@ -5018,10 +5018,10 @@
         <v>192</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D177" s="6" t="s">
         <v>9</v>
@@ -5039,10 +5039,10 @@
         <v>193</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D178" s="6" t="s">
         <v>9</v>
@@ -5123,10 +5123,10 @@
         <v>197</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C182" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D182" s="6" t="s">
         <v>9</v>
@@ -5144,10 +5144,10 @@
         <v>198</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D183" s="6" t="s">
         <v>9</v>
@@ -5165,10 +5165,10 @@
         <v>199</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C184" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D184" s="6" t="s">
         <v>9</v>
@@ -5186,10 +5186,10 @@
         <v>200</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D185" s="6" t="s">
         <v>9</v>
@@ -5207,10 +5207,10 @@
         <v>201</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D186" s="6" t="s">
         <v>9</v>
@@ -5354,7 +5354,7 @@
         <v>208</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C193" s="6" t="s">
         <v>8</v>
@@ -5375,7 +5375,7 @@
         <v>209</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C194" s="6" t="s">
         <v>8</v>
@@ -5399,7 +5399,7 @@
         <v>7</v>
       </c>
       <c r="C195" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D195" s="6" t="s">
         <v>12</v>
@@ -5903,7 +5903,7 @@
         <v>8</v>
       </c>
       <c r="C219" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D219" s="6" t="s">
         <v>9</v>
@@ -5924,7 +5924,7 @@
         <v>7</v>
       </c>
       <c r="C220" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D220" s="6" t="s">
         <v>12</v>
@@ -6134,7 +6134,7 @@
         <v>7</v>
       </c>
       <c r="C230" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D230" s="6" t="s">
         <v>9</v>
@@ -6176,7 +6176,7 @@
         <v>8</v>
       </c>
       <c r="C232" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D232" s="6" t="s">
         <v>12</v>
@@ -6323,7 +6323,7 @@
         <v>7</v>
       </c>
       <c r="C239" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D239" s="6" t="s">
         <v>9</v>
@@ -6386,7 +6386,7 @@
         <v>7</v>
       </c>
       <c r="C242" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D242" s="6" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
validated all breadcrumbs data in page data files
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="266">
   <si>
     <t>-PAGE-</t>
   </si>
@@ -808,6 +808,9 @@
   </si>
   <si>
     <t>https://status.heatlabs.net</t>
+  </si>
+  <si>
+    <t>https://discord.heatlabs.net</t>
   </si>
 </sst>
 </file>
@@ -1307,7 +1310,7 @@
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
@@ -1378,7 +1381,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="7" t="s">
@@ -1405,13 +1408,13 @@
         <v>12</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -1438,7 +1441,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1459,7 +1462,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="3" t="s">
@@ -1482,7 +1485,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="11" t="s">
@@ -1515,7 +1518,7 @@
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1542,7 +1545,7 @@
         <v>12</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1563,7 +1566,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="3" t="s">
@@ -1613,13 +1616,13 @@
         <v>12</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -1629,7 +1632,7 @@
       <c r="I15" s="10">
         <f>COUNTIF(E:E,"VALID")
 </f>
-        <v>85</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16">
@@ -1646,7 +1649,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1667,7 +1670,7 @@
         <v>12</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1709,7 +1712,7 @@
         <v>12</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1730,7 +1733,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1751,7 +1754,7 @@
         <v>12</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1814,7 +1817,7 @@
         <v>12</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1961,7 +1964,7 @@
         <v>12</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -2045,7 +2048,7 @@
         <v>12</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2129,7 +2132,7 @@
         <v>12</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -2192,7 +2195,7 @@
         <v>9</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -2360,7 +2363,7 @@
         <v>12</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -2381,7 +2384,7 @@
         <v>12</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -2402,7 +2405,7 @@
         <v>12</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -2423,7 +2426,7 @@
         <v>12</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -2444,7 +2447,7 @@
         <v>12</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -2465,7 +2468,7 @@
         <v>12</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -2486,7 +2489,7 @@
         <v>12</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -2507,7 +2510,7 @@
         <v>12</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -2528,7 +2531,7 @@
         <v>12</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -2549,7 +2552,7 @@
         <v>12</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -2591,7 +2594,7 @@
         <v>9</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -2612,7 +2615,7 @@
         <v>9</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
@@ -2696,7 +2699,7 @@
         <v>12</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -2717,7 +2720,7 @@
         <v>12</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -2738,7 +2741,7 @@
         <v>12</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
@@ -2780,7 +2783,7 @@
         <v>12</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
@@ -2906,7 +2909,7 @@
         <v>12</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
@@ -3116,7 +3119,7 @@
         <v>9</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
@@ -3137,7 +3140,7 @@
         <v>9</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -3158,7 +3161,7 @@
         <v>9</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -3179,7 +3182,7 @@
         <v>9</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
@@ -3389,7 +3392,7 @@
         <v>9</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -3410,7 +3413,7 @@
         <v>9</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -3431,7 +3434,7 @@
         <v>9</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
@@ -3452,7 +3455,7 @@
         <v>9</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
@@ -3473,7 +3476,7 @@
         <v>9</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
@@ -3494,7 +3497,7 @@
         <v>9</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
@@ -3536,7 +3539,7 @@
         <v>12</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
@@ -3578,7 +3581,7 @@
         <v>9</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
@@ -3641,7 +3644,7 @@
         <v>9</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
@@ -3662,7 +3665,7 @@
         <v>9</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
@@ -3725,7 +3728,7 @@
         <v>12</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
@@ -3746,7 +3749,7 @@
         <v>9</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
@@ -3767,7 +3770,7 @@
         <v>9</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
@@ -3809,7 +3812,7 @@
         <v>12</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
@@ -3830,7 +3833,7 @@
         <v>9</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
@@ -3851,7 +3854,7 @@
         <v>9</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
@@ -3872,7 +3875,7 @@
         <v>9</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
@@ -3893,7 +3896,7 @@
         <v>9</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
@@ -3914,7 +3917,7 @@
         <v>12</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
@@ -3935,7 +3938,7 @@
         <v>9</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
@@ -3956,7 +3959,7 @@
         <v>9</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
@@ -3977,7 +3980,7 @@
         <v>9</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
@@ -3998,7 +4001,7 @@
         <v>9</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
@@ -4040,7 +4043,7 @@
         <v>9</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
@@ -4061,7 +4064,7 @@
         <v>9</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
@@ -4082,7 +4085,7 @@
         <v>9</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
@@ -4103,7 +4106,7 @@
         <v>9</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
@@ -4124,7 +4127,7 @@
         <v>9</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
@@ -4145,7 +4148,7 @@
         <v>9</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
@@ -4166,7 +4169,7 @@
         <v>12</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
@@ -4187,7 +4190,7 @@
         <v>9</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
@@ -4208,7 +4211,7 @@
         <v>9</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
@@ -4229,7 +4232,7 @@
         <v>9</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
@@ -4250,7 +4253,7 @@
         <v>9</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
@@ -4271,7 +4274,7 @@
         <v>9</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
@@ -4292,7 +4295,7 @@
         <v>9</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
@@ -4313,7 +4316,7 @@
         <v>9</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
@@ -4334,7 +4337,7 @@
         <v>9</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
@@ -4355,7 +4358,7 @@
         <v>9</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
@@ -4397,7 +4400,7 @@
         <v>9</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
@@ -4439,7 +4442,7 @@
         <v>9</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
@@ -4523,7 +4526,7 @@
         <v>9</v>
       </c>
       <c r="E153" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F153" s="2"/>
       <c r="G153" s="2"/>
@@ -4649,7 +4652,7 @@
         <v>9</v>
       </c>
       <c r="E159" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F159" s="2"/>
       <c r="G159" s="2"/>
@@ -4733,7 +4736,7 @@
         <v>9</v>
       </c>
       <c r="E163" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F163" s="2"/>
       <c r="G163" s="2"/>
@@ -4796,7 +4799,7 @@
         <v>9</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F166" s="2"/>
       <c r="G166" s="2"/>
@@ -4817,7 +4820,7 @@
         <v>9</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F167" s="2"/>
       <c r="G167" s="2"/>
@@ -4838,7 +4841,7 @@
         <v>9</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F168" s="2"/>
       <c r="G168" s="2"/>
@@ -4859,7 +4862,7 @@
         <v>9</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F169" s="2"/>
       <c r="G169" s="2"/>
@@ -4880,7 +4883,7 @@
         <v>9</v>
       </c>
       <c r="E170" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F170" s="2"/>
       <c r="G170" s="2"/>
@@ -4901,7 +4904,7 @@
         <v>9</v>
       </c>
       <c r="E171" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F171" s="2"/>
       <c r="G171" s="2"/>
@@ -5006,7 +5009,7 @@
         <v>9</v>
       </c>
       <c r="E176" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F176" s="2"/>
       <c r="G176" s="2"/>
@@ -5153,7 +5156,7 @@
         <v>9</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F183" s="2"/>
       <c r="G183" s="2"/>
@@ -5174,7 +5177,7 @@
         <v>9</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
@@ -5216,7 +5219,7 @@
         <v>9</v>
       </c>
       <c r="E186" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F186" s="2"/>
       <c r="G186" s="2"/>
@@ -5426,7 +5429,7 @@
         <v>12</v>
       </c>
       <c r="E196" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F196" s="2"/>
       <c r="G196" s="2"/>
@@ -5489,7 +5492,7 @@
         <v>12</v>
       </c>
       <c r="E199" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F199" s="2"/>
       <c r="G199" s="2"/>
@@ -5531,7 +5534,7 @@
         <v>12</v>
       </c>
       <c r="E201" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F201" s="2"/>
       <c r="G201" s="2"/>
@@ -5573,7 +5576,7 @@
         <v>12</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F203" s="2"/>
       <c r="G203" s="2"/>
@@ -5762,7 +5765,7 @@
         <v>9</v>
       </c>
       <c r="E212" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F212" s="2"/>
       <c r="G212" s="2"/>
@@ -5825,7 +5828,7 @@
         <v>9</v>
       </c>
       <c r="E215" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F215" s="2"/>
       <c r="G215" s="2"/>
@@ -5930,7 +5933,7 @@
         <v>12</v>
       </c>
       <c r="E220" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F220" s="2"/>
       <c r="G220" s="2"/>
@@ -5951,7 +5954,7 @@
         <v>12</v>
       </c>
       <c r="E221" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F221" s="2"/>
       <c r="G221" s="2"/>
@@ -5972,7 +5975,7 @@
         <v>12</v>
       </c>
       <c r="E222" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F222" s="2"/>
       <c r="G222" s="2"/>
@@ -6035,7 +6038,7 @@
         <v>12</v>
       </c>
       <c r="E225" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F225" s="2"/>
       <c r="G225" s="2"/>
@@ -6056,7 +6059,7 @@
         <v>12</v>
       </c>
       <c r="E226" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F226" s="2"/>
       <c r="G226" s="2"/>
@@ -6077,7 +6080,7 @@
         <v>12</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F227" s="2"/>
       <c r="G227" s="2"/>
@@ -6182,7 +6185,7 @@
         <v>12</v>
       </c>
       <c r="E232" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F232" s="2"/>
       <c r="G232" s="2"/>
@@ -6203,7 +6206,7 @@
         <v>12</v>
       </c>
       <c r="E233" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F233" s="2"/>
       <c r="G233" s="2"/>
@@ -6266,7 +6269,7 @@
         <v>12</v>
       </c>
       <c r="E236" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F236" s="2"/>
       <c r="G236" s="2"/>
@@ -6308,7 +6311,7 @@
         <v>12</v>
       </c>
       <c r="E238" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F238" s="2"/>
       <c r="G238" s="2"/>
@@ -6371,7 +6374,7 @@
         <v>12</v>
       </c>
       <c r="E241" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F241" s="2"/>
       <c r="G241" s="2"/>
@@ -6434,7 +6437,7 @@
         <v>12</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F244" s="2"/>
       <c r="G244" s="2"/>
@@ -6455,7 +6458,7 @@
         <v>12</v>
       </c>
       <c r="E245" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F245" s="2"/>
       <c r="G245" s="2"/>
@@ -6547,11 +6550,21 @@
       <c r="I249" s="2"/>
     </row>
     <row r="250">
-      <c r="A250" s="14"/>
-      <c r="B250" s="6"/>
-      <c r="C250" s="6"/>
-      <c r="D250" s="6"/>
-      <c r="E250" s="6"/>
+      <c r="A250" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B250" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C250" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D250" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E250" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="F250" s="2"/>
       <c r="G250" s="2"/>
       <c r="H250" s="2"/>
@@ -14992,7 +15005,8 @@
     <hyperlink r:id="rId246" ref="A247"/>
     <hyperlink r:id="rId247" ref="A248"/>
     <hyperlink r:id="rId248" ref="A249"/>
+    <hyperlink r:id="rId249" ref="A250"/>
   </hyperlinks>
-  <drawing r:id="rId249"/>
+  <drawing r:id="rId250"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
validated all https data in page data files
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -1378,7 +1378,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>9</v>
@@ -1405,7 +1405,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>9</v>
@@ -1438,7 +1438,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>9</v>
@@ -1459,7 +1459,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>9</v>
@@ -1482,7 +1482,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>9</v>
@@ -1518,7 +1518,7 @@
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1528,7 +1528,7 @@
       <c r="I11" s="10">
         <f>COUNTIF(D:D,"HTTPS")
 </f>
-        <v>95</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12">
@@ -1542,7 +1542,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>9</v>
@@ -1563,7 +1563,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>9</v>
@@ -1613,7 +1613,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>9</v>
@@ -1646,7 +1646,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>9</v>
@@ -1667,7 +1667,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>9</v>
@@ -1709,7 +1709,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>9</v>
@@ -1730,7 +1730,7 @@
         <v>7</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>9</v>
@@ -1751,7 +1751,7 @@
         <v>8</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>9</v>
@@ -1814,7 +1814,7 @@
         <v>7</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>9</v>
@@ -1961,7 +1961,7 @@
         <v>8</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>9</v>
@@ -2045,7 +2045,7 @@
         <v>7</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>9</v>
@@ -2129,7 +2129,7 @@
         <v>7</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>9</v>
@@ -2591,7 +2591,7 @@
         <v>8</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>13</v>
@@ -2612,7 +2612,7 @@
         <v>8</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>13</v>
@@ -2696,7 +2696,7 @@
         <v>8</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>9</v>
@@ -2717,7 +2717,7 @@
         <v>8</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>9</v>
@@ -2738,7 +2738,7 @@
         <v>7</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>9</v>
@@ -2780,7 +2780,7 @@
         <v>7</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>9</v>
@@ -2906,7 +2906,7 @@
         <v>8</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>9</v>
@@ -3116,7 +3116,7 @@
         <v>8</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>13</v>
@@ -3137,7 +3137,7 @@
         <v>8</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>13</v>
@@ -3158,7 +3158,7 @@
         <v>8</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>13</v>
@@ -3179,7 +3179,7 @@
         <v>8</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>13</v>
@@ -3389,7 +3389,7 @@
         <v>8</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>13</v>
@@ -3410,7 +3410,7 @@
         <v>8</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>13</v>
@@ -3431,7 +3431,7 @@
         <v>8</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E101" s="6" t="s">
         <v>13</v>
@@ -3452,7 +3452,7 @@
         <v>8</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E102" s="6" t="s">
         <v>13</v>
@@ -3473,7 +3473,7 @@
         <v>8</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E103" s="6" t="s">
         <v>13</v>
@@ -3494,7 +3494,7 @@
         <v>8</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>13</v>
@@ -3536,7 +3536,7 @@
         <v>7</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>9</v>
@@ -3578,7 +3578,7 @@
         <v>8</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>13</v>
@@ -3641,7 +3641,7 @@
         <v>8</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E111" s="6" t="s">
         <v>13</v>
@@ -3662,7 +3662,7 @@
         <v>8</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>13</v>
@@ -3725,7 +3725,7 @@
         <v>7</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>9</v>
@@ -3746,7 +3746,7 @@
         <v>8</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E116" s="6" t="s">
         <v>13</v>
@@ -3767,7 +3767,7 @@
         <v>8</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E117" s="6" t="s">
         <v>13</v>
@@ -3830,7 +3830,7 @@
         <v>8</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E120" s="6" t="s">
         <v>13</v>
@@ -3851,7 +3851,7 @@
         <v>8</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E121" s="6" t="s">
         <v>13</v>
@@ -3872,7 +3872,7 @@
         <v>8</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>13</v>
@@ -3893,7 +3893,7 @@
         <v>7</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E123" s="6" t="s">
         <v>13</v>
@@ -3935,7 +3935,7 @@
         <v>7</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E125" s="6" t="s">
         <v>13</v>
@@ -3956,7 +3956,7 @@
         <v>8</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E126" s="6" t="s">
         <v>13</v>
@@ -3977,7 +3977,7 @@
         <v>8</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E127" s="6" t="s">
         <v>13</v>
@@ -3998,7 +3998,7 @@
         <v>8</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>13</v>
@@ -4040,7 +4040,7 @@
         <v>8</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>13</v>
@@ -4061,7 +4061,7 @@
         <v>8</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E131" s="6" t="s">
         <v>13</v>
@@ -4082,7 +4082,7 @@
         <v>8</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E132" s="6" t="s">
         <v>13</v>
@@ -4103,7 +4103,7 @@
         <v>8</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E133" s="6" t="s">
         <v>13</v>
@@ -4124,7 +4124,7 @@
         <v>8</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E134" s="6" t="s">
         <v>13</v>
@@ -4145,7 +4145,7 @@
         <v>8</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E135" s="6" t="s">
         <v>13</v>
@@ -4166,7 +4166,7 @@
         <v>8</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E136" s="6" t="s">
         <v>9</v>
@@ -4187,7 +4187,7 @@
         <v>8</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E137" s="6" t="s">
         <v>13</v>
@@ -4208,7 +4208,7 @@
         <v>8</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E138" s="6" t="s">
         <v>13</v>
@@ -4229,7 +4229,7 @@
         <v>8</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E139" s="6" t="s">
         <v>13</v>
@@ -4250,7 +4250,7 @@
         <v>8</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E140" s="6" t="s">
         <v>13</v>
@@ -4271,7 +4271,7 @@
         <v>8</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E141" s="6" t="s">
         <v>13</v>
@@ -4292,7 +4292,7 @@
         <v>8</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E142" s="6" t="s">
         <v>13</v>
@@ -4313,7 +4313,7 @@
         <v>8</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E143" s="6" t="s">
         <v>13</v>
@@ -4334,7 +4334,7 @@
         <v>8</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E144" s="6" t="s">
         <v>13</v>
@@ -4355,7 +4355,7 @@
         <v>8</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E145" s="6" t="s">
         <v>13</v>
@@ -4376,7 +4376,7 @@
         <v>8</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E146" s="6" t="s">
         <v>9</v>
@@ -4397,7 +4397,7 @@
         <v>8</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E147" s="6" t="s">
         <v>13</v>
@@ -4418,7 +4418,7 @@
         <v>7</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E148" s="6" t="s">
         <v>9</v>
@@ -4439,7 +4439,7 @@
         <v>8</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E149" s="6" t="s">
         <v>13</v>
@@ -4460,7 +4460,7 @@
         <v>7</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E150" s="6" t="s">
         <v>13</v>
@@ -4481,7 +4481,7 @@
         <v>8</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E151" s="6" t="s">
         <v>13</v>
@@ -4523,7 +4523,7 @@
         <v>7</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E153" s="6" t="s">
         <v>13</v>
@@ -4586,7 +4586,7 @@
         <v>8</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E156" s="6" t="s">
         <v>13</v>
@@ -4649,7 +4649,7 @@
         <v>8</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E159" s="6" t="s">
         <v>13</v>
@@ -4733,7 +4733,7 @@
         <v>8</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E163" s="6" t="s">
         <v>13</v>
@@ -4775,7 +4775,7 @@
         <v>8</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E165" s="6" t="s">
         <v>13</v>
@@ -4796,7 +4796,7 @@
         <v>7</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E166" s="6" t="s">
         <v>13</v>
@@ -4817,7 +4817,7 @@
         <v>8</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E167" s="6" t="s">
         <v>13</v>
@@ -4838,7 +4838,7 @@
         <v>8</v>
       </c>
       <c r="D168" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E168" s="6" t="s">
         <v>13</v>
@@ -4859,7 +4859,7 @@
         <v>8</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E169" s="6" t="s">
         <v>13</v>
@@ -4880,7 +4880,7 @@
         <v>8</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E170" s="6" t="s">
         <v>13</v>
@@ -4901,7 +4901,7 @@
         <v>7</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E171" s="6" t="s">
         <v>13</v>
@@ -5006,7 +5006,7 @@
         <v>8</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E176" s="6" t="s">
         <v>13</v>
@@ -5153,7 +5153,7 @@
         <v>8</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E183" s="6" t="s">
         <v>13</v>
@@ -5174,7 +5174,7 @@
         <v>8</v>
       </c>
       <c r="D184" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E184" s="6" t="s">
         <v>13</v>
@@ -5216,7 +5216,7 @@
         <v>8</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E186" s="6" t="s">
         <v>13</v>
@@ -5426,7 +5426,7 @@
         <v>7</v>
       </c>
       <c r="D196" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E196" s="6" t="s">
         <v>9</v>
@@ -5489,7 +5489,7 @@
         <v>7</v>
       </c>
       <c r="D199" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E199" s="6" t="s">
         <v>9</v>
@@ -5531,7 +5531,7 @@
         <v>7</v>
       </c>
       <c r="D201" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E201" s="6" t="s">
         <v>9</v>
@@ -5573,7 +5573,7 @@
         <v>8</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E203" s="6" t="s">
         <v>9</v>
@@ -5762,7 +5762,7 @@
         <v>7</v>
       </c>
       <c r="D212" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E212" s="6" t="s">
         <v>13</v>
@@ -5825,7 +5825,7 @@
         <v>7</v>
       </c>
       <c r="D215" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E215" s="6" t="s">
         <v>13</v>
@@ -5930,7 +5930,7 @@
         <v>7</v>
       </c>
       <c r="D220" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E220" s="6" t="s">
         <v>9</v>
@@ -5951,7 +5951,7 @@
         <v>7</v>
       </c>
       <c r="D221" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E221" s="6" t="s">
         <v>9</v>
@@ -5972,7 +5972,7 @@
         <v>7</v>
       </c>
       <c r="D222" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E222" s="6" t="s">
         <v>9</v>
@@ -6035,7 +6035,7 @@
         <v>7</v>
       </c>
       <c r="D225" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E225" s="6" t="s">
         <v>9</v>
@@ -6056,7 +6056,7 @@
         <v>8</v>
       </c>
       <c r="D226" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E226" s="6" t="s">
         <v>9</v>
@@ -6077,7 +6077,7 @@
         <v>7</v>
       </c>
       <c r="D227" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E227" s="6" t="s">
         <v>9</v>
@@ -6182,7 +6182,7 @@
         <v>7</v>
       </c>
       <c r="D232" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E232" s="6" t="s">
         <v>9</v>
@@ -6203,7 +6203,7 @@
         <v>7</v>
       </c>
       <c r="D233" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E233" s="6" t="s">
         <v>9</v>
@@ -6266,7 +6266,7 @@
         <v>7</v>
       </c>
       <c r="D236" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E236" s="6" t="s">
         <v>9</v>
@@ -6308,7 +6308,7 @@
         <v>7</v>
       </c>
       <c r="D238" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E238" s="6" t="s">
         <v>9</v>
@@ -6371,7 +6371,7 @@
         <v>8</v>
       </c>
       <c r="D241" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E241" s="6" t="s">
         <v>9</v>
@@ -6434,7 +6434,7 @@
         <v>7</v>
       </c>
       <c r="D244" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E244" s="6" t="s">
         <v>9</v>
@@ -6455,7 +6455,7 @@
         <v>7</v>
       </c>
       <c r="D245" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E245" s="6" t="s">
         <v>9</v>
@@ -6560,7 +6560,7 @@
         <v>8</v>
       </c>
       <c r="D250" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E250" s="6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
validated all index data in page data files
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="268">
   <si>
     <t>-PAGE-</t>
   </si>
@@ -57,15 +57,18 @@
     <t>VALID</t>
   </si>
   <si>
+    <t>https://discord.heatlabs.net</t>
+  </si>
+  <si>
     <t>https://heatlabs.net</t>
   </si>
   <si>
+    <t>GOOGLE API STATUS</t>
+  </si>
+  <si>
     <t>https://heatlabs.net/agents</t>
   </si>
   <si>
-    <t>GOOGLE API STATUS</t>
-  </si>
-  <si>
     <t>https://heatlabs.net/agents/akira</t>
   </si>
   <si>
@@ -75,36 +78,36 @@
     <t>https://heatlabs.net/agents/arblast</t>
   </si>
   <si>
+    <t>HTTPS PAGE STATUS</t>
+  </si>
+  <si>
     <t>https://heatlabs.net/agents/atom</t>
   </si>
   <si>
-    <t>HTTPS PAGE STATUS</t>
+    <t>NOT HTTPS</t>
   </si>
   <si>
     <t>https://heatlabs.net/agents/blitz</t>
   </si>
   <si>
-    <t>NOT HTTPS</t>
-  </si>
-  <si>
     <t>https://heatlabs.net/agents/chopper</t>
   </si>
   <si>
     <t>https://heatlabs.net/agents/ember</t>
   </si>
   <si>
+    <t>BREADCRUMB STATUS</t>
+  </si>
+  <si>
     <t>https://heatlabs.net/agents/fantome</t>
   </si>
   <si>
-    <t>BREADCRUMB STATUS</t>
+    <t>INVALID</t>
   </si>
   <si>
     <t>https://heatlabs.net/agents/hound</t>
   </si>
   <si>
-    <t>INVALID</t>
-  </si>
-  <si>
     <t>https://heatlabs.net/agents/jager</t>
   </si>
   <si>
@@ -255,6 +258,9 @@
     <t>https://heatlabs.net/check-compare</t>
   </si>
   <si>
+    <t>https://heatlabs.net/game-data</t>
+  </si>
+  <si>
     <t>https://heatlabs.net/guides</t>
   </si>
   <si>
@@ -810,14 +816,14 @@
     <t>https://status.heatlabs.net</t>
   </si>
   <si>
-    <t>https://discord.heatlabs.net</t>
+    <t>heatlabs.net/playground/roulette</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -868,6 +874,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1006,7 +1016,7 @@
     <xf borderId="6" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1310,7 +1320,7 @@
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>139</v>
+        <v>72</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
@@ -1320,7 +1330,7 @@
       <c r="I3" s="10">
         <f>COUNTIF(B:B,"INDEXED")
 </f>
-        <v>110</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4">
@@ -1331,7 +1341,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>12</v>
@@ -1355,10 +1365,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3" t="s">
@@ -1375,7 +1385,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>9</v>
@@ -1402,7 +1412,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
@@ -1414,7 +1424,7 @@
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -1432,10 +1442,10 @@
         <v>19</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -1456,7 +1466,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>9</v>
@@ -1479,7 +1489,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>9</v>
@@ -1506,19 +1516,19 @@
         <v>7</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1539,13 +1549,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1557,7 +1567,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>8</v>
@@ -1580,7 +1590,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>8</v>
@@ -1607,7 +1617,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>8</v>
@@ -1622,7 +1632,7 @@
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -1643,7 +1653,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>9</v>
@@ -1682,10 +1692,10 @@
         <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>9</v>
@@ -1703,10 +1713,10 @@
         <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>9</v>
@@ -1748,7 +1758,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>9</v>
@@ -1772,10 +1782,10 @@
         <v>8</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1790,7 +1800,7 @@
         <v>7</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>12</v>
@@ -1814,10 +1824,10 @@
         <v>7</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1835,10 +1845,10 @@
         <v>7</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1850,16 +1860,16 @@
         <v>41</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1871,16 +1881,16 @@
         <v>42</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1916,7 +1926,7 @@
         <v>7</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>12</v>
@@ -1961,10 +1971,10 @@
         <v>8</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1982,10 +1992,10 @@
         <v>8</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -2000,7 +2010,7 @@
         <v>7</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>12</v>
@@ -2045,10 +2055,10 @@
         <v>7</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2060,10 +2070,10 @@
         <v>51</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>9</v>
@@ -2081,10 +2091,10 @@
         <v>52</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>9</v>
@@ -2102,10 +2112,10 @@
         <v>53</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>9</v>
@@ -2123,10 +2133,10 @@
         <v>54</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>9</v>
@@ -2144,10 +2154,10 @@
         <v>55</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>9</v>
@@ -2186,10 +2196,10 @@
         <v>57</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>9</v>
@@ -2210,13 +2220,13 @@
         <v>7</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -2228,16 +2238,16 @@
         <v>59</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -2249,16 +2259,16 @@
         <v>60</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -2273,7 +2283,7 @@
         <v>7</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>12</v>
@@ -2294,7 +2304,7 @@
         <v>7</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>12</v>
@@ -2315,7 +2325,7 @@
         <v>7</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>12</v>
@@ -2354,7 +2364,7 @@
         <v>65</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>7</v>
@@ -2375,10 +2385,10 @@
         <v>66</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>12</v>
@@ -2396,7 +2406,7 @@
         <v>67</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>8</v>
@@ -2417,7 +2427,7 @@
         <v>68</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>8</v>
@@ -2438,7 +2448,7 @@
         <v>69</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>8</v>
@@ -2459,7 +2469,7 @@
         <v>70</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>8</v>
@@ -2480,7 +2490,7 @@
         <v>71</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>8</v>
@@ -2501,7 +2511,7 @@
         <v>72</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>8</v>
@@ -2522,7 +2532,7 @@
         <v>73</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>8</v>
@@ -2543,10 +2553,10 @@
         <v>74</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>12</v>
@@ -2564,16 +2574,16 @@
         <v>75</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -2585,16 +2595,16 @@
         <v>76</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -2606,7 +2616,7 @@
         <v>77</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>8</v>
@@ -2627,16 +2637,16 @@
         <v>78</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -2654,10 +2664,10 @@
         <v>8</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -2672,7 +2682,7 @@
         <v>7</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>12</v>
@@ -2686,11 +2696,11 @@
       <c r="I65" s="2"/>
     </row>
     <row r="66">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>8</v>
@@ -2711,16 +2721,16 @@
         <v>82</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -2732,10 +2742,10 @@
         <v>83</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>9</v>
@@ -2753,7 +2763,7 @@
         <v>84</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>8</v>
@@ -2795,16 +2805,16 @@
         <v>86</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
@@ -2816,10 +2826,10 @@
         <v>87</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>9</v>
@@ -2900,7 +2910,7 @@
         <v>91</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>8</v>
@@ -2921,16 +2931,16 @@
         <v>92</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
@@ -2948,10 +2958,10 @@
         <v>8</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
@@ -2963,16 +2973,16 @@
         <v>94</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
@@ -2987,7 +2997,7 @@
         <v>7</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>12</v>
@@ -3005,16 +3015,16 @@
         <v>96</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
@@ -3071,13 +3081,13 @@
         <v>7</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
@@ -3089,16 +3099,16 @@
         <v>100</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
@@ -3110,16 +3120,16 @@
         <v>101</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
@@ -3131,10 +3141,10 @@
         <v>102</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>12</v>
@@ -3200,10 +3210,10 @@
         <v>8</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
@@ -3221,10 +3231,10 @@
         <v>8</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
@@ -3299,7 +3309,7 @@
         <v>110</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>8</v>
@@ -3341,7 +3351,7 @@
         <v>112</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>8</v>
@@ -3362,7 +3372,7 @@
         <v>113</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>8</v>
@@ -3389,10 +3399,10 @@
         <v>8</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -3410,10 +3420,10 @@
         <v>8</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -3425,7 +3435,7 @@
         <v>116</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>8</v>
@@ -3446,7 +3456,7 @@
         <v>117</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>8</v>
@@ -3488,7 +3498,7 @@
         <v>119</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>8</v>
@@ -3515,10 +3525,10 @@
         <v>8</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
@@ -3533,13 +3543,13 @@
         <v>7</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
@@ -3572,16 +3582,16 @@
         <v>123</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
@@ -3620,10 +3630,10 @@
         <v>8</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
@@ -3641,10 +3651,10 @@
         <v>8</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
@@ -3656,16 +3666,16 @@
         <v>127</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
@@ -3677,16 +3687,16 @@
         <v>128</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
@@ -3698,16 +3708,16 @@
         <v>129</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
@@ -3722,7 +3732,7 @@
         <v>7</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>9</v>
@@ -3740,16 +3750,16 @@
         <v>131</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
@@ -3761,16 +3771,16 @@
         <v>132</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
@@ -3782,16 +3792,16 @@
         <v>133</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
@@ -3806,7 +3816,7 @@
         <v>8</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>12</v>
@@ -3824,16 +3834,16 @@
         <v>135</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
@@ -3845,10 +3855,10 @@
         <v>136</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>12</v>
@@ -3866,7 +3876,7 @@
         <v>137</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>8</v>
@@ -3887,10 +3897,10 @@
         <v>138</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>12</v>
@@ -3929,7 +3939,7 @@
         <v>140</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>7</v>
@@ -3950,7 +3960,7 @@
         <v>141</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>8</v>
@@ -3971,10 +3981,10 @@
         <v>142</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>12</v>
@@ -3992,7 +4002,7 @@
         <v>143</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C128" s="6" t="s">
         <v>8</v>
@@ -4019,10 +4029,10 @@
         <v>8</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
@@ -4034,7 +4044,7 @@
         <v>145</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C130" s="6" t="s">
         <v>8</v>
@@ -4055,16 +4065,16 @@
         <v>146</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C131" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
@@ -4076,7 +4086,7 @@
         <v>147</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C132" s="6" t="s">
         <v>8</v>
@@ -4097,7 +4107,7 @@
         <v>148</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C133" s="6" t="s">
         <v>8</v>
@@ -4118,7 +4128,7 @@
         <v>149</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C134" s="6" t="s">
         <v>8</v>
@@ -4139,7 +4149,7 @@
         <v>150</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C135" s="6" t="s">
         <v>8</v>
@@ -4166,10 +4176,10 @@
         <v>8</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
@@ -4181,7 +4191,7 @@
         <v>152</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C137" s="6" t="s">
         <v>8</v>
@@ -4202,16 +4212,16 @@
         <v>153</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C138" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
@@ -4223,7 +4233,7 @@
         <v>154</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>8</v>
@@ -4244,7 +4254,7 @@
         <v>155</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C140" s="6" t="s">
         <v>8</v>
@@ -4265,7 +4275,7 @@
         <v>156</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>8</v>
@@ -4286,7 +4296,7 @@
         <v>157</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C142" s="6" t="s">
         <v>8</v>
@@ -4307,7 +4317,7 @@
         <v>158</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>8</v>
@@ -4328,7 +4338,7 @@
         <v>159</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C144" s="6" t="s">
         <v>8</v>
@@ -4349,7 +4359,7 @@
         <v>160</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C145" s="6" t="s">
         <v>8</v>
@@ -4376,10 +4386,10 @@
         <v>8</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F146" s="2"/>
       <c r="G146" s="2"/>
@@ -4391,7 +4401,7 @@
         <v>162</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>8</v>
@@ -4415,7 +4425,7 @@
         <v>7</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D148" s="6" t="s">
         <v>9</v>
@@ -4433,7 +4443,7 @@
         <v>164</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>8</v>
@@ -4454,16 +4464,16 @@
         <v>165</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F150" s="2"/>
       <c r="G150" s="2"/>
@@ -4475,7 +4485,7 @@
         <v>166</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C151" s="6" t="s">
         <v>8</v>
@@ -4496,16 +4506,16 @@
         <v>167</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E152" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F152" s="2"/>
       <c r="G152" s="2"/>
@@ -4517,10 +4527,10 @@
         <v>168</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D153" s="6" t="s">
         <v>12</v>
@@ -4559,16 +4569,16 @@
         <v>170</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F155" s="2"/>
       <c r="G155" s="2"/>
@@ -4586,10 +4596,10 @@
         <v>8</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F156" s="2"/>
       <c r="G156" s="2"/>
@@ -4601,7 +4611,7 @@
         <v>172</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C157" s="6" t="s">
         <v>8</v>
@@ -4622,16 +4632,16 @@
         <v>173</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C158" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E158" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F158" s="2"/>
       <c r="G158" s="2"/>
@@ -4643,16 +4653,16 @@
         <v>174</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C159" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E159" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F159" s="2"/>
       <c r="G159" s="2"/>
@@ -4685,16 +4695,16 @@
         <v>176</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C161" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E161" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F161" s="2"/>
       <c r="G161" s="2"/>
@@ -4733,10 +4743,10 @@
         <v>8</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E163" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F163" s="2"/>
       <c r="G163" s="2"/>
@@ -4769,7 +4779,7 @@
         <v>180</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C165" s="6" t="s">
         <v>8</v>
@@ -4793,13 +4803,13 @@
         <v>8</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F166" s="2"/>
       <c r="G166" s="2"/>
@@ -4811,7 +4821,7 @@
         <v>182</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C167" s="6" t="s">
         <v>8</v>
@@ -4832,10 +4842,10 @@
         <v>183</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>12</v>
@@ -4853,7 +4863,7 @@
         <v>184</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>8</v>
@@ -4874,7 +4884,7 @@
         <v>185</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C170" s="6" t="s">
         <v>8</v>
@@ -4895,10 +4905,10 @@
         <v>186</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D171" s="6" t="s">
         <v>12</v>
@@ -4916,16 +4926,16 @@
         <v>187</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D172" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F172" s="2"/>
       <c r="G172" s="2"/>
@@ -4937,16 +4947,16 @@
         <v>188</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D173" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E173" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F173" s="2"/>
       <c r="G173" s="2"/>
@@ -5006,10 +5016,10 @@
         <v>8</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E176" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F176" s="2"/>
       <c r="G176" s="2"/>
@@ -5021,7 +5031,7 @@
         <v>192</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C177" s="6" t="s">
         <v>8</v>
@@ -5042,16 +5052,16 @@
         <v>193</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C178" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D178" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E178" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F178" s="2"/>
       <c r="G178" s="2"/>
@@ -5063,7 +5073,7 @@
         <v>194</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C179" s="6" t="s">
         <v>8</v>
@@ -5153,10 +5163,10 @@
         <v>8</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F183" s="2"/>
       <c r="G183" s="2"/>
@@ -5174,10 +5184,10 @@
         <v>8</v>
       </c>
       <c r="D184" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
@@ -5189,16 +5199,16 @@
         <v>200</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E185" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
@@ -5210,7 +5220,7 @@
         <v>201</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C186" s="6" t="s">
         <v>8</v>
@@ -5252,16 +5262,16 @@
         <v>203</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C188" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E188" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F188" s="2"/>
       <c r="G188" s="2"/>
@@ -5357,16 +5367,16 @@
         <v>208</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C193" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D193" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E193" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F193" s="2"/>
       <c r="G193" s="2"/>
@@ -5378,16 +5388,16 @@
         <v>209</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C194" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E194" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F194" s="2"/>
       <c r="G194" s="2"/>
@@ -5402,7 +5412,7 @@
         <v>7</v>
       </c>
       <c r="C195" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D195" s="6" t="s">
         <v>12</v>
@@ -5423,13 +5433,13 @@
         <v>7</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D196" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E196" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F196" s="2"/>
       <c r="G196" s="2"/>
@@ -5447,10 +5457,10 @@
         <v>7</v>
       </c>
       <c r="D197" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E197" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F197" s="2"/>
       <c r="G197" s="2"/>
@@ -5462,10 +5472,10 @@
         <v>213</v>
       </c>
       <c r="B198" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C198" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D198" s="6" t="s">
         <v>9</v>
@@ -5504,10 +5514,10 @@
         <v>215</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D200" s="6" t="s">
         <v>9</v>
@@ -5546,10 +5556,10 @@
         <v>217</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C202" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D202" s="6" t="s">
         <v>9</v>
@@ -5570,7 +5580,7 @@
         <v>7</v>
       </c>
       <c r="C203" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D203" s="6" t="s">
         <v>9</v>
@@ -5591,13 +5601,13 @@
         <v>7</v>
       </c>
       <c r="C204" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D204" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E204" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F204" s="2"/>
       <c r="G204" s="2"/>
@@ -5609,7 +5619,7 @@
         <v>220</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C205" s="6" t="s">
         <v>8</v>
@@ -5633,7 +5643,7 @@
         <v>7</v>
       </c>
       <c r="C206" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D206" s="6" t="s">
         <v>12</v>
@@ -5651,16 +5661,16 @@
         <v>222</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C207" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E207" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F207" s="2"/>
       <c r="G207" s="2"/>
@@ -5672,16 +5682,16 @@
         <v>223</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C208" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D208" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E208" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F208" s="2"/>
       <c r="G208" s="2"/>
@@ -5693,16 +5703,16 @@
         <v>224</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C209" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D209" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E209" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F209" s="2"/>
       <c r="G209" s="2"/>
@@ -5759,13 +5769,13 @@
         <v>8</v>
       </c>
       <c r="C212" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D212" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E212" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F212" s="2"/>
       <c r="G212" s="2"/>
@@ -5777,16 +5787,16 @@
         <v>228</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C213" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D213" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E213" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F213" s="2"/>
       <c r="G213" s="2"/>
@@ -5804,10 +5814,10 @@
         <v>7</v>
       </c>
       <c r="D214" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E214" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F214" s="2"/>
       <c r="G214" s="2"/>
@@ -5867,10 +5877,10 @@
         <v>7</v>
       </c>
       <c r="D217" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E217" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F217" s="2"/>
       <c r="G217" s="2"/>
@@ -5903,7 +5913,7 @@
         <v>234</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C219" s="6" t="s">
         <v>7</v>
@@ -6029,7 +6039,7 @@
         <v>240</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C225" s="6" t="s">
         <v>7</v>
@@ -6053,7 +6063,7 @@
         <v>7</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D226" s="6" t="s">
         <v>9</v>
@@ -6095,13 +6105,13 @@
         <v>7</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D228" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E228" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F228" s="2"/>
       <c r="G228" s="2"/>
@@ -6140,10 +6150,10 @@
         <v>7</v>
       </c>
       <c r="D230" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F230" s="2"/>
       <c r="G230" s="2"/>
@@ -6176,7 +6186,7 @@
         <v>247</v>
       </c>
       <c r="B232" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C232" s="6" t="s">
         <v>7</v>
@@ -6218,10 +6228,10 @@
         <v>249</v>
       </c>
       <c r="B234" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C234" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D234" s="6" t="s">
         <v>9</v>
@@ -6239,10 +6249,10 @@
         <v>250</v>
       </c>
       <c r="B235" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C235" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D235" s="6" t="s">
         <v>9</v>
@@ -6263,7 +6273,7 @@
         <v>7</v>
       </c>
       <c r="C236" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D236" s="6" t="s">
         <v>9</v>
@@ -6281,10 +6291,10 @@
         <v>252</v>
       </c>
       <c r="B237" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C237" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D237" s="6" t="s">
         <v>9</v>
@@ -6365,10 +6375,10 @@
         <v>256</v>
       </c>
       <c r="B241" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C241" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D241" s="6" t="s">
         <v>9</v>
@@ -6386,16 +6396,16 @@
         <v>257</v>
       </c>
       <c r="B242" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C242" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D242" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E242" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F242" s="2"/>
       <c r="G242" s="2"/>
@@ -6410,10 +6420,10 @@
         <v>7</v>
       </c>
       <c r="C243" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D243" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E243" s="6" t="s">
         <v>9</v>
@@ -6434,10 +6444,10 @@
         <v>7</v>
       </c>
       <c r="D244" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F244" s="2"/>
       <c r="G244" s="2"/>
@@ -6455,7 +6465,7 @@
         <v>7</v>
       </c>
       <c r="D245" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E245" s="6" t="s">
         <v>9</v>
@@ -6470,10 +6480,10 @@
         <v>261</v>
       </c>
       <c r="B246" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C246" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D246" s="6" t="s">
         <v>9</v>
@@ -6494,7 +6504,7 @@
         <v>7</v>
       </c>
       <c r="C247" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D247" s="6" t="s">
         <v>9</v>
@@ -6512,7 +6522,7 @@
         <v>263</v>
       </c>
       <c r="B248" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C248" s="6" t="s">
         <v>8</v>
@@ -6554,16 +6564,16 @@
         <v>265</v>
       </c>
       <c r="B250" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C250" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D250" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E250" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F250" s="2"/>
       <c r="G250" s="2"/>
@@ -6571,22 +6581,42 @@
       <c r="I250" s="2"/>
     </row>
     <row r="251">
-      <c r="A251" s="14"/>
-      <c r="B251" s="6"/>
-      <c r="C251" s="6"/>
-      <c r="D251" s="6"/>
-      <c r="E251" s="6"/>
+      <c r="A251" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="B251" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C251" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D251" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E251" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="F251" s="2"/>
       <c r="G251" s="2"/>
       <c r="H251" s="2"/>
       <c r="I251" s="2"/>
     </row>
     <row r="252">
-      <c r="A252" s="14"/>
-      <c r="B252" s="6"/>
-      <c r="C252" s="6"/>
-      <c r="D252" s="6"/>
-      <c r="E252" s="6"/>
+      <c r="A252" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B252" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C252" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D252" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E252" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="F252" s="2"/>
       <c r="G252" s="2"/>
       <c r="H252" s="2"/>
@@ -15006,7 +15036,9 @@
     <hyperlink r:id="rId247" ref="A248"/>
     <hyperlink r:id="rId248" ref="A249"/>
     <hyperlink r:id="rId249" ref="A250"/>
+    <hyperlink r:id="rId250" ref="A251"/>
+    <hyperlink r:id="rId251" ref="A252"/>
   </hyperlinks>
-  <drawing r:id="rId250"/>
+  <drawing r:id="rId252"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed game-data page from page data files, added missing roulette page to page data files
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="pages" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">pages!$A$1:$E$992</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">pages!$A$1:$E$991</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="267">
   <si>
     <t>-PAGE-</t>
   </si>
@@ -258,9 +258,6 @@
     <t>https://heatlabs.net/check-compare</t>
   </si>
   <si>
-    <t>https://heatlabs.net/game-data</t>
-  </si>
-  <si>
     <t>https://heatlabs.net/guides</t>
   </si>
   <si>
@@ -666,6 +663,9 @@
     <t>https://heatlabs.net/playground/heat-labs-app</t>
   </si>
   <si>
+    <t>https://heatlabs.net/playground/roulette</t>
+  </si>
+  <si>
     <t>https://heatlabs.net/playground/soundboard</t>
   </si>
   <si>
@@ -814,9 +814,6 @@
   </si>
   <si>
     <t>https://status.heatlabs.net</t>
-  </si>
-  <si>
-    <t>heatlabs.net/playground/roulette</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1327,7 @@
       <c r="I3" s="10">
         <f>COUNTIF(B:B,"INDEXED")
 </f>
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4">
@@ -1424,7 +1421,7 @@
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -1528,7 +1525,7 @@
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1632,7 +1629,7 @@
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -2696,20 +2693,20 @@
       <c r="I65" s="2"/>
     </row>
     <row r="66">
-      <c r="A66" s="14" t="s">
+      <c r="A66" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -2724,13 +2721,13 @@
         <v>7</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -2766,7 +2763,7 @@
         <v>7</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>9</v>
@@ -2784,10 +2781,10 @@
         <v>85</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>9</v>
@@ -2805,10 +2802,10 @@
         <v>86</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>9</v>
@@ -2829,13 +2826,13 @@
         <v>7</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
@@ -2847,16 +2844,16 @@
         <v>88</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -2868,16 +2865,16 @@
         <v>89</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
@@ -2889,16 +2886,16 @@
         <v>90</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
@@ -2910,16 +2907,16 @@
         <v>91</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
@@ -2937,10 +2934,10 @@
         <v>8</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
@@ -2952,7 +2949,7 @@
         <v>93</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>8</v>
@@ -2973,16 +2970,16 @@
         <v>94</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
@@ -2997,7 +2994,7 @@
         <v>7</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>12</v>
@@ -3036,16 +3033,16 @@
         <v>97</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -3057,16 +3054,16 @@
         <v>98</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
@@ -3078,16 +3075,16 @@
         <v>99</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
@@ -3099,7 +3096,7 @@
         <v>100</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>8</v>
@@ -3123,13 +3120,13 @@
         <v>7</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
@@ -3141,10 +3138,10 @@
         <v>102</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>12</v>
@@ -3231,10 +3228,10 @@
         <v>8</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
@@ -3330,7 +3327,7 @@
         <v>111</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>8</v>
@@ -3351,7 +3348,7 @@
         <v>112</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>8</v>
@@ -3414,16 +3411,16 @@
         <v>115</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -3456,7 +3453,7 @@
         <v>117</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>8</v>
@@ -3477,7 +3474,7 @@
         <v>118</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>8</v>
@@ -3498,7 +3495,7 @@
         <v>119</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>8</v>
@@ -3519,7 +3516,7 @@
         <v>120</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>8</v>
@@ -3540,16 +3537,16 @@
         <v>121</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
@@ -3561,10 +3558,10 @@
         <v>122</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>9</v>
@@ -3582,10 +3579,10 @@
         <v>123</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>9</v>
@@ -3603,16 +3600,16 @@
         <v>124</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C109" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
@@ -3624,16 +3621,16 @@
         <v>125</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
@@ -3645,7 +3642,7 @@
         <v>126</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>8</v>
@@ -3666,16 +3663,16 @@
         <v>127</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
@@ -3708,16 +3705,16 @@
         <v>129</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
@@ -3753,7 +3750,7 @@
         <v>7</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>9</v>
@@ -3771,16 +3768,16 @@
         <v>132</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
@@ -3813,16 +3810,16 @@
         <v>134</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
@@ -3837,13 +3834,13 @@
         <v>7</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
@@ -3858,7 +3855,7 @@
         <v>7</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>12</v>
@@ -3921,7 +3918,7 @@
         <v>7</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>12</v>
@@ -3942,7 +3939,7 @@
         <v>7</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>12</v>
@@ -3963,7 +3960,7 @@
         <v>7</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>12</v>
@@ -3984,7 +3981,7 @@
         <v>7</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>12</v>
@@ -4050,10 +4047,10 @@
         <v>8</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
@@ -4071,10 +4068,10 @@
         <v>8</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
@@ -4197,10 +4194,10 @@
         <v>8</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
@@ -4218,10 +4215,10 @@
         <v>8</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
@@ -4407,10 +4404,10 @@
         <v>8</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
@@ -4428,10 +4425,10 @@
         <v>8</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F148" s="2"/>
       <c r="G148" s="2"/>
@@ -4446,13 +4443,13 @@
         <v>7</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
@@ -4467,13 +4464,13 @@
         <v>7</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F150" s="2"/>
       <c r="G150" s="2"/>
@@ -4488,7 +4485,7 @@
         <v>7</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D151" s="6" t="s">
         <v>12</v>
@@ -4509,7 +4506,7 @@
         <v>7</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D152" s="6" t="s">
         <v>12</v>
@@ -4527,16 +4524,16 @@
         <v>168</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C153" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E153" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F153" s="2"/>
       <c r="G153" s="2"/>
@@ -4548,16 +4545,16 @@
         <v>169</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E154" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F154" s="2"/>
       <c r="G154" s="2"/>
@@ -4569,16 +4566,16 @@
         <v>170</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F155" s="2"/>
       <c r="G155" s="2"/>
@@ -4611,16 +4608,16 @@
         <v>172</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C157" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E157" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F157" s="2"/>
       <c r="G157" s="2"/>
@@ -4638,10 +4635,10 @@
         <v>8</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E158" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F158" s="2"/>
       <c r="G158" s="2"/>
@@ -4653,7 +4650,7 @@
         <v>174</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C159" s="6" t="s">
         <v>8</v>
@@ -4674,16 +4671,16 @@
         <v>175</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C160" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E160" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F160" s="2"/>
       <c r="G160" s="2"/>
@@ -4695,16 +4692,16 @@
         <v>176</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C161" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E161" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F161" s="2"/>
       <c r="G161" s="2"/>
@@ -4758,16 +4755,16 @@
         <v>179</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E164" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
@@ -4779,16 +4776,16 @@
         <v>180</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C165" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F165" s="2"/>
       <c r="G165" s="2"/>
@@ -4800,16 +4797,16 @@
         <v>181</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C166" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F166" s="2"/>
       <c r="G166" s="2"/>
@@ -4824,7 +4821,7 @@
         <v>7</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D167" s="6" t="s">
         <v>12</v>
@@ -4845,7 +4842,7 @@
         <v>7</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>12</v>
@@ -4929,7 +4926,7 @@
         <v>7</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D172" s="6" t="s">
         <v>12</v>
@@ -4947,16 +4944,16 @@
         <v>188</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D173" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E173" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F173" s="2"/>
       <c r="G173" s="2"/>
@@ -5031,16 +5028,16 @@
         <v>192</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C177" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D177" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E177" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F177" s="2"/>
       <c r="G177" s="2"/>
@@ -5058,10 +5055,10 @@
         <v>8</v>
       </c>
       <c r="D178" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E178" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F178" s="2"/>
       <c r="G178" s="2"/>
@@ -5073,7 +5070,7 @@
         <v>194</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C179" s="6" t="s">
         <v>8</v>
@@ -5178,16 +5175,16 @@
         <v>199</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C184" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D184" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
@@ -5220,16 +5217,16 @@
         <v>201</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C186" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E186" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F186" s="2"/>
       <c r="G186" s="2"/>
@@ -5241,16 +5238,16 @@
         <v>202</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C187" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D187" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E187" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F187" s="2"/>
       <c r="G187" s="2"/>
@@ -5262,16 +5259,16 @@
         <v>203</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C188" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E188" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F188" s="2"/>
       <c r="G188" s="2"/>
@@ -5388,16 +5385,16 @@
         <v>209</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C194" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E194" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F194" s="2"/>
       <c r="G194" s="2"/>
@@ -5433,7 +5430,7 @@
         <v>7</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D196" s="6" t="s">
         <v>12</v>
@@ -5457,10 +5454,10 @@
         <v>7</v>
       </c>
       <c r="D197" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E197" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F197" s="2"/>
       <c r="G197" s="2"/>
@@ -5493,10 +5490,10 @@
         <v>214</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D199" s="6" t="s">
         <v>9</v>
@@ -5514,10 +5511,10 @@
         <v>215</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D200" s="6" t="s">
         <v>9</v>
@@ -5538,7 +5535,7 @@
         <v>7</v>
       </c>
       <c r="C201" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D201" s="6" t="s">
         <v>9</v>
@@ -6560,7 +6557,7 @@
       <c r="I249" s="2"/>
     </row>
     <row r="250">
-      <c r="A250" s="5" t="s">
+      <c r="A250" s="14" t="s">
         <v>265</v>
       </c>
       <c r="B250" s="6" t="s">
@@ -6581,7 +6578,7 @@
       <c r="I250" s="2"/>
     </row>
     <row r="251">
-      <c r="A251" s="14" t="s">
+      <c r="A251" s="5" t="s">
         <v>266</v>
       </c>
       <c r="B251" s="6" t="s">
@@ -6602,21 +6599,11 @@
       <c r="I251" s="2"/>
     </row>
     <row r="252">
-      <c r="A252" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="B252" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C252" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D252" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E252" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="A252" s="15"/>
+      <c r="B252" s="16"/>
+      <c r="C252" s="16"/>
+      <c r="D252" s="16"/>
+      <c r="E252" s="16"/>
       <c r="F252" s="2"/>
       <c r="G252" s="2"/>
       <c r="H252" s="2"/>
@@ -14751,22 +14738,11 @@
       <c r="H991" s="2"/>
       <c r="I991" s="2"/>
     </row>
-    <row r="992">
-      <c r="A992" s="15"/>
-      <c r="B992" s="16"/>
-      <c r="C992" s="16"/>
-      <c r="D992" s="16"/>
-      <c r="E992" s="16"/>
-      <c r="F992" s="2"/>
-      <c r="G992" s="2"/>
-      <c r="H992" s="2"/>
-      <c r="I992" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$E$992">
-    <sortState ref="A1:E992">
-      <sortCondition ref="A1:A992"/>
-      <sortCondition ref="D1:D992"/>
+  <autoFilter ref="$A$1:$E$991">
+    <sortState ref="A1:E991">
+      <sortCondition ref="A1:A991"/>
+      <sortCondition ref="D1:D991"/>
     </sortState>
   </autoFilter>
   <mergeCells count="4">
@@ -14776,13 +14752,13 @@
     <mergeCell ref="G13:I13"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:C992">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:C991">
       <formula1>"NOT INDEXED,NOT NEEDED,PENDING,INDEXED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D992">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D991">
       <formula1>"NOT NEEDED,NOT HTTPS,UNKNOWN,HTTPS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E992">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E991">
       <formula1>"NOT NEEDED,INVALID,UNKNOWN,VALID"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15037,8 +15013,7 @@
     <hyperlink r:id="rId248" ref="A249"/>
     <hyperlink r:id="rId249" ref="A250"/>
     <hyperlink r:id="rId250" ref="A251"/>
-    <hyperlink r:id="rId251" ref="A252"/>
   </hyperlinks>
-  <drawing r:id="rId252"/>
+  <drawing r:id="rId251"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
validated all pages data
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -42,33 +42,33 @@
     <t>PENDING</t>
   </si>
   <si>
+    <t>HTTPS</t>
+  </si>
+  <si>
+    <t>VALID</t>
+  </si>
+  <si>
+    <t>NOT INDEXED</t>
+  </si>
+  <si>
+    <t>https://changelog.heatlabs.net</t>
+  </si>
+  <si>
+    <t>https://discord.heatlabs.net</t>
+  </si>
+  <si>
+    <t>https://heatlabs.net</t>
+  </si>
+  <si>
+    <t>GOOGLE API STATUS</t>
+  </si>
+  <si>
+    <t>https://heatlabs.net/agents</t>
+  </si>
+  <si>
     <t>UNKNOWN</t>
   </si>
   <si>
-    <t>NOT INDEXED</t>
-  </si>
-  <si>
-    <t>https://changelog.heatlabs.net</t>
-  </si>
-  <si>
-    <t>HTTPS</t>
-  </si>
-  <si>
-    <t>VALID</t>
-  </si>
-  <si>
-    <t>https://discord.heatlabs.net</t>
-  </si>
-  <si>
-    <t>https://heatlabs.net</t>
-  </si>
-  <si>
-    <t>GOOGLE API STATUS</t>
-  </si>
-  <si>
-    <t>https://heatlabs.net/agents</t>
-  </si>
-  <si>
     <t>https://heatlabs.net/agents/akira</t>
   </si>
   <si>
@@ -849,7 +849,7 @@
     <t>https://heatlabs.net/video-showcase</t>
   </si>
   <si>
-    <t>https://mod.heatlabs.net</t>
+    <t>https://mods.heatlabs.net</t>
   </si>
   <si>
     <t>https://social.heatlabs.net</t>
@@ -1336,14 +1336,14 @@
         <v>9</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>7</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>7</v>
@@ -1360,16 +1360,16 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
@@ -1379,12 +1379,12 @@
       <c r="I3" s="10">
         <f>COUNTIF(B:B,"INDEXED")
 </f>
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>7</v>
@@ -1393,10 +1393,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1405,7 +1405,7 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>7</v>
@@ -1414,21 +1414,21 @@
         <v>7</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>7</v>
@@ -1437,17 +1437,17 @@
         <v>7</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>7</v>
@@ -1464,10 +1464,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="10">
@@ -1497,10 +1497,10 @@
         <v>7</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1518,10 +1518,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="3" t="s">
@@ -1541,20 +1541,20 @@
         <v>7</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -1568,16 +1568,16 @@
         <v>7</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>141</v>
+        <v>229</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1587,7 +1587,7 @@
       <c r="I11" s="10">
         <f>COUNTIF(D:D,"HTTPS")
 </f>
-        <v>113</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
@@ -1601,10 +1601,10 @@
         <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1622,10 +1622,10 @@
         <v>7</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="3" t="s">
@@ -1645,20 +1645,20 @@
         <v>8</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>29</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -1672,16 +1672,16 @@
         <v>8</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -1691,7 +1691,7 @@
       <c r="I15" s="10">
         <f>COUNTIF(E:E,"VALID")
 </f>
-        <v>112</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16">
@@ -1705,10 +1705,10 @@
         <v>8</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1720,16 +1720,16 @@
         <v>32</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1747,10 +1747,10 @@
         <v>7</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1768,10 +1768,10 @@
         <v>8</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1789,10 +1789,10 @@
         <v>7</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1810,10 +1810,10 @@
         <v>7</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1831,10 +1831,10 @@
         <v>8</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1846,16 +1846,16 @@
         <v>38</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1873,10 +1873,10 @@
         <v>7</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1894,10 +1894,10 @@
         <v>7</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1915,10 +1915,10 @@
         <v>7</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1930,16 +1930,16 @@
         <v>42</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1957,10 +1957,10 @@
         <v>7</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1978,10 +1978,10 @@
         <v>7</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -1999,10 +1999,10 @@
         <v>7</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -2020,10 +2020,10 @@
         <v>7</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -2041,10 +2041,10 @@
         <v>8</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -2062,10 +2062,10 @@
         <v>8</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -2083,10 +2083,10 @@
         <v>7</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -2104,10 +2104,10 @@
         <v>7</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2119,7 +2119,7 @@
         <v>51</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>8</v>
@@ -2128,7 +2128,7 @@
         <v>9</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -2140,16 +2140,16 @@
         <v>52</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -2167,10 +2167,10 @@
         <v>8</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -2398,10 +2398,10 @@
         <v>7</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -2419,10 +2419,10 @@
         <v>8</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -2440,10 +2440,10 @@
         <v>7</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -2461,10 +2461,10 @@
         <v>8</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -2482,10 +2482,10 @@
         <v>7</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -2503,10 +2503,10 @@
         <v>8</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -2524,10 +2524,10 @@
         <v>8</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -2545,10 +2545,10 @@
         <v>7</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -2566,10 +2566,10 @@
         <v>7</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -2587,10 +2587,10 @@
         <v>8</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -2602,16 +2602,16 @@
         <v>75</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -2629,10 +2629,10 @@
         <v>7</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -2644,16 +2644,16 @@
         <v>77</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -2671,10 +2671,10 @@
         <v>7</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
@@ -2692,10 +2692,10 @@
         <v>7</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -2713,10 +2713,10 @@
         <v>7</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -2734,10 +2734,10 @@
         <v>7</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
@@ -2755,10 +2755,10 @@
         <v>8</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -2776,10 +2776,10 @@
         <v>7</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -2797,10 +2797,10 @@
         <v>7</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
@@ -2818,10 +2818,10 @@
         <v>7</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
@@ -2839,10 +2839,10 @@
         <v>7</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
@@ -2860,10 +2860,10 @@
         <v>7</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
@@ -2881,10 +2881,10 @@
         <v>7</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
@@ -2902,10 +2902,10 @@
         <v>7</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -2923,10 +2923,10 @@
         <v>7</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
@@ -2938,16 +2938,16 @@
         <v>91</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
@@ -2959,16 +2959,16 @@
         <v>92</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
@@ -2980,7 +2980,7 @@
         <v>93</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>7</v>
@@ -2989,7 +2989,7 @@
         <v>9</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
@@ -3007,10 +3007,10 @@
         <v>7</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
@@ -3028,10 +3028,10 @@
         <v>7</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
@@ -3049,10 +3049,10 @@
         <v>8</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
@@ -3070,10 +3070,10 @@
         <v>8</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
@@ -3091,10 +3091,10 @@
         <v>7</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -3106,16 +3106,16 @@
         <v>99</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
@@ -3133,10 +3133,10 @@
         <v>7</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
@@ -3154,10 +3154,10 @@
         <v>7</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
@@ -3169,16 +3169,16 @@
         <v>102</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
@@ -3196,10 +3196,10 @@
         <v>7</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -3217,10 +3217,10 @@
         <v>8</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -3238,10 +3238,10 @@
         <v>7</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
@@ -3259,10 +3259,10 @@
         <v>8</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
@@ -3280,10 +3280,10 @@
         <v>8</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
@@ -3301,10 +3301,10 @@
         <v>7</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
@@ -3322,10 +3322,10 @@
         <v>7</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
@@ -3343,10 +3343,10 @@
         <v>7</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -3364,10 +3364,10 @@
         <v>8</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -3385,10 +3385,10 @@
         <v>7</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
@@ -3406,10 +3406,10 @@
         <v>8</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
@@ -3427,10 +3427,10 @@
         <v>8</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
@@ -3448,10 +3448,10 @@
         <v>7</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -3469,10 +3469,10 @@
         <v>7</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -3490,10 +3490,10 @@
         <v>7</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
@@ -3511,10 +3511,10 @@
         <v>8</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
@@ -3532,10 +3532,10 @@
         <v>7</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
@@ -3553,10 +3553,10 @@
         <v>7</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
@@ -3574,10 +3574,10 @@
         <v>7</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
@@ -3595,10 +3595,10 @@
         <v>7</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
@@ -3616,10 +3616,10 @@
         <v>8</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
@@ -3637,10 +3637,10 @@
         <v>8</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
@@ -3658,10 +3658,10 @@
         <v>7</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
@@ -3679,10 +3679,10 @@
         <v>7</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
@@ -3700,10 +3700,10 @@
         <v>7</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
@@ -3721,10 +3721,10 @@
         <v>8</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
@@ -3742,10 +3742,10 @@
         <v>7</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
@@ -3763,10 +3763,10 @@
         <v>7</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
@@ -3784,10 +3784,10 @@
         <v>8</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
@@ -3805,10 +3805,10 @@
         <v>7</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
@@ -3826,10 +3826,10 @@
         <v>7</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
@@ -3847,10 +3847,10 @@
         <v>7</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
@@ -3868,10 +3868,10 @@
         <v>8</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
@@ -3889,10 +3889,10 @@
         <v>7</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
@@ -3910,10 +3910,10 @@
         <v>8</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
@@ -3931,10 +3931,10 @@
         <v>7</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
@@ -3952,10 +3952,10 @@
         <v>8</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
@@ -3973,10 +3973,10 @@
         <v>8</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
@@ -3994,10 +3994,10 @@
         <v>7</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
@@ -4015,10 +4015,10 @@
         <v>7</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
@@ -4036,10 +4036,10 @@
         <v>8</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
@@ -4057,10 +4057,10 @@
         <v>7</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
@@ -4078,10 +4078,10 @@
         <v>7</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
@@ -4099,10 +4099,10 @@
         <v>8</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
@@ -4120,10 +4120,10 @@
         <v>7</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
@@ -4141,10 +4141,10 @@
         <v>8</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
@@ -4162,10 +4162,10 @@
         <v>7</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
@@ -4183,10 +4183,10 @@
         <v>7</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
@@ -4198,16 +4198,16 @@
         <v>151</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C135" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
@@ -4225,10 +4225,10 @@
         <v>7</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
@@ -4246,10 +4246,10 @@
         <v>7</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
@@ -4267,10 +4267,10 @@
         <v>7</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
@@ -4288,10 +4288,10 @@
         <v>7</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
@@ -4309,10 +4309,10 @@
         <v>8</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
@@ -4330,10 +4330,10 @@
         <v>8</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
@@ -4351,10 +4351,10 @@
         <v>7</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
@@ -4372,10 +4372,10 @@
         <v>8</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
@@ -4393,10 +4393,10 @@
         <v>7</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
@@ -4414,10 +4414,10 @@
         <v>7</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
@@ -4435,10 +4435,10 @@
         <v>7</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F146" s="2"/>
       <c r="G146" s="2"/>
@@ -4456,10 +4456,10 @@
         <v>8</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
@@ -4477,10 +4477,10 @@
         <v>8</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F148" s="2"/>
       <c r="G148" s="2"/>
@@ -4498,10 +4498,10 @@
         <v>7</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
@@ -4519,10 +4519,10 @@
         <v>7</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F150" s="2"/>
       <c r="G150" s="2"/>
@@ -4540,10 +4540,10 @@
         <v>7</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F151" s="2"/>
       <c r="G151" s="2"/>
@@ -4561,10 +4561,10 @@
         <v>7</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E152" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F152" s="2"/>
       <c r="G152" s="2"/>
@@ -4582,10 +4582,10 @@
         <v>8</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E153" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F153" s="2"/>
       <c r="G153" s="2"/>
@@ -4603,10 +4603,10 @@
         <v>7</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E154" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F154" s="2"/>
       <c r="G154" s="2"/>
@@ -4624,10 +4624,10 @@
         <v>8</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F155" s="2"/>
       <c r="G155" s="2"/>
@@ -4645,10 +4645,10 @@
         <v>7</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F156" s="2"/>
       <c r="G156" s="2"/>
@@ -4666,10 +4666,10 @@
         <v>7</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E157" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F157" s="2"/>
       <c r="G157" s="2"/>
@@ -4687,10 +4687,10 @@
         <v>7</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E158" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F158" s="2"/>
       <c r="G158" s="2"/>
@@ -4708,10 +4708,10 @@
         <v>7</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E159" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F159" s="2"/>
       <c r="G159" s="2"/>
@@ -4729,10 +4729,10 @@
         <v>8</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E160" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F160" s="2"/>
       <c r="G160" s="2"/>
@@ -4750,10 +4750,10 @@
         <v>7</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E161" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F161" s="2"/>
       <c r="G161" s="2"/>
@@ -4771,10 +4771,10 @@
         <v>7</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E162" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F162" s="2"/>
       <c r="G162" s="2"/>
@@ -4792,10 +4792,10 @@
         <v>7</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E163" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F163" s="2"/>
       <c r="G163" s="2"/>
@@ -4813,10 +4813,10 @@
         <v>7</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E164" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
@@ -4834,10 +4834,10 @@
         <v>8</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F165" s="2"/>
       <c r="G165" s="2"/>
@@ -4855,10 +4855,10 @@
         <v>8</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F166" s="2"/>
       <c r="G166" s="2"/>
@@ -4876,10 +4876,10 @@
         <v>7</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F167" s="2"/>
       <c r="G167" s="2"/>
@@ -4897,10 +4897,10 @@
         <v>8</v>
       </c>
       <c r="D168" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F168" s="2"/>
       <c r="G168" s="2"/>
@@ -4912,16 +4912,16 @@
         <v>185</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F169" s="2"/>
       <c r="G169" s="2"/>
@@ -4939,10 +4939,10 @@
         <v>8</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E170" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F170" s="2"/>
       <c r="G170" s="2"/>
@@ -4960,10 +4960,10 @@
         <v>8</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E171" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F171" s="2"/>
       <c r="G171" s="2"/>
@@ -4981,10 +4981,10 @@
         <v>8</v>
       </c>
       <c r="D172" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F172" s="2"/>
       <c r="G172" s="2"/>
@@ -5002,10 +5002,10 @@
         <v>7</v>
       </c>
       <c r="D173" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E173" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F173" s="2"/>
       <c r="G173" s="2"/>
@@ -5023,10 +5023,10 @@
         <v>8</v>
       </c>
       <c r="D174" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E174" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F174" s="2"/>
       <c r="G174" s="2"/>
@@ -5044,10 +5044,10 @@
         <v>8</v>
       </c>
       <c r="D175" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E175" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F175" s="2"/>
       <c r="G175" s="2"/>
@@ -5065,10 +5065,10 @@
         <v>8</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E176" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F176" s="2"/>
       <c r="G176" s="2"/>
@@ -5086,10 +5086,10 @@
         <v>7</v>
       </c>
       <c r="D177" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E177" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F177" s="2"/>
       <c r="G177" s="2"/>
@@ -5107,10 +5107,10 @@
         <v>8</v>
       </c>
       <c r="D178" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E178" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F178" s="2"/>
       <c r="G178" s="2"/>
@@ -5128,10 +5128,10 @@
         <v>7</v>
       </c>
       <c r="D179" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E179" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F179" s="2"/>
       <c r="G179" s="2"/>
@@ -5149,10 +5149,10 @@
         <v>7</v>
       </c>
       <c r="D180" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E180" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F180" s="2"/>
       <c r="G180" s="2"/>
@@ -5170,10 +5170,10 @@
         <v>7</v>
       </c>
       <c r="D181" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E181" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F181" s="2"/>
       <c r="G181" s="2"/>
@@ -5191,10 +5191,10 @@
         <v>7</v>
       </c>
       <c r="D182" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E182" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F182" s="2"/>
       <c r="G182" s="2"/>
@@ -5212,10 +5212,10 @@
         <v>7</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F183" s="2"/>
       <c r="G183" s="2"/>
@@ -5233,10 +5233,10 @@
         <v>7</v>
       </c>
       <c r="D184" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
@@ -5254,10 +5254,10 @@
         <v>7</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E185" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
@@ -5275,10 +5275,10 @@
         <v>8</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E186" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F186" s="2"/>
       <c r="G186" s="2"/>
@@ -5296,10 +5296,10 @@
         <v>8</v>
       </c>
       <c r="D187" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E187" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F187" s="2"/>
       <c r="G187" s="2"/>
@@ -5317,10 +5317,10 @@
         <v>8</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E188" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F188" s="2"/>
       <c r="G188" s="2"/>
@@ -5338,10 +5338,10 @@
         <v>8</v>
       </c>
       <c r="D189" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E189" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F189" s="2"/>
       <c r="G189" s="2"/>
@@ -5359,10 +5359,10 @@
         <v>8</v>
       </c>
       <c r="D190" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E190" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F190" s="2"/>
       <c r="G190" s="2"/>
@@ -5380,10 +5380,10 @@
         <v>8</v>
       </c>
       <c r="D191" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E191" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F191" s="2"/>
       <c r="G191" s="2"/>
@@ -5401,10 +5401,10 @@
         <v>8</v>
       </c>
       <c r="D192" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E192" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F192" s="2"/>
       <c r="G192" s="2"/>
@@ -5422,10 +5422,10 @@
         <v>8</v>
       </c>
       <c r="D193" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E193" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F193" s="2"/>
       <c r="G193" s="2"/>
@@ -5443,10 +5443,10 @@
         <v>8</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E194" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F194" s="2"/>
       <c r="G194" s="2"/>
@@ -5464,10 +5464,10 @@
         <v>8</v>
       </c>
       <c r="D195" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E195" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F195" s="2"/>
       <c r="G195" s="2"/>
@@ -5485,10 +5485,10 @@
         <v>8</v>
       </c>
       <c r="D196" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E196" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F196" s="2"/>
       <c r="G196" s="2"/>
@@ -5506,10 +5506,10 @@
         <v>8</v>
       </c>
       <c r="D197" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E197" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F197" s="2"/>
       <c r="G197" s="2"/>
@@ -5527,10 +5527,10 @@
         <v>7</v>
       </c>
       <c r="D198" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E198" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F198" s="2"/>
       <c r="G198" s="2"/>
@@ -5548,10 +5548,10 @@
         <v>8</v>
       </c>
       <c r="D199" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E199" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F199" s="2"/>
       <c r="G199" s="2"/>
@@ -5563,16 +5563,16 @@
         <v>216</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D200" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E200" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F200" s="2"/>
       <c r="G200" s="2"/>
@@ -5590,10 +5590,10 @@
         <v>7</v>
       </c>
       <c r="D201" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E201" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F201" s="2"/>
       <c r="G201" s="2"/>
@@ -5611,10 +5611,10 @@
         <v>8</v>
       </c>
       <c r="D202" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E202" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F202" s="2"/>
       <c r="G202" s="2"/>
@@ -5632,10 +5632,10 @@
         <v>8</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F203" s="2"/>
       <c r="G203" s="2"/>
@@ -5653,10 +5653,10 @@
         <v>8</v>
       </c>
       <c r="D204" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E204" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F204" s="2"/>
       <c r="G204" s="2"/>
@@ -5674,10 +5674,10 @@
         <v>8</v>
       </c>
       <c r="D205" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E205" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F205" s="2"/>
       <c r="G205" s="2"/>
@@ -5695,10 +5695,10 @@
         <v>8</v>
       </c>
       <c r="D206" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E206" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F206" s="2"/>
       <c r="G206" s="2"/>
@@ -5716,10 +5716,10 @@
         <v>7</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E207" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F207" s="2"/>
       <c r="G207" s="2"/>
@@ -5737,10 +5737,10 @@
         <v>7</v>
       </c>
       <c r="D208" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E208" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F208" s="2"/>
       <c r="G208" s="2"/>
@@ -5758,10 +5758,10 @@
         <v>7</v>
       </c>
       <c r="D209" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E209" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F209" s="2"/>
       <c r="G209" s="2"/>
@@ -5779,10 +5779,10 @@
         <v>7</v>
       </c>
       <c r="D210" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E210" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F210" s="2"/>
       <c r="G210" s="2"/>
@@ -5800,10 +5800,10 @@
         <v>7</v>
       </c>
       <c r="D211" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E211" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F211" s="2"/>
       <c r="G211" s="2"/>
@@ -5815,16 +5815,16 @@
         <v>228</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C212" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D212" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E212" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F212" s="2"/>
       <c r="G212" s="2"/>
@@ -5842,10 +5842,10 @@
         <v>7</v>
       </c>
       <c r="D213" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E213" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F213" s="2"/>
       <c r="G213" s="2"/>
@@ -5863,10 +5863,10 @@
         <v>8</v>
       </c>
       <c r="D214" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E214" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F214" s="2"/>
       <c r="G214" s="2"/>
@@ -5884,10 +5884,10 @@
         <v>7</v>
       </c>
       <c r="D215" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E215" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F215" s="2"/>
       <c r="G215" s="2"/>
@@ -5905,10 +5905,10 @@
         <v>7</v>
       </c>
       <c r="D216" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E216" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F216" s="2"/>
       <c r="G216" s="2"/>
@@ -5926,10 +5926,10 @@
         <v>7</v>
       </c>
       <c r="D217" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E217" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F217" s="2"/>
       <c r="G217" s="2"/>
@@ -5941,16 +5941,16 @@
         <v>234</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D218" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E218" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F218" s="2"/>
       <c r="G218" s="2"/>
@@ -5968,10 +5968,10 @@
         <v>7</v>
       </c>
       <c r="D219" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E219" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F219" s="2"/>
       <c r="G219" s="2"/>
@@ -5989,10 +5989,10 @@
         <v>8</v>
       </c>
       <c r="D220" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E220" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F220" s="2"/>
       <c r="G220" s="2"/>
@@ -6010,10 +6010,10 @@
         <v>7</v>
       </c>
       <c r="D221" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E221" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F221" s="2"/>
       <c r="G221" s="2"/>
@@ -6031,10 +6031,10 @@
         <v>7</v>
       </c>
       <c r="D222" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E222" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F222" s="2"/>
       <c r="G222" s="2"/>
@@ -6052,10 +6052,10 @@
         <v>8</v>
       </c>
       <c r="D223" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E223" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F223" s="2"/>
       <c r="G223" s="2"/>
@@ -6067,7 +6067,7 @@
         <v>240</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C224" s="6" t="s">
         <v>8</v>
@@ -6076,7 +6076,7 @@
         <v>9</v>
       </c>
       <c r="E224" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F224" s="2"/>
       <c r="G224" s="2"/>
@@ -6088,16 +6088,16 @@
         <v>241</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C225" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D225" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E225" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F225" s="2"/>
       <c r="G225" s="2"/>
@@ -6115,10 +6115,10 @@
         <v>7</v>
       </c>
       <c r="D226" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E226" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F226" s="2"/>
       <c r="G226" s="2"/>
@@ -6136,10 +6136,10 @@
         <v>7</v>
       </c>
       <c r="D227" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F227" s="2"/>
       <c r="G227" s="2"/>
@@ -6157,10 +6157,10 @@
         <v>7</v>
       </c>
       <c r="D228" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E228" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F228" s="2"/>
       <c r="G228" s="2"/>
@@ -6178,10 +6178,10 @@
         <v>7</v>
       </c>
       <c r="D229" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E229" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F229" s="2"/>
       <c r="G229" s="2"/>
@@ -6199,10 +6199,10 @@
         <v>7</v>
       </c>
       <c r="D230" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F230" s="2"/>
       <c r="G230" s="2"/>
@@ -6220,10 +6220,10 @@
         <v>7</v>
       </c>
       <c r="D231" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E231" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F231" s="2"/>
       <c r="G231" s="2"/>
@@ -6241,10 +6241,10 @@
         <v>7</v>
       </c>
       <c r="D232" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E232" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F232" s="2"/>
       <c r="G232" s="2"/>
@@ -6262,10 +6262,10 @@
         <v>7</v>
       </c>
       <c r="D233" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E233" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F233" s="2"/>
       <c r="G233" s="2"/>
@@ -6283,10 +6283,10 @@
         <v>7</v>
       </c>
       <c r="D234" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F234" s="2"/>
       <c r="G234" s="2"/>
@@ -6304,10 +6304,10 @@
         <v>7</v>
       </c>
       <c r="D235" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E235" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F235" s="2"/>
       <c r="G235" s="2"/>
@@ -6325,10 +6325,10 @@
         <v>7</v>
       </c>
       <c r="D236" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E236" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F236" s="2"/>
       <c r="G236" s="2"/>
@@ -6346,10 +6346,10 @@
         <v>7</v>
       </c>
       <c r="D237" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E237" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F237" s="2"/>
       <c r="G237" s="2"/>
@@ -6367,10 +6367,10 @@
         <v>7</v>
       </c>
       <c r="D238" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E238" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F238" s="2"/>
       <c r="G238" s="2"/>
@@ -6388,10 +6388,10 @@
         <v>7</v>
       </c>
       <c r="D239" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F239" s="2"/>
       <c r="G239" s="2"/>
@@ -6409,10 +6409,10 @@
         <v>7</v>
       </c>
       <c r="D240" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F240" s="2"/>
       <c r="G240" s="2"/>
@@ -6430,10 +6430,10 @@
         <v>7</v>
       </c>
       <c r="D241" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E241" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F241" s="2"/>
       <c r="G241" s="2"/>
@@ -6451,10 +6451,10 @@
         <v>7</v>
       </c>
       <c r="D242" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E242" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F242" s="2"/>
       <c r="G242" s="2"/>
@@ -6472,10 +6472,10 @@
         <v>7</v>
       </c>
       <c r="D243" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E243" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F243" s="2"/>
       <c r="G243" s="2"/>
@@ -6493,10 +6493,10 @@
         <v>7</v>
       </c>
       <c r="D244" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F244" s="2"/>
       <c r="G244" s="2"/>
@@ -6514,10 +6514,10 @@
         <v>7</v>
       </c>
       <c r="D245" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E245" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F245" s="2"/>
       <c r="G245" s="2"/>
@@ -6535,10 +6535,10 @@
         <v>7</v>
       </c>
       <c r="D246" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E246" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F246" s="2"/>
       <c r="G246" s="2"/>
@@ -6556,10 +6556,10 @@
         <v>7</v>
       </c>
       <c r="D247" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E247" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F247" s="2"/>
       <c r="G247" s="2"/>
@@ -6577,10 +6577,10 @@
         <v>7</v>
       </c>
       <c r="D248" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E248" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F248" s="2"/>
       <c r="G248" s="2"/>
@@ -6598,10 +6598,10 @@
         <v>7</v>
       </c>
       <c r="D249" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E249" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F249" s="2"/>
       <c r="G249" s="2"/>
@@ -6613,7 +6613,7 @@
         <v>266</v>
       </c>
       <c r="B250" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C250" s="6" t="s">
         <v>7</v>
@@ -6622,7 +6622,7 @@
         <v>9</v>
       </c>
       <c r="E250" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F250" s="2"/>
       <c r="G250" s="2"/>
@@ -6640,10 +6640,10 @@
         <v>7</v>
       </c>
       <c r="D251" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E251" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F251" s="2"/>
       <c r="G251" s="2"/>
@@ -6661,10 +6661,10 @@
         <v>7</v>
       </c>
       <c r="D252" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E252" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F252" s="2"/>
       <c r="G252" s="2"/>
@@ -6682,10 +6682,10 @@
         <v>7</v>
       </c>
       <c r="D253" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E253" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F253" s="2"/>
       <c r="G253" s="2"/>
@@ -6703,10 +6703,10 @@
         <v>7</v>
       </c>
       <c r="D254" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E254" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F254" s="2"/>
       <c r="G254" s="2"/>
@@ -6724,10 +6724,10 @@
         <v>7</v>
       </c>
       <c r="D255" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E255" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F255" s="2"/>
       <c r="G255" s="2"/>
@@ -6745,10 +6745,10 @@
         <v>8</v>
       </c>
       <c r="D256" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E256" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F256" s="2"/>
       <c r="G256" s="2"/>
@@ -6766,10 +6766,10 @@
         <v>7</v>
       </c>
       <c r="D257" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E257" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F257" s="2"/>
       <c r="G257" s="2"/>
@@ -6787,10 +6787,10 @@
         <v>7</v>
       </c>
       <c r="D258" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E258" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F258" s="2"/>
       <c r="G258" s="2"/>
@@ -6808,10 +6808,10 @@
         <v>7</v>
       </c>
       <c r="D259" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E259" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F259" s="2"/>
       <c r="G259" s="2"/>
@@ -6829,10 +6829,10 @@
         <v>7</v>
       </c>
       <c r="D260" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E260" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F260" s="2"/>
       <c r="G260" s="2"/>
@@ -6844,16 +6844,16 @@
         <v>277</v>
       </c>
       <c r="B261" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C261" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D261" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E261" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F261" s="2"/>
       <c r="G261" s="2"/>
@@ -6865,16 +6865,16 @@
         <v>278</v>
       </c>
       <c r="B262" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C262" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D262" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E262" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F262" s="2"/>
       <c r="G262" s="2"/>
@@ -6892,10 +6892,10 @@
         <v>8</v>
       </c>
       <c r="D263" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E263" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F263" s="2"/>
       <c r="G263" s="2"/>
@@ -6913,10 +6913,10 @@
         <v>8</v>
       </c>
       <c r="D264" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E264" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F264" s="2"/>
       <c r="G264" s="2"/>
@@ -6934,10 +6934,10 @@
         <v>8</v>
       </c>
       <c r="D265" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E265" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F265" s="2"/>
       <c r="G265" s="2"/>

</xml_diff>

<commit_message>
updated page data files after adding the missing blog post
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="pages" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">pages!$A$1:$E$991</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">pages!$A$1:$E$992</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="283">
   <si>
     <t>-PAGE-</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>https://heatlabs.net/blog/meet-the-team-ven0m</t>
+  </si>
+  <si>
+    <t>https://heatlabs.net/blog/minestones-and-feedback</t>
   </si>
   <si>
     <t>https://heatlabs.net/blog/new-playground-features</t>
@@ -1369,7 +1372,7 @@
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
@@ -1473,7 +1476,7 @@
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -1577,7 +1580,7 @@
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1681,7 +1684,7 @@
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -2539,10 +2542,10 @@
         <v>72</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>17</v>
@@ -2581,10 +2584,10 @@
         <v>74</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>17</v>
@@ -2605,7 +2608,7 @@
         <v>8</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>17</v>
@@ -2623,16 +2626,16 @@
         <v>76</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -2644,16 +2647,16 @@
         <v>77</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -2665,10 +2668,10 @@
         <v>78</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>17</v>
@@ -2752,7 +2755,7 @@
         <v>7</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>17</v>
@@ -2773,7 +2776,7 @@
         <v>7</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>17</v>
@@ -2938,7 +2941,7 @@
         <v>91</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>7</v>
@@ -2980,16 +2983,16 @@
         <v>93</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
@@ -3046,13 +3049,13 @@
         <v>7</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
@@ -3088,7 +3091,7 @@
         <v>7</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>17</v>
@@ -3109,7 +3112,7 @@
         <v>7</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>17</v>
@@ -3130,7 +3133,7 @@
         <v>7</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>17</v>
@@ -3154,10 +3157,10 @@
         <v>7</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
@@ -3172,13 +3175,13 @@
         <v>7</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
@@ -3193,13 +3196,13 @@
         <v>7</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -3211,16 +3214,16 @@
         <v>104</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -3232,16 +3235,16 @@
         <v>105</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
@@ -3256,13 +3259,13 @@
         <v>7</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
@@ -3274,7 +3277,7 @@
         <v>107</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>8</v>
@@ -3295,16 +3298,16 @@
         <v>108</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
@@ -3322,10 +3325,10 @@
         <v>7</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
@@ -3343,10 +3346,10 @@
         <v>7</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -3358,16 +3361,16 @@
         <v>111</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -3379,10 +3382,10 @@
         <v>112</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>17</v>
@@ -3400,10 +3403,10 @@
         <v>113</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>17</v>
@@ -3421,7 +3424,7 @@
         <v>114</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>8</v>
@@ -3445,7 +3448,7 @@
         <v>7</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>17</v>
@@ -3508,7 +3511,7 @@
         <v>7</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>17</v>
@@ -3529,7 +3532,7 @@
         <v>7</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>17</v>
@@ -3613,7 +3616,7 @@
         <v>7</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>17</v>
@@ -3655,7 +3658,7 @@
         <v>7</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>17</v>
@@ -3718,7 +3721,7 @@
         <v>7</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>17</v>
@@ -3739,7 +3742,7 @@
         <v>7</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>17</v>
@@ -3781,7 +3784,7 @@
         <v>7</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>17</v>
@@ -3802,7 +3805,7 @@
         <v>7</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>17</v>
@@ -3862,10 +3865,10 @@
         <v>135</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>17</v>
@@ -3886,7 +3889,7 @@
         <v>8</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>17</v>
@@ -3907,7 +3910,7 @@
         <v>8</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>17</v>
@@ -3925,10 +3928,10 @@
         <v>138</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>17</v>
@@ -3946,10 +3949,10 @@
         <v>139</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>17</v>
@@ -3967,7 +3970,7 @@
         <v>140</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C124" s="6" t="s">
         <v>8</v>
@@ -3991,7 +3994,7 @@
         <v>7</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>17</v>
@@ -4033,7 +4036,7 @@
         <v>7</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>17</v>
@@ -4054,7 +4057,7 @@
         <v>7</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>17</v>
@@ -4096,7 +4099,7 @@
         <v>7</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D130" s="6" t="s">
         <v>17</v>
@@ -4117,7 +4120,7 @@
         <v>7</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>17</v>
@@ -4138,7 +4141,7 @@
         <v>7</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D132" s="6" t="s">
         <v>17</v>
@@ -4159,13 +4162,13 @@
         <v>7</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
@@ -4183,10 +4186,10 @@
         <v>7</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
@@ -4198,7 +4201,7 @@
         <v>151</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C135" s="6" t="s">
         <v>7</v>
@@ -4219,7 +4222,7 @@
         <v>152</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C136" s="6" t="s">
         <v>7</v>
@@ -4306,7 +4309,7 @@
         <v>7</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D140" s="6" t="s">
         <v>17</v>
@@ -4348,7 +4351,7 @@
         <v>7</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D142" s="6" t="s">
         <v>17</v>
@@ -4369,7 +4372,7 @@
         <v>7</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D143" s="6" t="s">
         <v>17</v>
@@ -4390,7 +4393,7 @@
         <v>7</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D144" s="6" t="s">
         <v>17</v>
@@ -4453,7 +4456,7 @@
         <v>7</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D147" s="6" t="s">
         <v>17</v>
@@ -4495,7 +4498,7 @@
         <v>7</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>17</v>
@@ -4579,7 +4582,7 @@
         <v>7</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D153" s="6" t="s">
         <v>17</v>
@@ -4600,7 +4603,7 @@
         <v>7</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D154" s="6" t="s">
         <v>17</v>
@@ -4621,7 +4624,7 @@
         <v>7</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D155" s="6" t="s">
         <v>17</v>
@@ -4642,7 +4645,7 @@
         <v>7</v>
       </c>
       <c r="C156" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D156" s="6" t="s">
         <v>17</v>
@@ -4726,7 +4729,7 @@
         <v>7</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D160" s="6" t="s">
         <v>17</v>
@@ -4747,7 +4750,7 @@
         <v>7</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>17</v>
@@ -4831,7 +4834,7 @@
         <v>7</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D165" s="6" t="s">
         <v>17</v>
@@ -4849,7 +4852,7 @@
         <v>182</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C166" s="6" t="s">
         <v>8</v>
@@ -4870,10 +4873,10 @@
         <v>183</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D167" s="6" t="s">
         <v>17</v>
@@ -4891,10 +4894,10 @@
         <v>184</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>17</v>
@@ -4912,7 +4915,7 @@
         <v>185</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>8</v>
@@ -4975,7 +4978,7 @@
         <v>188</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>8</v>
@@ -4996,10 +4999,10 @@
         <v>189</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D173" s="6" t="s">
         <v>17</v>
@@ -5017,10 +5020,10 @@
         <v>190</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D174" s="6" t="s">
         <v>17</v>
@@ -5080,10 +5083,10 @@
         <v>193</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D177" s="6" t="s">
         <v>17</v>
@@ -5101,10 +5104,10 @@
         <v>194</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D178" s="6" t="s">
         <v>17</v>
@@ -5122,10 +5125,10 @@
         <v>195</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D179" s="6" t="s">
         <v>17</v>
@@ -5269,10 +5272,10 @@
         <v>202</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D186" s="6" t="s">
         <v>17</v>
@@ -5353,7 +5356,7 @@
         <v>206</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C190" s="6" t="s">
         <v>8</v>
@@ -5395,7 +5398,7 @@
         <v>208</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C192" s="6" t="s">
         <v>8</v>
@@ -5500,7 +5503,7 @@
         <v>213</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C197" s="6" t="s">
         <v>8</v>
@@ -5524,7 +5527,7 @@
         <v>7</v>
       </c>
       <c r="C198" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D198" s="6" t="s">
         <v>17</v>
@@ -5542,10 +5545,10 @@
         <v>215</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D199" s="6" t="s">
         <v>17</v>
@@ -5566,7 +5569,7 @@
         <v>8</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D200" s="6" t="s">
         <v>17</v>
@@ -5584,7 +5587,7 @@
         <v>217</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C201" s="6" t="s">
         <v>7</v>
@@ -5605,10 +5608,10 @@
         <v>218</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C202" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D202" s="6" t="s">
         <v>17</v>
@@ -5713,7 +5716,7 @@
         <v>8</v>
       </c>
       <c r="C207" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D207" s="6" t="s">
         <v>17</v>
@@ -5731,7 +5734,7 @@
         <v>224</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C208" s="6" t="s">
         <v>7</v>
@@ -5758,10 +5761,10 @@
         <v>7</v>
       </c>
       <c r="D209" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E209" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F209" s="2"/>
       <c r="G209" s="2"/>
@@ -5779,10 +5782,10 @@
         <v>7</v>
       </c>
       <c r="D210" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E210" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F210" s="2"/>
       <c r="G210" s="2"/>
@@ -5818,7 +5821,7 @@
         <v>7</v>
       </c>
       <c r="C212" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D212" s="6" t="s">
         <v>17</v>
@@ -5839,7 +5842,7 @@
         <v>7</v>
       </c>
       <c r="C213" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D213" s="6" t="s">
         <v>17</v>
@@ -5860,7 +5863,7 @@
         <v>7</v>
       </c>
       <c r="C214" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D214" s="6" t="s">
         <v>17</v>
@@ -5881,7 +5884,7 @@
         <v>7</v>
       </c>
       <c r="C215" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D215" s="6" t="s">
         <v>17</v>
@@ -5941,10 +5944,10 @@
         <v>234</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C218" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D218" s="6" t="s">
         <v>17</v>
@@ -5962,16 +5965,16 @@
         <v>235</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C219" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D219" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E219" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F219" s="2"/>
       <c r="G219" s="2"/>
@@ -5983,16 +5986,16 @@
         <v>236</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C220" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D220" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E220" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F220" s="2"/>
       <c r="G220" s="2"/>
@@ -6004,16 +6007,16 @@
         <v>237</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C221" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D221" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E221" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F221" s="2"/>
       <c r="G221" s="2"/>
@@ -6031,10 +6034,10 @@
         <v>7</v>
       </c>
       <c r="D222" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E222" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F222" s="2"/>
       <c r="G222" s="2"/>
@@ -6046,10 +6049,10 @@
         <v>239</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C223" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D223" s="6" t="s">
         <v>17</v>
@@ -6067,16 +6070,16 @@
         <v>240</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C224" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D224" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E224" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F224" s="2"/>
       <c r="G224" s="2"/>
@@ -6091,13 +6094,13 @@
         <v>7</v>
       </c>
       <c r="C225" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D225" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E225" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F225" s="2"/>
       <c r="G225" s="2"/>
@@ -6136,10 +6139,10 @@
         <v>7</v>
       </c>
       <c r="D227" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F227" s="2"/>
       <c r="G227" s="2"/>
@@ -6178,10 +6181,10 @@
         <v>7</v>
       </c>
       <c r="D229" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E229" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F229" s="2"/>
       <c r="G229" s="2"/>
@@ -6609,7 +6612,7 @@
       <c r="I249" s="2"/>
     </row>
     <row r="250">
-      <c r="A250" s="15" t="s">
+      <c r="A250" s="5" t="s">
         <v>266</v>
       </c>
       <c r="B250" s="6" t="s">
@@ -6619,10 +6622,10 @@
         <v>7</v>
       </c>
       <c r="D250" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E250" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F250" s="2"/>
       <c r="G250" s="2"/>
@@ -6630,7 +6633,7 @@
       <c r="I250" s="2"/>
     </row>
     <row r="251">
-      <c r="A251" s="5" t="s">
+      <c r="A251" s="15" t="s">
         <v>267</v>
       </c>
       <c r="B251" s="6" t="s">
@@ -6640,10 +6643,10 @@
         <v>7</v>
       </c>
       <c r="D251" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E251" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F251" s="2"/>
       <c r="G251" s="2"/>
@@ -6742,7 +6745,7 @@
         <v>7</v>
       </c>
       <c r="C256" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D256" s="6" t="s">
         <v>17</v>
@@ -6763,7 +6766,7 @@
         <v>7</v>
       </c>
       <c r="C257" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D257" s="6" t="s">
         <v>17</v>
@@ -6787,10 +6790,10 @@
         <v>7</v>
       </c>
       <c r="D258" s="6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E258" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F258" s="2"/>
       <c r="G258" s="2"/>
@@ -6808,10 +6811,10 @@
         <v>7</v>
       </c>
       <c r="D259" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E259" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F259" s="2"/>
       <c r="G259" s="2"/>
@@ -6847,7 +6850,7 @@
         <v>7</v>
       </c>
       <c r="C261" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D261" s="6" t="s">
         <v>17</v>
@@ -6945,11 +6948,21 @@
       <c r="I265" s="2"/>
     </row>
     <row r="266">
-      <c r="A266" s="16"/>
-      <c r="B266" s="17"/>
-      <c r="C266" s="17"/>
-      <c r="D266" s="17"/>
-      <c r="E266" s="17"/>
+      <c r="A266" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B266" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C266" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D266" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E266" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F266" s="2"/>
       <c r="G266" s="2"/>
       <c r="H266" s="2"/>
@@ -14930,11 +14943,22 @@
       <c r="H991" s="2"/>
       <c r="I991" s="2"/>
     </row>
+    <row r="992">
+      <c r="A992" s="16"/>
+      <c r="B992" s="17"/>
+      <c r="C992" s="17"/>
+      <c r="D992" s="17"/>
+      <c r="E992" s="17"/>
+      <c r="F992" s="2"/>
+      <c r="G992" s="2"/>
+      <c r="H992" s="2"/>
+      <c r="I992" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$E$991">
-    <sortState ref="A1:E991">
-      <sortCondition ref="A1:A991"/>
-      <sortCondition ref="D1:D991"/>
+  <autoFilter ref="$A$1:$E$992">
+    <sortState ref="A1:E992">
+      <sortCondition ref="A1:A992"/>
+      <sortCondition ref="D1:D992"/>
     </sortState>
   </autoFilter>
   <mergeCells count="4">
@@ -14944,13 +14968,13 @@
     <mergeCell ref="G13:I13"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:C991">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:C992">
       <formula1>"NOT INDEXED,NOT NEEDED,PENDING,INDEXED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D991">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D992">
       <formula1>"NOT NEEDED,NOT HTTPS,UNKNOWN,HTTPS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E991">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E992">
       <formula1>"NOT NEEDED,INVALID,UNKNOWN,VALID"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15219,7 +15243,8 @@
     <hyperlink r:id="rId262" ref="A263"/>
     <hyperlink r:id="rId263" ref="A264"/>
     <hyperlink r:id="rId264" ref="A265"/>
+    <hyperlink r:id="rId265" ref="A266"/>
   </hyperlinks>
-  <drawing r:id="rId265"/>
+  <drawing r:id="rId266"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated page data files with missing page
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -180,10 +180,10 @@
     <t>https://heatlabs.net/blog/easter-egg-friday-04</t>
   </si>
   <si>
+    <t>https://heatlabs.net/blog/easter-egg-friday-05</t>
+  </si>
+  <si>
     <t>NOT NEEDED</t>
-  </si>
-  <si>
-    <t>https://heatlabs.net/blog/easter-egg-friday-05</t>
   </si>
   <si>
     <t>https://heatlabs.net/blog/easter-egg-friday-06</t>
@@ -1369,7 +1369,7 @@
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
@@ -1473,7 +1473,7 @@
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -1577,7 +1577,7 @@
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1681,7 +1681,7 @@
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -2182,16 +2182,16 @@
         <v>54</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -2200,19 +2200,19 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="C40" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -2224,16 +2224,16 @@
         <v>57</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -2245,16 +2245,16 @@
         <v>58</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -2266,16 +2266,16 @@
         <v>59</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -2287,16 +2287,16 @@
         <v>60</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -2308,16 +2308,16 @@
         <v>61</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -2329,16 +2329,16 @@
         <v>62</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -2350,16 +2350,16 @@
         <v>63</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -2371,16 +2371,16 @@
         <v>64</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>

</xml_diff>

<commit_message>
validated HTTPS section in page data files
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="pages" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">pages!$A$1:$E$991</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">pages!$A$1:$E$990</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="287">
   <si>
     <t>-PAGE-</t>
   </si>
@@ -1384,7 +1384,7 @@
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
@@ -1488,7 +1488,7 @@
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -1592,7 +1592,7 @@
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1602,7 +1602,7 @@
       <c r="I11" s="10">
         <f>COUNTIF(D:D,"HTTPS")
 </f>
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -1696,7 +1696,7 @@
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -1706,7 +1706,7 @@
       <c r="I15" s="10">
         <f>COUNTIF(E:E,"VALID")
 </f>
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16">
@@ -2245,10 +2245,10 @@
         <v>7</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -2350,10 +2350,10 @@
         <v>8</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -2413,10 +2413,10 @@
         <v>65</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -2434,10 +2434,10 @@
         <v>65</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -2455,10 +2455,10 @@
         <v>65</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -2476,10 +2476,10 @@
         <v>65</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -2497,10 +2497,10 @@
         <v>65</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -2581,10 +2581,10 @@
         <v>8</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -2592,20 +2592,20 @@
       <c r="I57" s="2"/>
     </row>
     <row r="58">
-      <c r="A58" s="14" t="s">
-        <v>73</v>
+      <c r="A58" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -2614,13 +2614,13 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>15</v>
@@ -2635,7 +2635,7 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>8</v>
@@ -2656,13 +2656,13 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>15</v>
@@ -2677,19 +2677,19 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
@@ -2698,10 +2698,10 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>7</v>
@@ -2719,10 +2719,10 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>7</v>
@@ -2740,7 +2740,7 @@
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>8</v>
@@ -2761,13 +2761,13 @@
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>15</v>
@@ -2782,7 +2782,7 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>8</v>
@@ -2803,13 +2803,13 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>15</v>
@@ -2824,13 +2824,13 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>15</v>
@@ -2845,7 +2845,7 @@
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>8</v>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>8</v>
@@ -2887,7 +2887,7 @@
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>8</v>
@@ -2908,13 +2908,13 @@
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>15</v>
@@ -2929,13 +2929,13 @@
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>15</v>
@@ -2950,7 +2950,7 @@
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>8</v>
@@ -2971,13 +2971,13 @@
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>15</v>
@@ -2992,7 +2992,7 @@
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>8</v>
@@ -3013,13 +3013,13 @@
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>15</v>
@@ -3034,19 +3034,19 @@
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
@@ -3055,7 +3055,7 @@
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>7</v>
@@ -3076,7 +3076,7 @@
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>7</v>
@@ -3097,19 +3097,19 @@
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -3118,13 +3118,13 @@
     </row>
     <row r="83">
       <c r="A83" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>15</v>
@@ -3139,7 +3139,7 @@
     </row>
     <row r="84">
       <c r="A84" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>7</v>
@@ -3160,7 +3160,7 @@
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>7</v>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>7</v>
@@ -3202,7 +3202,7 @@
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>7</v>
@@ -3211,10 +3211,10 @@
         <v>7</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -3223,19 +3223,19 @@
     </row>
     <row r="88">
       <c r="A88" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -3244,19 +3244,19 @@
     </row>
     <row r="89">
       <c r="A89" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
@@ -3265,19 +3265,19 @@
     </row>
     <row r="90">
       <c r="A90" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
@@ -3286,19 +3286,19 @@
     </row>
     <row r="91">
       <c r="A91" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
@@ -3307,19 +3307,19 @@
     </row>
     <row r="92">
       <c r="A92" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
@@ -3328,19 +3328,19 @@
     </row>
     <row r="93">
       <c r="A93" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
@@ -3349,19 +3349,19 @@
     </row>
     <row r="94">
       <c r="A94" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -3370,7 +3370,7 @@
     </row>
     <row r="95">
       <c r="A95" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>7</v>
@@ -3379,10 +3379,10 @@
         <v>7</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -3391,7 +3391,7 @@
     </row>
     <row r="96">
       <c r="A96" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>7</v>
@@ -3400,10 +3400,10 @@
         <v>7</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
@@ -3412,19 +3412,19 @@
     </row>
     <row r="97">
       <c r="A97" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
@@ -3433,13 +3433,13 @@
     </row>
     <row r="98">
       <c r="A98" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>15</v>
@@ -3454,10 +3454,10 @@
     </row>
     <row r="99">
       <c r="A99" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>7</v>
@@ -3475,13 +3475,13 @@
     </row>
     <row r="100">
       <c r="A100" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>15</v>
@@ -3496,13 +3496,13 @@
     </row>
     <row r="101">
       <c r="A101" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>15</v>
@@ -3517,7 +3517,7 @@
     </row>
     <row r="102">
       <c r="A102" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>7</v>
@@ -3538,7 +3538,7 @@
     </row>
     <row r="103">
       <c r="A103" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>7</v>
@@ -3559,13 +3559,13 @@
     </row>
     <row r="104">
       <c r="A104" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>15</v>
@@ -3580,13 +3580,13 @@
     </row>
     <row r="105">
       <c r="A105" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>15</v>
@@ -3601,7 +3601,7 @@
     </row>
     <row r="106">
       <c r="A106" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>7</v>
@@ -3622,7 +3622,7 @@
     </row>
     <row r="107">
       <c r="A107" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>7</v>
@@ -3643,7 +3643,7 @@
     </row>
     <row r="108">
       <c r="A108" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>7</v>
@@ -3664,7 +3664,7 @@
     </row>
     <row r="109">
       <c r="A109" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>7</v>
@@ -3685,13 +3685,13 @@
     </row>
     <row r="110">
       <c r="A110" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>15</v>
@@ -3706,13 +3706,13 @@
     </row>
     <row r="111">
       <c r="A111" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>15</v>
@@ -3727,7 +3727,7 @@
     </row>
     <row r="112">
       <c r="A112" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>7</v>
@@ -3748,7 +3748,7 @@
     </row>
     <row r="113">
       <c r="A113" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>7</v>
@@ -3769,7 +3769,7 @@
     </row>
     <row r="114">
       <c r="A114" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B114" s="6" t="s">
         <v>7</v>
@@ -3790,7 +3790,7 @@
     </row>
     <row r="115">
       <c r="A115" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>7</v>
@@ -3811,7 +3811,7 @@
     </row>
     <row r="116">
       <c r="A116" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>7</v>
@@ -3832,13 +3832,13 @@
     </row>
     <row r="117">
       <c r="A117" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>15</v>
@@ -3853,13 +3853,13 @@
     </row>
     <row r="118">
       <c r="A118" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>15</v>
@@ -3874,7 +3874,7 @@
     </row>
     <row r="119">
       <c r="A119" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B119" s="6" t="s">
         <v>7</v>
@@ -3895,7 +3895,7 @@
     </row>
     <row r="120">
       <c r="A120" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>7</v>
@@ -3916,10 +3916,10 @@
     </row>
     <row r="121">
       <c r="A121" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>7</v>
@@ -3937,7 +3937,7 @@
     </row>
     <row r="122">
       <c r="A122" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>8</v>
@@ -3958,13 +3958,13 @@
     </row>
     <row r="123">
       <c r="A123" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>15</v>
@@ -3979,13 +3979,13 @@
     </row>
     <row r="124">
       <c r="A124" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>15</v>
@@ -4000,13 +4000,13 @@
     </row>
     <row r="125">
       <c r="A125" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>15</v>
@@ -4021,13 +4021,13 @@
     </row>
     <row r="126">
       <c r="A126" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>15</v>
@@ -4042,7 +4042,7 @@
     </row>
     <row r="127">
       <c r="A127" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>7</v>
@@ -4063,7 +4063,7 @@
     </row>
     <row r="128">
       <c r="A128" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>7</v>
@@ -4084,13 +4084,13 @@
     </row>
     <row r="129">
       <c r="A129" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D129" s="6" t="s">
         <v>15</v>
@@ -4105,13 +4105,13 @@
     </row>
     <row r="130">
       <c r="A130" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D130" s="6" t="s">
         <v>15</v>
@@ -4126,7 +4126,7 @@
     </row>
     <row r="131">
       <c r="A131" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>7</v>
@@ -4147,13 +4147,13 @@
     </row>
     <row r="132">
       <c r="A132" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D132" s="6" t="s">
         <v>15</v>
@@ -4168,13 +4168,13 @@
     </row>
     <row r="133">
       <c r="A133" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D133" s="6" t="s">
         <v>15</v>
@@ -4189,13 +4189,13 @@
     </row>
     <row r="134">
       <c r="A134" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D134" s="6" t="s">
         <v>15</v>
@@ -4210,19 +4210,19 @@
     </row>
     <row r="135">
       <c r="A135" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
@@ -4231,7 +4231,7 @@
     </row>
     <row r="136">
       <c r="A136" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>7</v>
@@ -4240,10 +4240,10 @@
         <v>7</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
@@ -4252,10 +4252,10 @@
     </row>
     <row r="137">
       <c r="A137" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C137" s="6" t="s">
         <v>7</v>
@@ -4273,10 +4273,10 @@
     </row>
     <row r="138">
       <c r="A138" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C138" s="6" t="s">
         <v>7</v>
@@ -4294,7 +4294,7 @@
     </row>
     <row r="139">
       <c r="A139" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>7</v>
@@ -4315,7 +4315,7 @@
     </row>
     <row r="140">
       <c r="A140" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>7</v>
@@ -4336,7 +4336,7 @@
     </row>
     <row r="141">
       <c r="A141" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B141" s="6" t="s">
         <v>7</v>
@@ -4357,7 +4357,7 @@
     </row>
     <row r="142">
       <c r="A142" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B142" s="6" t="s">
         <v>7</v>
@@ -4378,13 +4378,13 @@
     </row>
     <row r="143">
       <c r="A143" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B143" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D143" s="6" t="s">
         <v>15</v>
@@ -4399,13 +4399,13 @@
     </row>
     <row r="144">
       <c r="A144" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B144" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D144" s="6" t="s">
         <v>15</v>
@@ -4420,13 +4420,13 @@
     </row>
     <row r="145">
       <c r="A145" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B145" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D145" s="6" t="s">
         <v>15</v>
@@ -4441,13 +4441,13 @@
     </row>
     <row r="146">
       <c r="A146" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B146" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D146" s="6" t="s">
         <v>15</v>
@@ -4462,7 +4462,7 @@
     </row>
     <row r="147">
       <c r="A147" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B147" s="6" t="s">
         <v>7</v>
@@ -4483,7 +4483,7 @@
     </row>
     <row r="148">
       <c r="A148" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B148" s="6" t="s">
         <v>7</v>
@@ -4504,13 +4504,13 @@
     </row>
     <row r="149">
       <c r="A149" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B149" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>15</v>
@@ -4525,7 +4525,7 @@
     </row>
     <row r="150">
       <c r="A150" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B150" s="6" t="s">
         <v>7</v>
@@ -4546,13 +4546,13 @@
     </row>
     <row r="151">
       <c r="A151" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B151" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D151" s="6" t="s">
         <v>15</v>
@@ -4567,7 +4567,7 @@
     </row>
     <row r="152">
       <c r="A152" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B152" s="6" t="s">
         <v>7</v>
@@ -4588,7 +4588,7 @@
     </row>
     <row r="153">
       <c r="A153" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B153" s="6" t="s">
         <v>7</v>
@@ -4609,7 +4609,7 @@
     </row>
     <row r="154">
       <c r="A154" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B154" s="6" t="s">
         <v>7</v>
@@ -4630,13 +4630,13 @@
     </row>
     <row r="155">
       <c r="A155" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B155" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D155" s="6" t="s">
         <v>15</v>
@@ -4651,13 +4651,13 @@
     </row>
     <row r="156">
       <c r="A156" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B156" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C156" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D156" s="6" t="s">
         <v>15</v>
@@ -4672,7 +4672,7 @@
     </row>
     <row r="157">
       <c r="A157" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B157" s="6" t="s">
         <v>7</v>
@@ -4693,7 +4693,7 @@
     </row>
     <row r="158">
       <c r="A158" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B158" s="6" t="s">
         <v>7</v>
@@ -4714,7 +4714,7 @@
     </row>
     <row r="159">
       <c r="A159" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B159" s="6" t="s">
         <v>7</v>
@@ -4735,7 +4735,7 @@
     </row>
     <row r="160">
       <c r="A160" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B160" s="6" t="s">
         <v>7</v>
@@ -4756,7 +4756,7 @@
     </row>
     <row r="161">
       <c r="A161" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B161" s="6" t="s">
         <v>7</v>
@@ -4777,13 +4777,13 @@
     </row>
     <row r="162">
       <c r="A162" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B162" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D162" s="6" t="s">
         <v>15</v>
@@ -4798,13 +4798,13 @@
     </row>
     <row r="163">
       <c r="A163" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B163" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D163" s="6" t="s">
         <v>15</v>
@@ -4819,7 +4819,7 @@
     </row>
     <row r="164">
       <c r="A164" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B164" s="6" t="s">
         <v>7</v>
@@ -4840,7 +4840,7 @@
     </row>
     <row r="165">
       <c r="A165" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B165" s="6" t="s">
         <v>7</v>
@@ -4861,7 +4861,7 @@
     </row>
     <row r="166">
       <c r="A166" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B166" s="6" t="s">
         <v>7</v>
@@ -4882,7 +4882,7 @@
     </row>
     <row r="167">
       <c r="A167" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B167" s="6" t="s">
         <v>7</v>
@@ -4903,13 +4903,13 @@
     </row>
     <row r="168">
       <c r="A168" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>15</v>
@@ -4924,13 +4924,13 @@
     </row>
     <row r="169">
       <c r="A169" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D169" s="6" t="s">
         <v>15</v>
@@ -4945,13 +4945,13 @@
     </row>
     <row r="170">
       <c r="A170" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D170" s="6" t="s">
         <v>15</v>
@@ -4966,10 +4966,10 @@
     </row>
     <row r="171">
       <c r="A171" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C171" s="6" t="s">
         <v>8</v>
@@ -4987,7 +4987,7 @@
     </row>
     <row r="172">
       <c r="A172" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B172" s="6" t="s">
         <v>7</v>
@@ -5008,7 +5008,7 @@
     </row>
     <row r="173">
       <c r="A173" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B173" s="6" t="s">
         <v>7</v>
@@ -5029,10 +5029,10 @@
     </row>
     <row r="174">
       <c r="A174" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C174" s="6" t="s">
         <v>8</v>
@@ -5050,13 +5050,13 @@
     </row>
     <row r="175">
       <c r="A175" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D175" s="6" t="s">
         <v>15</v>
@@ -5071,13 +5071,13 @@
     </row>
     <row r="176">
       <c r="A176" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D176" s="6" t="s">
         <v>15</v>
@@ -5092,7 +5092,7 @@
     </row>
     <row r="177">
       <c r="A177" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B177" s="6" t="s">
         <v>8</v>
@@ -5113,7 +5113,7 @@
     </row>
     <row r="178">
       <c r="A178" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B178" s="6" t="s">
         <v>8</v>
@@ -5134,13 +5134,13 @@
     </row>
     <row r="179">
       <c r="A179" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D179" s="6" t="s">
         <v>15</v>
@@ -5155,13 +5155,13 @@
     </row>
     <row r="180">
       <c r="A180" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D180" s="6" t="s">
         <v>15</v>
@@ -5176,13 +5176,13 @@
     </row>
     <row r="181">
       <c r="A181" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C181" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D181" s="6" t="s">
         <v>15</v>
@@ -5197,7 +5197,7 @@
     </row>
     <row r="182">
       <c r="A182" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B182" s="6" t="s">
         <v>7</v>
@@ -5218,7 +5218,7 @@
     </row>
     <row r="183">
       <c r="A183" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B183" s="6" t="s">
         <v>7</v>
@@ -5239,7 +5239,7 @@
     </row>
     <row r="184">
       <c r="A184" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B184" s="6" t="s">
         <v>7</v>
@@ -5260,7 +5260,7 @@
     </row>
     <row r="185">
       <c r="A185" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B185" s="6" t="s">
         <v>7</v>
@@ -5281,7 +5281,7 @@
     </row>
     <row r="186">
       <c r="A186" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B186" s="6" t="s">
         <v>7</v>
@@ -5302,7 +5302,7 @@
     </row>
     <row r="187">
       <c r="A187" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B187" s="6" t="s">
         <v>7</v>
@@ -5323,13 +5323,13 @@
     </row>
     <row r="188">
       <c r="A188" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C188" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D188" s="6" t="s">
         <v>15</v>
@@ -5344,7 +5344,7 @@
     </row>
     <row r="189">
       <c r="A189" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B189" s="6" t="s">
         <v>8</v>
@@ -5365,7 +5365,7 @@
     </row>
     <row r="190">
       <c r="A190" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B190" s="6" t="s">
         <v>8</v>
@@ -5386,7 +5386,7 @@
     </row>
     <row r="191">
       <c r="A191" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B191" s="6" t="s">
         <v>8</v>
@@ -5407,10 +5407,10 @@
     </row>
     <row r="192">
       <c r="A192" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C192" s="6" t="s">
         <v>8</v>
@@ -5428,7 +5428,7 @@
     </row>
     <row r="193">
       <c r="A193" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B193" s="6" t="s">
         <v>7</v>
@@ -5449,13 +5449,13 @@
     </row>
     <row r="194">
       <c r="A194" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B194" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C194" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D194" s="6" t="s">
         <v>15</v>
@@ -5470,13 +5470,13 @@
     </row>
     <row r="195">
       <c r="A195" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C195" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D195" s="6" t="s">
         <v>15</v>
@@ -5491,7 +5491,7 @@
     </row>
     <row r="196">
       <c r="A196" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B196" s="6" t="s">
         <v>8</v>
@@ -5512,7 +5512,7 @@
     </row>
     <row r="197">
       <c r="A197" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B197" s="6" t="s">
         <v>8</v>
@@ -5533,7 +5533,7 @@
     </row>
     <row r="198">
       <c r="A198" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B198" s="6" t="s">
         <v>8</v>
@@ -5554,10 +5554,10 @@
     </row>
     <row r="199">
       <c r="A199" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C199" s="6" t="s">
         <v>8</v>
@@ -5575,13 +5575,13 @@
     </row>
     <row r="200">
       <c r="A200" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B200" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D200" s="6" t="s">
         <v>15</v>
@@ -5596,10 +5596,10 @@
     </row>
     <row r="201">
       <c r="A201" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C201" s="6" t="s">
         <v>7</v>
@@ -5617,7 +5617,7 @@
     </row>
     <row r="202">
       <c r="A202" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B202" s="6" t="s">
         <v>8</v>
@@ -5638,19 +5638,19 @@
     </row>
     <row r="203">
       <c r="A203" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F203" s="2"/>
       <c r="G203" s="2"/>
@@ -5659,13 +5659,13 @@
     </row>
     <row r="204">
       <c r="A204" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C204" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D204" s="6" t="s">
         <v>15</v>
@@ -5680,13 +5680,13 @@
     </row>
     <row r="205">
       <c r="A205" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B205" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C205" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D205" s="6" t="s">
         <v>15</v>
@@ -5701,7 +5701,7 @@
     </row>
     <row r="206">
       <c r="A206" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B206" s="6" t="s">
         <v>8</v>
@@ -5722,13 +5722,13 @@
     </row>
     <row r="207">
       <c r="A207" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B207" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C207" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D207" s="6" t="s">
         <v>15</v>
@@ -5743,7 +5743,7 @@
     </row>
     <row r="208">
       <c r="A208" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B208" s="6" t="s">
         <v>8</v>
@@ -5764,13 +5764,13 @@
     </row>
     <row r="209">
       <c r="A209" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B209" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C209" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D209" s="6" t="s">
         <v>15</v>
@@ -5785,10 +5785,10 @@
     </row>
     <row r="210">
       <c r="A210" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C210" s="6" t="s">
         <v>7</v>
@@ -5806,19 +5806,19 @@
     </row>
     <row r="211">
       <c r="A211" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B211" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C211" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D211" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E211" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F211" s="2"/>
       <c r="G211" s="2"/>
@@ -5827,19 +5827,19 @@
     </row>
     <row r="212">
       <c r="A212" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C212" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D212" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E212" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F212" s="2"/>
       <c r="G212" s="2"/>
@@ -5848,7 +5848,7 @@
     </row>
     <row r="213">
       <c r="A213" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B213" s="6" t="s">
         <v>7</v>
@@ -5857,10 +5857,10 @@
         <v>7</v>
       </c>
       <c r="D213" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E213" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F213" s="2"/>
       <c r="G213" s="2"/>
@@ -5869,7 +5869,7 @@
     </row>
     <row r="214">
       <c r="A214" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B214" s="6" t="s">
         <v>7</v>
@@ -5890,7 +5890,7 @@
     </row>
     <row r="215">
       <c r="A215" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B215" s="6" t="s">
         <v>7</v>
@@ -5911,7 +5911,7 @@
     </row>
     <row r="216">
       <c r="A216" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B216" s="6" t="s">
         <v>7</v>
@@ -5932,13 +5932,13 @@
     </row>
     <row r="217">
       <c r="A217" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B217" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C217" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D217" s="6" t="s">
         <v>15</v>
@@ -5953,13 +5953,13 @@
     </row>
     <row r="218">
       <c r="A218" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B218" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C218" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D218" s="6" t="s">
         <v>15</v>
@@ -5974,7 +5974,7 @@
     </row>
     <row r="219">
       <c r="A219" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B219" s="6" t="s">
         <v>7</v>
@@ -5995,7 +5995,7 @@
     </row>
     <row r="220">
       <c r="A220" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B220" s="6" t="s">
         <v>7</v>
@@ -6016,10 +6016,10 @@
     </row>
     <row r="221">
       <c r="A221" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C221" s="6" t="s">
         <v>7</v>
@@ -6037,19 +6037,19 @@
     </row>
     <row r="222">
       <c r="A222" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B222" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C222" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D222" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E222" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F222" s="2"/>
       <c r="G222" s="2"/>
@@ -6058,19 +6058,19 @@
     </row>
     <row r="223">
       <c r="A223" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C223" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D223" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E223" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F223" s="2"/>
       <c r="G223" s="2"/>
@@ -6079,13 +6079,13 @@
     </row>
     <row r="224">
       <c r="A224" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C224" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D224" s="6" t="s">
         <v>15</v>
@@ -6100,7 +6100,7 @@
     </row>
     <row r="225">
       <c r="A225" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B225" s="6" t="s">
         <v>7</v>
@@ -6109,10 +6109,10 @@
         <v>7</v>
       </c>
       <c r="D225" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E225" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F225" s="2"/>
       <c r="G225" s="2"/>
@@ -6121,19 +6121,19 @@
     </row>
     <row r="226">
       <c r="A226" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C226" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D226" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E226" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F226" s="2"/>
       <c r="G226" s="2"/>
@@ -6142,19 +6142,19 @@
     </row>
     <row r="227">
       <c r="A227" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C227" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D227" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F227" s="2"/>
       <c r="G227" s="2"/>
@@ -6163,7 +6163,7 @@
     </row>
     <row r="228">
       <c r="A228" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B228" s="6" t="s">
         <v>7</v>
@@ -6172,10 +6172,10 @@
         <v>7</v>
       </c>
       <c r="D228" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E228" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F228" s="2"/>
       <c r="G228" s="2"/>
@@ -6184,7 +6184,7 @@
     </row>
     <row r="229">
       <c r="A229" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B229" s="6" t="s">
         <v>7</v>
@@ -6204,20 +6204,20 @@
       <c r="I229" s="2"/>
     </row>
     <row r="230">
-      <c r="A230" s="5" t="s">
-        <v>245</v>
+      <c r="A230" s="14" t="s">
+        <v>246</v>
       </c>
       <c r="B230" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C230" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D230" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F230" s="2"/>
       <c r="G230" s="2"/>
@@ -6225,20 +6225,20 @@
       <c r="I230" s="2"/>
     </row>
     <row r="231">
-      <c r="A231" s="14" t="s">
-        <v>246</v>
+      <c r="A231" s="5" t="s">
+        <v>247</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C231" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D231" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E231" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F231" s="2"/>
       <c r="G231" s="2"/>
@@ -6247,7 +6247,7 @@
     </row>
     <row r="232">
       <c r="A232" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B232" s="6" t="s">
         <v>7</v>
@@ -6268,7 +6268,7 @@
     </row>
     <row r="233">
       <c r="A233" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B233" s="6" t="s">
         <v>7</v>
@@ -6277,10 +6277,10 @@
         <v>7</v>
       </c>
       <c r="D233" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E233" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F233" s="2"/>
       <c r="G233" s="2"/>
@@ -6289,7 +6289,7 @@
     </row>
     <row r="234">
       <c r="A234" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B234" s="6" t="s">
         <v>7</v>
@@ -6298,10 +6298,10 @@
         <v>7</v>
       </c>
       <c r="D234" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F234" s="2"/>
       <c r="G234" s="2"/>
@@ -6310,7 +6310,7 @@
     </row>
     <row r="235">
       <c r="A235" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B235" s="6" t="s">
         <v>7</v>
@@ -6331,7 +6331,7 @@
     </row>
     <row r="236">
       <c r="A236" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B236" s="6" t="s">
         <v>7</v>
@@ -6352,7 +6352,7 @@
     </row>
     <row r="237">
       <c r="A237" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B237" s="6" t="s">
         <v>7</v>
@@ -6373,7 +6373,7 @@
     </row>
     <row r="238">
       <c r="A238" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B238" s="6" t="s">
         <v>7</v>
@@ -6394,7 +6394,7 @@
     </row>
     <row r="239">
       <c r="A239" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B239" s="6" t="s">
         <v>7</v>
@@ -6415,7 +6415,7 @@
     </row>
     <row r="240">
       <c r="A240" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B240" s="6" t="s">
         <v>7</v>
@@ -6436,7 +6436,7 @@
     </row>
     <row r="241">
       <c r="A241" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B241" s="6" t="s">
         <v>7</v>
@@ -6457,7 +6457,7 @@
     </row>
     <row r="242">
       <c r="A242" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B242" s="6" t="s">
         <v>7</v>
@@ -6478,7 +6478,7 @@
     </row>
     <row r="243">
       <c r="A243" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B243" s="6" t="s">
         <v>7</v>
@@ -6499,7 +6499,7 @@
     </row>
     <row r="244">
       <c r="A244" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B244" s="6" t="s">
         <v>7</v>
@@ -6520,7 +6520,7 @@
     </row>
     <row r="245">
       <c r="A245" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B245" s="6" t="s">
         <v>7</v>
@@ -6541,7 +6541,7 @@
     </row>
     <row r="246">
       <c r="A246" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B246" s="6" t="s">
         <v>7</v>
@@ -6562,7 +6562,7 @@
     </row>
     <row r="247">
       <c r="A247" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B247" s="6" t="s">
         <v>7</v>
@@ -6583,7 +6583,7 @@
     </row>
     <row r="248">
       <c r="A248" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B248" s="6" t="s">
         <v>7</v>
@@ -6603,8 +6603,8 @@
       <c r="I248" s="2"/>
     </row>
     <row r="249">
-      <c r="A249" s="5" t="s">
-        <v>264</v>
+      <c r="A249" s="15" t="s">
+        <v>265</v>
       </c>
       <c r="B249" s="6" t="s">
         <v>7</v>
@@ -6624,8 +6624,8 @@
       <c r="I249" s="2"/>
     </row>
     <row r="250">
-      <c r="A250" s="15" t="s">
-        <v>265</v>
+      <c r="A250" s="5" t="s">
+        <v>266</v>
       </c>
       <c r="B250" s="6" t="s">
         <v>7</v>
@@ -6646,7 +6646,7 @@
     </row>
     <row r="251">
       <c r="A251" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B251" s="6" t="s">
         <v>7</v>
@@ -6667,7 +6667,7 @@
     </row>
     <row r="252">
       <c r="A252" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B252" s="6" t="s">
         <v>7</v>
@@ -6688,7 +6688,7 @@
     </row>
     <row r="253">
       <c r="A253" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B253" s="6" t="s">
         <v>7</v>
@@ -6709,7 +6709,7 @@
     </row>
     <row r="254">
       <c r="A254" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B254" s="6" t="s">
         <v>7</v>
@@ -6718,10 +6718,10 @@
         <v>7</v>
       </c>
       <c r="D254" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E254" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F254" s="2"/>
       <c r="G254" s="2"/>
@@ -6730,7 +6730,7 @@
     </row>
     <row r="255">
       <c r="A255" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B255" s="6" t="s">
         <v>7</v>
@@ -6739,10 +6739,10 @@
         <v>7</v>
       </c>
       <c r="D255" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E255" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F255" s="2"/>
       <c r="G255" s="2"/>
@@ -6751,7 +6751,7 @@
     </row>
     <row r="256">
       <c r="A256" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B256" s="6" t="s">
         <v>7</v>
@@ -6772,7 +6772,7 @@
     </row>
     <row r="257">
       <c r="A257" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B257" s="6" t="s">
         <v>7</v>
@@ -6793,7 +6793,7 @@
     </row>
     <row r="258">
       <c r="A258" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B258" s="6" t="s">
         <v>7</v>
@@ -6814,7 +6814,7 @@
     </row>
     <row r="259">
       <c r="A259" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B259" s="6" t="s">
         <v>7</v>
@@ -6835,7 +6835,7 @@
     </row>
     <row r="260">
       <c r="A260" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B260" s="6" t="s">
         <v>7</v>
@@ -6856,7 +6856,7 @@
     </row>
     <row r="261">
       <c r="A261" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B261" s="6" t="s">
         <v>7</v>
@@ -6877,7 +6877,7 @@
     </row>
     <row r="262">
       <c r="A262" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B262" s="6" t="s">
         <v>7</v>
@@ -6886,10 +6886,10 @@
         <v>7</v>
       </c>
       <c r="D262" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E262" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F262" s="2"/>
       <c r="G262" s="2"/>
@@ -6898,7 +6898,7 @@
     </row>
     <row r="263">
       <c r="A263" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B263" s="6" t="s">
         <v>7</v>
@@ -6907,10 +6907,10 @@
         <v>7</v>
       </c>
       <c r="D263" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E263" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F263" s="2"/>
       <c r="G263" s="2"/>
@@ -6919,7 +6919,7 @@
     </row>
     <row r="264">
       <c r="A264" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B264" s="6" t="s">
         <v>7</v>
@@ -6940,7 +6940,7 @@
     </row>
     <row r="265">
       <c r="A265" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B265" s="6" t="s">
         <v>7</v>
@@ -6961,13 +6961,13 @@
     </row>
     <row r="266">
       <c r="A266" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B266" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C266" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D266" s="6" t="s">
         <v>15</v>
@@ -6982,7 +6982,7 @@
     </row>
     <row r="267">
       <c r="A267" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B267" s="6" t="s">
         <v>7</v>
@@ -7003,7 +7003,7 @@
     </row>
     <row r="268">
       <c r="A268" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B268" s="6" t="s">
         <v>7</v>
@@ -7024,7 +7024,7 @@
     </row>
     <row r="269">
       <c r="A269" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B269" s="6" t="s">
         <v>7</v>
@@ -7045,19 +7045,19 @@
     </row>
     <row r="270">
       <c r="A270" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B270" s="6" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="C270" s="6" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="D270" s="6" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="E270" s="6" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="F270" s="2"/>
       <c r="G270" s="2"/>
@@ -7065,21 +7065,11 @@
       <c r="I270" s="2"/>
     </row>
     <row r="271">
-      <c r="A271" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="B271" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C271" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D271" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E271" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="A271" s="16"/>
+      <c r="B271" s="17"/>
+      <c r="C271" s="17"/>
+      <c r="D271" s="17"/>
+      <c r="E271" s="17"/>
       <c r="F271" s="2"/>
       <c r="G271" s="2"/>
       <c r="H271" s="2"/>
@@ -14994,22 +14984,11 @@
       <c r="H990" s="2"/>
       <c r="I990" s="2"/>
     </row>
-    <row r="991">
-      <c r="A991" s="16"/>
-      <c r="B991" s="17"/>
-      <c r="C991" s="17"/>
-      <c r="D991" s="17"/>
-      <c r="E991" s="17"/>
-      <c r="F991" s="2"/>
-      <c r="G991" s="2"/>
-      <c r="H991" s="2"/>
-      <c r="I991" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$E$991">
-    <sortState ref="A1:E991">
-      <sortCondition ref="A1:A991"/>
-      <sortCondition ref="D1:D991"/>
+  <autoFilter ref="$A$1:$E$990">
+    <sortState ref="A1:E990">
+      <sortCondition ref="A1:A990"/>
+      <sortCondition ref="D1:D990"/>
     </sortState>
   </autoFilter>
   <mergeCells count="4">
@@ -15019,13 +14998,13 @@
     <mergeCell ref="G13:I13"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:C991">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:C990">
       <formula1>"NOT INDEXED,NOT NEEDED,PENDING,INDEXED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D991">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D990">
       <formula1>"NOT NEEDED,NOT HTTPS,UNKNOWN,HTTPS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E991">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E990">
       <formula1>"NOT NEEDED,INVALID,UNKNOWN,VALID"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15299,8 +15278,7 @@
     <hyperlink r:id="rId267" ref="A268"/>
     <hyperlink r:id="rId268" ref="A269"/>
     <hyperlink r:id="rId269" ref="A270"/>
-    <hyperlink r:id="rId270" ref="A271"/>
   </hyperlinks>
-  <drawing r:id="rId271"/>
+  <drawing r:id="rId270"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated page data files with 2 missing pages
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="pages" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">pages!$A$1:$E$990</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">pages!$A$1:$E$992</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="290">
   <si>
     <t>-PAGE-</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>https://heatlabs.net/blog/easter-egg-friday-13</t>
+  </si>
+  <si>
+    <t>https://heatlabs.net/blog/easter-egg-friday-14</t>
+  </si>
+  <si>
+    <t>https://heatlabs.net/blog/easter-egg-friday-15</t>
   </si>
   <si>
     <t>https://heatlabs.net/blog/exploring-animation-and-movement-desync</t>
@@ -1595,7 +1601,7 @@
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1699,7 +1705,7 @@
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -2515,10 +2521,10 @@
         <v>70</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>15</v>
@@ -2536,10 +2542,10 @@
         <v>71</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>15</v>
@@ -2574,7 +2580,7 @@
       <c r="I56" s="2"/>
     </row>
     <row r="57">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -2584,10 +2590,10 @@
         <v>7</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -2605,10 +2611,10 @@
         <v>7</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -2616,20 +2622,20 @@
       <c r="I58" s="2"/>
     </row>
     <row r="59">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="14" t="s">
         <v>75</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -2644,13 +2650,13 @@
         <v>8</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -2662,10 +2668,10 @@
         <v>77</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>15</v>
@@ -2686,13 +2692,13 @@
         <v>8</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
@@ -2731,10 +2737,10 @@
         <v>7</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -2746,7 +2752,7 @@
         <v>81</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>7</v>
@@ -2770,7 +2776,7 @@
         <v>8</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>15</v>
@@ -2791,7 +2797,7 @@
         <v>8</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>15</v>
@@ -2809,10 +2815,10 @@
         <v>84</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>15</v>
@@ -2851,7 +2857,7 @@
         <v>86</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>7</v>
@@ -2914,10 +2920,10 @@
         <v>89</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>15</v>
@@ -2938,7 +2944,7 @@
         <v>8</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>15</v>
@@ -2956,10 +2962,10 @@
         <v>91</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>15</v>
@@ -2980,7 +2986,7 @@
         <v>8</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>15</v>
@@ -3001,7 +3007,7 @@
         <v>8</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>15</v>
@@ -3022,7 +3028,7 @@
         <v>8</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>15</v>
@@ -3040,16 +3046,16 @@
         <v>95</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
@@ -3061,16 +3067,16 @@
         <v>96</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
@@ -3109,10 +3115,10 @@
         <v>7</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -3130,10 +3136,10 @@
         <v>7</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
@@ -3214,10 +3220,10 @@
         <v>7</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -3232,7 +3238,7 @@
         <v>7</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>15</v>
@@ -3271,7 +3277,7 @@
         <v>106</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>8</v>
@@ -3313,7 +3319,7 @@
         <v>108</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>8</v>
@@ -3334,7 +3340,7 @@
         <v>109</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>7</v>
@@ -3358,13 +3364,13 @@
         <v>7</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -3376,16 +3382,16 @@
         <v>111</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -3418,10 +3424,10 @@
         <v>113</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>15</v>
@@ -3445,10 +3451,10 @@
         <v>7</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
@@ -3463,7 +3469,7 @@
         <v>8</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>15</v>
@@ -3484,7 +3490,7 @@
         <v>7</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>15</v>
@@ -3502,7 +3508,7 @@
         <v>117</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>7</v>
@@ -3526,7 +3532,7 @@
         <v>7</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>15</v>
@@ -3568,7 +3574,7 @@
         <v>7</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>15</v>
@@ -3610,7 +3616,7 @@
         <v>7</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>15</v>
@@ -3841,7 +3847,7 @@
         <v>7</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>15</v>
@@ -3883,7 +3889,7 @@
         <v>7</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>15</v>
@@ -3922,7 +3928,7 @@
         <v>137</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>7</v>
@@ -3943,7 +3949,7 @@
         <v>138</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>7</v>
@@ -3967,7 +3973,7 @@
         <v>8</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>15</v>
@@ -3985,7 +3991,7 @@
         <v>140</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C124" s="6" t="s">
         <v>7</v>
@@ -4048,10 +4054,10 @@
         <v>143</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>15</v>
@@ -4093,7 +4099,7 @@
         <v>7</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D129" s="6" t="s">
         <v>15</v>
@@ -4135,7 +4141,7 @@
         <v>7</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>15</v>
@@ -4156,7 +4162,7 @@
         <v>7</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D132" s="6" t="s">
         <v>15</v>
@@ -4222,10 +4228,10 @@
         <v>7</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
@@ -4240,7 +4246,7 @@
         <v>7</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D136" s="6" t="s">
         <v>15</v>
@@ -4258,16 +4264,16 @@
         <v>153</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C137" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
@@ -4300,7 +4306,7 @@
         <v>155</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>7</v>
@@ -4387,7 +4393,7 @@
         <v>7</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D143" s="6" t="s">
         <v>15</v>
@@ -4471,7 +4477,7 @@
         <v>7</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D147" s="6" t="s">
         <v>15</v>
@@ -4513,7 +4519,7 @@
         <v>7</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>15</v>
@@ -4534,7 +4540,7 @@
         <v>7</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D150" s="6" t="s">
         <v>15</v>
@@ -4555,7 +4561,7 @@
         <v>7</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D151" s="6" t="s">
         <v>15</v>
@@ -4576,7 +4582,7 @@
         <v>7</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D152" s="6" t="s">
         <v>15</v>
@@ -4639,7 +4645,7 @@
         <v>7</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D155" s="6" t="s">
         <v>15</v>
@@ -4681,7 +4687,7 @@
         <v>7</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D157" s="6" t="s">
         <v>15</v>
@@ -4786,7 +4792,7 @@
         <v>7</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D162" s="6" t="s">
         <v>15</v>
@@ -4828,7 +4834,7 @@
         <v>7</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D164" s="6" t="s">
         <v>15</v>
@@ -4909,10 +4915,10 @@
         <v>184</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>15</v>
@@ -4975,7 +4981,7 @@
         <v>7</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D171" s="6" t="s">
         <v>15</v>
@@ -4993,7 +4999,7 @@
         <v>188</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>8</v>
@@ -5035,7 +5041,7 @@
         <v>190</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C174" s="6" t="s">
         <v>8</v>
@@ -5059,7 +5065,7 @@
         <v>7</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D175" s="6" t="s">
         <v>15</v>
@@ -5098,10 +5104,10 @@
         <v>193</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D177" s="6" t="s">
         <v>15</v>
@@ -5140,10 +5146,10 @@
         <v>195</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D179" s="6" t="s">
         <v>15</v>
@@ -5203,10 +5209,10 @@
         <v>198</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C182" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D182" s="6" t="s">
         <v>15</v>
@@ -5329,10 +5335,10 @@
         <v>204</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C188" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D188" s="6" t="s">
         <v>15</v>
@@ -5350,10 +5356,10 @@
         <v>205</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C189" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D189" s="6" t="s">
         <v>15</v>
@@ -5413,7 +5419,7 @@
         <v>208</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C192" s="6" t="s">
         <v>8</v>
@@ -5434,7 +5440,7 @@
         <v>209</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C193" s="6" t="s">
         <v>8</v>
@@ -5458,7 +5464,7 @@
         <v>7</v>
       </c>
       <c r="C194" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D194" s="6" t="s">
         <v>15</v>
@@ -5476,7 +5482,7 @@
         <v>211</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C195" s="6" t="s">
         <v>8</v>
@@ -5497,10 +5503,10 @@
         <v>212</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D196" s="6" t="s">
         <v>15</v>
@@ -5560,7 +5566,7 @@
         <v>215</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C199" s="6" t="s">
         <v>8</v>
@@ -5581,10 +5587,10 @@
         <v>216</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D200" s="6" t="s">
         <v>15</v>
@@ -5602,10 +5608,10 @@
         <v>217</v>
       </c>
       <c r="B201" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C201" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="C201" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="D201" s="6" t="s">
         <v>15</v>
@@ -5623,7 +5629,7 @@
         <v>218</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C202" s="6" t="s">
         <v>7</v>
@@ -5644,16 +5650,16 @@
         <v>219</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F203" s="2"/>
       <c r="G203" s="2"/>
@@ -5668,7 +5674,7 @@
         <v>8</v>
       </c>
       <c r="C204" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D204" s="6" t="s">
         <v>15</v>
@@ -5686,16 +5692,16 @@
         <v>221</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C205" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D205" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E205" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F205" s="2"/>
       <c r="G205" s="2"/>
@@ -5710,7 +5716,7 @@
         <v>8</v>
       </c>
       <c r="C206" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D206" s="6" t="s">
         <v>15</v>
@@ -5731,7 +5737,7 @@
         <v>8</v>
       </c>
       <c r="C207" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D207" s="6" t="s">
         <v>15</v>
@@ -5752,7 +5758,7 @@
         <v>8</v>
       </c>
       <c r="C208" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D208" s="6" t="s">
         <v>15</v>
@@ -5773,7 +5779,7 @@
         <v>8</v>
       </c>
       <c r="C209" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D209" s="6" t="s">
         <v>15</v>
@@ -5791,10 +5797,10 @@
         <v>226</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C210" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D210" s="6" t="s">
         <v>15</v>
@@ -5818,10 +5824,10 @@
         <v>7</v>
       </c>
       <c r="D211" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E211" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F211" s="2"/>
       <c r="G211" s="2"/>
@@ -5839,10 +5845,10 @@
         <v>7</v>
       </c>
       <c r="D212" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E212" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F212" s="2"/>
       <c r="G212" s="2"/>
@@ -5854,16 +5860,16 @@
         <v>229</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C213" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D213" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E213" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F213" s="2"/>
       <c r="G213" s="2"/>
@@ -5881,10 +5887,10 @@
         <v>7</v>
       </c>
       <c r="D214" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E214" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F214" s="2"/>
       <c r="G214" s="2"/>
@@ -5997,14 +6003,14 @@
       <c r="I219" s="2"/>
     </row>
     <row r="220">
-      <c r="A220" s="14" t="s">
+      <c r="A220" s="5" t="s">
         <v>236</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C220" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D220" s="6" t="s">
         <v>15</v>
@@ -6039,14 +6045,14 @@
       <c r="I221" s="2"/>
     </row>
     <row r="222">
-      <c r="A222" s="5" t="s">
+      <c r="A222" s="14" t="s">
         <v>238</v>
       </c>
       <c r="B222" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C222" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D222" s="6" t="s">
         <v>15</v>
@@ -6070,10 +6076,10 @@
         <v>7</v>
       </c>
       <c r="D223" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E223" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F223" s="2"/>
       <c r="G223" s="2"/>
@@ -6088,7 +6094,7 @@
         <v>8</v>
       </c>
       <c r="C224" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D224" s="6" t="s">
         <v>15</v>
@@ -6112,10 +6118,10 @@
         <v>7</v>
       </c>
       <c r="D225" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E225" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F225" s="2"/>
       <c r="G225" s="2"/>
@@ -6127,10 +6133,10 @@
         <v>242</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D226" s="6" t="s">
         <v>15</v>
@@ -6148,16 +6154,16 @@
         <v>243</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C227" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D227" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F227" s="2"/>
       <c r="G227" s="2"/>
@@ -6175,10 +6181,10 @@
         <v>7</v>
       </c>
       <c r="D228" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E228" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F228" s="2"/>
       <c r="G228" s="2"/>
@@ -6190,16 +6196,16 @@
         <v>245</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C229" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D229" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E229" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F229" s="2"/>
       <c r="G229" s="2"/>
@@ -6217,10 +6223,10 @@
         <v>7</v>
       </c>
       <c r="D230" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F230" s="2"/>
       <c r="G230" s="2"/>
@@ -6228,20 +6234,20 @@
       <c r="I230" s="2"/>
     </row>
     <row r="231">
-      <c r="A231" s="14" t="s">
+      <c r="A231" s="5" t="s">
         <v>247</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C231" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D231" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E231" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F231" s="2"/>
       <c r="G231" s="2"/>
@@ -6259,10 +6265,10 @@
         <v>7</v>
       </c>
       <c r="D232" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E232" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F232" s="2"/>
       <c r="G232" s="2"/>
@@ -6270,11 +6276,11 @@
       <c r="I232" s="2"/>
     </row>
     <row r="233">
-      <c r="A233" s="5" t="s">
+      <c r="A233" s="14" t="s">
         <v>249</v>
       </c>
       <c r="B233" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C233" s="6" t="s">
         <v>7</v>
@@ -6301,10 +6307,10 @@
         <v>7</v>
       </c>
       <c r="D234" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F234" s="2"/>
       <c r="G234" s="2"/>
@@ -6364,10 +6370,10 @@
         <v>7</v>
       </c>
       <c r="D237" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E237" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F237" s="2"/>
       <c r="G237" s="2"/>
@@ -6606,7 +6612,7 @@
       <c r="I248" s="2"/>
     </row>
     <row r="249">
-      <c r="A249" s="15" t="s">
+      <c r="A249" s="5" t="s">
         <v>265</v>
       </c>
       <c r="B249" s="6" t="s">
@@ -6648,7 +6654,7 @@
       <c r="I250" s="2"/>
     </row>
     <row r="251">
-      <c r="A251" s="5" t="s">
+      <c r="A251" s="15" t="s">
         <v>267</v>
       </c>
       <c r="B251" s="6" t="s">
@@ -6742,10 +6748,10 @@
         <v>7</v>
       </c>
       <c r="D255" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E255" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F255" s="2"/>
       <c r="G255" s="2"/>
@@ -6784,10 +6790,10 @@
         <v>7</v>
       </c>
       <c r="D257" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E257" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F257" s="2"/>
       <c r="G257" s="2"/>
@@ -6910,10 +6916,10 @@
         <v>7</v>
       </c>
       <c r="D263" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E263" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F263" s="2"/>
       <c r="G263" s="2"/>
@@ -6952,10 +6958,10 @@
         <v>7</v>
       </c>
       <c r="D265" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E265" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F265" s="2"/>
       <c r="G265" s="2"/>
@@ -6991,7 +6997,7 @@
         <v>7</v>
       </c>
       <c r="C267" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D267" s="6" t="s">
         <v>15</v>
@@ -7012,7 +7018,7 @@
         <v>7</v>
       </c>
       <c r="C268" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D268" s="6" t="s">
         <v>15</v>
@@ -7072,16 +7078,16 @@
         <v>287</v>
       </c>
       <c r="B271" s="6" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="C271" s="6" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="D271" s="6" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="E271" s="6" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="F271" s="2"/>
       <c r="G271" s="2"/>
@@ -7089,22 +7095,42 @@
       <c r="I271" s="2"/>
     </row>
     <row r="272">
-      <c r="A272" s="16"/>
-      <c r="B272" s="17"/>
-      <c r="C272" s="17"/>
-      <c r="D272" s="17"/>
-      <c r="E272" s="17"/>
+      <c r="A272" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B272" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C272" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D272" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E272" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="F272" s="2"/>
       <c r="G272" s="2"/>
       <c r="H272" s="2"/>
       <c r="I272" s="2"/>
     </row>
     <row r="273">
-      <c r="A273" s="16"/>
-      <c r="B273" s="17"/>
-      <c r="C273" s="17"/>
-      <c r="D273" s="17"/>
-      <c r="E273" s="17"/>
+      <c r="A273" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B273" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C273" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D273" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E273" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="F273" s="2"/>
       <c r="G273" s="2"/>
       <c r="H273" s="2"/>
@@ -14997,11 +15023,33 @@
       <c r="H990" s="2"/>
       <c r="I990" s="2"/>
     </row>
+    <row r="991">
+      <c r="A991" s="16"/>
+      <c r="B991" s="17"/>
+      <c r="C991" s="17"/>
+      <c r="D991" s="17"/>
+      <c r="E991" s="17"/>
+      <c r="F991" s="2"/>
+      <c r="G991" s="2"/>
+      <c r="H991" s="2"/>
+      <c r="I991" s="2"/>
+    </row>
+    <row r="992">
+      <c r="A992" s="16"/>
+      <c r="B992" s="17"/>
+      <c r="C992" s="17"/>
+      <c r="D992" s="17"/>
+      <c r="E992" s="17"/>
+      <c r="F992" s="2"/>
+      <c r="G992" s="2"/>
+      <c r="H992" s="2"/>
+      <c r="I992" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$E$990">
-    <sortState ref="A1:E990">
-      <sortCondition ref="A1:A990"/>
-      <sortCondition ref="D1:D990"/>
+  <autoFilter ref="$A$1:$E$992">
+    <sortState ref="A1:E992">
+      <sortCondition ref="A1:A992"/>
+      <sortCondition ref="D1:D992"/>
     </sortState>
   </autoFilter>
   <mergeCells count="4">
@@ -15011,13 +15059,13 @@
     <mergeCell ref="G13:I13"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:C990">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:C992">
       <formula1>"NOT INDEXED,NOT NEEDED,PENDING,INDEXED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D990">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D992">
       <formula1>"NOT NEEDED,NOT HTTPS,UNKNOWN,HTTPS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E990">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E992">
       <formula1>"NOT NEEDED,INVALID,UNKNOWN,VALID"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15292,7 +15340,9 @@
     <hyperlink r:id="rId268" ref="A269"/>
     <hyperlink r:id="rId269" ref="A270"/>
     <hyperlink r:id="rId270" ref="A271"/>
+    <hyperlink r:id="rId271" ref="A272"/>
+    <hyperlink r:id="rId272" ref="A273"/>
   </hyperlinks>
-  <drawing r:id="rId271"/>
+  <drawing r:id="rId273"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated page data filed with 1 new page
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="294">
   <si>
     <t>-PAGE-</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>https://heatlabs.net/blog/heatlabs-coming-to-steam</t>
+  </si>
+  <si>
+    <t>https://heatlabs.net/blog/heatlabs-on-android</t>
   </si>
   <si>
     <t>https://heatlabs.net/blog/hunting-for-potential-hidden-servers</t>
@@ -1406,7 +1409,7 @@
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
@@ -1510,7 +1513,7 @@
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -1614,7 +1617,7 @@
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1718,7 +1721,7 @@
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -2698,7 +2701,7 @@
       <c r="I61" s="2"/>
     </row>
     <row r="62">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="14" t="s">
         <v>78</v>
       </c>
       <c r="B62" s="6" t="s">
@@ -2744,10 +2747,10 @@
         <v>80</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>15</v>
@@ -2765,16 +2768,16 @@
         <v>81</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
@@ -2786,16 +2789,16 @@
         <v>82</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -2807,7 +2810,7 @@
         <v>83</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>7</v>
@@ -2852,7 +2855,7 @@
         <v>8</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>15</v>
@@ -2891,10 +2894,10 @@
         <v>87</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>15</v>
@@ -2912,10 +2915,10 @@
         <v>88</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>15</v>
@@ -2936,7 +2939,7 @@
         <v>8</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>15</v>
@@ -2957,7 +2960,7 @@
         <v>8</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>15</v>
@@ -2978,7 +2981,7 @@
         <v>8</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>15</v>
@@ -2996,7 +2999,7 @@
         <v>92</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>7</v>
@@ -3017,10 +3020,10 @@
         <v>93</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>15</v>
@@ -3062,7 +3065,7 @@
         <v>8</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>15</v>
@@ -3104,7 +3107,7 @@
         <v>8</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>15</v>
@@ -3118,7 +3121,7 @@
       <c r="I81" s="2"/>
     </row>
     <row r="82">
-      <c r="A82" s="14" t="s">
+      <c r="A82" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B82" s="6" t="s">
@@ -3139,20 +3142,20 @@
       <c r="I82" s="2"/>
     </row>
     <row r="83">
-      <c r="A83" s="5" t="s">
+      <c r="A83" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
@@ -3212,10 +3215,10 @@
         <v>7</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
@@ -3317,10 +3320,10 @@
         <v>7</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
@@ -3335,13 +3338,13 @@
         <v>7</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
@@ -3356,13 +3359,13 @@
         <v>7</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
@@ -3374,16 +3377,16 @@
         <v>110</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -3395,16 +3398,16 @@
         <v>111</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -3419,13 +3422,13 @@
         <v>7</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
@@ -3437,16 +3440,16 @@
         <v>113</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
@@ -3458,7 +3461,7 @@
         <v>114</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>7</v>
@@ -3485,10 +3488,10 @@
         <v>7</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -3506,10 +3509,10 @@
         <v>7</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -3521,16 +3524,16 @@
         <v>117</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
@@ -3542,7 +3545,7 @@
         <v>118</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>7</v>
@@ -3563,7 +3566,7 @@
         <v>119</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>7</v>
@@ -3584,10 +3587,10 @@
         <v>120</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>15</v>
@@ -3608,7 +3611,7 @@
         <v>7</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>15</v>
@@ -3671,7 +3674,7 @@
         <v>7</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>15</v>
@@ -3692,7 +3695,7 @@
         <v>7</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>15</v>
@@ -3944,7 +3947,7 @@
         <v>7</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>15</v>
@@ -3965,7 +3968,7 @@
         <v>7</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>15</v>
@@ -4025,7 +4028,7 @@
         <v>141</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>7</v>
@@ -4088,7 +4091,7 @@
         <v>144</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C128" s="6" t="s">
         <v>7</v>
@@ -4109,10 +4112,10 @@
         <v>145</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D129" s="6" t="s">
         <v>15</v>
@@ -4130,10 +4133,10 @@
         <v>146</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D130" s="6" t="s">
         <v>15</v>
@@ -4196,7 +4199,7 @@
         <v>7</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D133" s="6" t="s">
         <v>15</v>
@@ -4217,7 +4220,7 @@
         <v>7</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D134" s="6" t="s">
         <v>15</v>
@@ -4259,7 +4262,7 @@
         <v>7</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D136" s="6" t="s">
         <v>15</v>
@@ -4280,7 +4283,7 @@
         <v>7</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D137" s="6" t="s">
         <v>15</v>
@@ -4325,10 +4328,10 @@
         <v>7</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
@@ -4346,10 +4349,10 @@
         <v>7</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
@@ -4361,7 +4364,7 @@
         <v>157</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>7</v>
@@ -4382,7 +4385,7 @@
         <v>158</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C142" s="6" t="s">
         <v>7</v>
@@ -4490,7 +4493,7 @@
         <v>7</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D147" s="6" t="s">
         <v>15</v>
@@ -4511,7 +4514,7 @@
         <v>7</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D148" s="6" t="s">
         <v>15</v>
@@ -4532,7 +4535,7 @@
         <v>7</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>15</v>
@@ -4553,7 +4556,7 @@
         <v>7</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D150" s="6" t="s">
         <v>15</v>
@@ -4616,7 +4619,7 @@
         <v>7</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D153" s="6" t="s">
         <v>15</v>
@@ -4658,7 +4661,7 @@
         <v>7</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D155" s="6" t="s">
         <v>15</v>
@@ -4742,7 +4745,7 @@
         <v>7</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D159" s="6" t="s">
         <v>15</v>
@@ -4763,7 +4766,7 @@
         <v>7</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D160" s="6" t="s">
         <v>15</v>
@@ -4889,7 +4892,7 @@
         <v>7</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D166" s="6" t="s">
         <v>15</v>
@@ -4910,7 +4913,7 @@
         <v>7</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D167" s="6" t="s">
         <v>15</v>
@@ -5012,10 +5015,10 @@
         <v>188</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D172" s="6" t="s">
         <v>15</v>
@@ -5033,10 +5036,10 @@
         <v>189</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D173" s="6" t="s">
         <v>15</v>
@@ -5054,10 +5057,10 @@
         <v>190</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D174" s="6" t="s">
         <v>15</v>
@@ -5075,7 +5078,7 @@
         <v>191</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C175" s="6" t="s">
         <v>8</v>
@@ -5138,7 +5141,7 @@
         <v>194</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C178" s="6" t="s">
         <v>8</v>
@@ -5159,10 +5162,10 @@
         <v>195</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D179" s="6" t="s">
         <v>15</v>
@@ -5180,10 +5183,10 @@
         <v>196</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D180" s="6" t="s">
         <v>15</v>
@@ -5225,7 +5228,7 @@
         <v>8</v>
       </c>
       <c r="C182" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D182" s="6" t="s">
         <v>15</v>
@@ -5243,7 +5246,7 @@
         <v>199</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C183" s="6" t="s">
         <v>7</v>
@@ -5264,10 +5267,10 @@
         <v>200</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C184" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D184" s="6" t="s">
         <v>15</v>
@@ -5285,10 +5288,10 @@
         <v>201</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D185" s="6" t="s">
         <v>15</v>
@@ -5432,10 +5435,10 @@
         <v>208</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C192" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D192" s="6" t="s">
         <v>15</v>
@@ -5516,7 +5519,7 @@
         <v>212</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C196" s="6" t="s">
         <v>8</v>
@@ -5561,7 +5564,7 @@
         <v>7</v>
       </c>
       <c r="C198" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D198" s="6" t="s">
         <v>15</v>
@@ -5579,10 +5582,10 @@
         <v>215</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D199" s="6" t="s">
         <v>15</v>
@@ -5663,7 +5666,7 @@
         <v>219</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>8</v>
@@ -5687,7 +5690,7 @@
         <v>7</v>
       </c>
       <c r="C204" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D204" s="6" t="s">
         <v>15</v>
@@ -5705,7 +5708,7 @@
         <v>221</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C205" s="6" t="s">
         <v>7</v>
@@ -5747,16 +5750,16 @@
         <v>223</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C207" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E207" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F207" s="2"/>
       <c r="G207" s="2"/>
@@ -5768,16 +5771,16 @@
         <v>224</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C208" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D208" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E208" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F208" s="2"/>
       <c r="G208" s="2"/>
@@ -5834,7 +5837,7 @@
         <v>8</v>
       </c>
       <c r="C211" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D211" s="6" t="s">
         <v>15</v>
@@ -5876,7 +5879,7 @@
         <v>8</v>
       </c>
       <c r="C213" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D213" s="6" t="s">
         <v>15</v>
@@ -5894,7 +5897,7 @@
         <v>230</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C214" s="6" t="s">
         <v>7</v>
@@ -5915,16 +5918,16 @@
         <v>231</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C215" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D215" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E215" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F215" s="2"/>
       <c r="G215" s="2"/>
@@ -5936,7 +5939,7 @@
         <v>232</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C216" s="6" t="s">
         <v>7</v>
@@ -5963,10 +5966,10 @@
         <v>7</v>
       </c>
       <c r="D217" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E217" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F217" s="2"/>
       <c r="G217" s="2"/>
@@ -5995,11 +5998,11 @@
       <c r="I218" s="2"/>
     </row>
     <row r="219">
-      <c r="A219" s="14" t="s">
+      <c r="A219" s="5" t="s">
         <v>235</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C219" s="6" t="s">
         <v>7</v>
@@ -6016,11 +6019,11 @@
       <c r="I219" s="2"/>
     </row>
     <row r="220">
-      <c r="A220" s="5" t="s">
+      <c r="A220" s="14" t="s">
         <v>236</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C220" s="6" t="s">
         <v>7</v>
@@ -6121,14 +6124,14 @@
       <c r="I224" s="2"/>
     </row>
     <row r="225">
-      <c r="A225" s="14" t="s">
+      <c r="A225" s="5" t="s">
         <v>241</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C225" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D225" s="6" t="s">
         <v>15</v>
@@ -6142,14 +6145,14 @@
       <c r="I225" s="2"/>
     </row>
     <row r="226">
-      <c r="A226" s="5" t="s">
+      <c r="A226" s="14" t="s">
         <v>242</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D226" s="6" t="s">
         <v>15</v>
@@ -6167,7 +6170,7 @@
         <v>243</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C227" s="6" t="s">
         <v>7</v>
@@ -6188,16 +6191,16 @@
         <v>244</v>
       </c>
       <c r="B228" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C228" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D228" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E228" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F228" s="2"/>
       <c r="G228" s="2"/>
@@ -6209,16 +6212,16 @@
         <v>245</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C229" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D229" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E229" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F229" s="2"/>
       <c r="G229" s="2"/>
@@ -6230,10 +6233,10 @@
         <v>246</v>
       </c>
       <c r="B230" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C230" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D230" s="6" t="s">
         <v>15</v>
@@ -6272,16 +6275,16 @@
         <v>248</v>
       </c>
       <c r="B232" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C232" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D232" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E232" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F232" s="2"/>
       <c r="G232" s="2"/>
@@ -6293,7 +6296,7 @@
         <v>249</v>
       </c>
       <c r="B233" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C233" s="6" t="s">
         <v>7</v>
@@ -6320,10 +6323,10 @@
         <v>7</v>
       </c>
       <c r="D234" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F234" s="2"/>
       <c r="G234" s="2"/>
@@ -6352,20 +6355,20 @@
       <c r="I235" s="2"/>
     </row>
     <row r="236">
-      <c r="A236" s="14" t="s">
+      <c r="A236" s="5" t="s">
         <v>252</v>
       </c>
       <c r="B236" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C236" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D236" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E236" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F236" s="2"/>
       <c r="G236" s="2"/>
@@ -6373,11 +6376,11 @@
       <c r="I236" s="2"/>
     </row>
     <row r="237">
-      <c r="A237" s="5" t="s">
+      <c r="A237" s="14" t="s">
         <v>253</v>
       </c>
       <c r="B237" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C237" s="6" t="s">
         <v>7</v>
@@ -6425,10 +6428,10 @@
         <v>7</v>
       </c>
       <c r="D239" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F239" s="2"/>
       <c r="G239" s="2"/>
@@ -6446,10 +6449,10 @@
         <v>7</v>
       </c>
       <c r="D240" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F240" s="2"/>
       <c r="G240" s="2"/>
@@ -6467,10 +6470,10 @@
         <v>7</v>
       </c>
       <c r="D241" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E241" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F241" s="2"/>
       <c r="G241" s="2"/>
@@ -6866,10 +6869,10 @@
         <v>7</v>
       </c>
       <c r="D260" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E260" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F260" s="2"/>
       <c r="G260" s="2"/>
@@ -6887,10 +6890,10 @@
         <v>7</v>
       </c>
       <c r="D261" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E261" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F261" s="2"/>
       <c r="G261" s="2"/>
@@ -7034,10 +7037,10 @@
         <v>7</v>
       </c>
       <c r="D268" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E268" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F268" s="2"/>
       <c r="G268" s="2"/>
@@ -7055,10 +7058,10 @@
         <v>7</v>
       </c>
       <c r="D269" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E269" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F269" s="2"/>
       <c r="G269" s="2"/>
@@ -7115,7 +7118,7 @@
         <v>7</v>
       </c>
       <c r="C272" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D272" s="6" t="s">
         <v>15</v>
@@ -7196,16 +7199,16 @@
         <v>292</v>
       </c>
       <c r="B276" s="6" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="C276" s="6" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="D276" s="6" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="E276" s="6" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="F276" s="2"/>
       <c r="G276" s="2"/>
@@ -7213,11 +7216,21 @@
       <c r="I276" s="2"/>
     </row>
     <row r="277">
-      <c r="A277" s="16"/>
-      <c r="B277" s="17"/>
-      <c r="C277" s="17"/>
-      <c r="D277" s="17"/>
-      <c r="E277" s="17"/>
+      <c r="A277" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B277" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C277" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D277" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E277" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="F277" s="2"/>
       <c r="G277" s="2"/>
       <c r="H277" s="2"/>
@@ -15399,7 +15412,8 @@
     <hyperlink r:id="rId273" ref="A274"/>
     <hyperlink r:id="rId274" ref="A275"/>
     <hyperlink r:id="rId275" ref="A276"/>
+    <hyperlink r:id="rId276" ref="A277"/>
   </hyperlinks>
-  <drawing r:id="rId276"/>
+  <drawing r:id="rId277"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated page data files with new easter egg friday blog post
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -219,10 +219,10 @@
     <t>https://heatlabs.net/blog/easter-egg-friday-12</t>
   </si>
   <si>
+    <t>https://heatlabs.net/blog/easter-egg-friday-13</t>
+  </si>
+  <si>
     <t>NOT NEEDED</t>
-  </si>
-  <si>
-    <t>https://heatlabs.net/blog/easter-egg-friday-13</t>
   </si>
   <si>
     <t>https://heatlabs.net/blog/easter-egg-friday-14</t>
@@ -1409,7 +1409,7 @@
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
@@ -1513,7 +1513,7 @@
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -2495,10 +2495,10 @@
         <v>67</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>15</v>
@@ -2513,13 +2513,13 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="C53" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>15</v>
@@ -2537,10 +2537,10 @@
         <v>70</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>15</v>
@@ -2558,10 +2558,10 @@
         <v>71</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>15</v>
@@ -7220,16 +7220,16 @@
         <v>293</v>
       </c>
       <c r="B277" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C277" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D277" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E277" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F277" s="2"/>
       <c r="G277" s="2"/>

</xml_diff>

<commit_message>
updated page data files with new steam news post
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="295">
   <si>
     <t>-PAGE-</t>
   </si>
@@ -778,6 +778,9 @@
   </si>
   <si>
     <t>https://heatlabs.net/steam-news/join-the-lodestar-program</t>
+  </si>
+  <si>
+    <t>https://heatlabs.net/steam-news/the-source-of-heat</t>
   </si>
   <si>
     <t>https://heatlabs.net/tanks</t>
@@ -1409,7 +1412,7 @@
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
@@ -1513,7 +1516,7 @@
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -1617,7 +1620,7 @@
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1721,7 +1724,7 @@
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -6418,20 +6421,20 @@
       <c r="I238" s="2"/>
     </row>
     <row r="239">
-      <c r="A239" s="5" t="s">
+      <c r="A239" s="14" t="s">
         <v>255</v>
       </c>
       <c r="B239" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C239" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D239" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F239" s="2"/>
       <c r="G239" s="2"/>
@@ -6449,10 +6452,10 @@
         <v>7</v>
       </c>
       <c r="D240" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F240" s="2"/>
       <c r="G240" s="2"/>
@@ -6470,10 +6473,10 @@
         <v>7</v>
       </c>
       <c r="D241" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E241" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F241" s="2"/>
       <c r="G241" s="2"/>
@@ -6491,10 +6494,10 @@
         <v>7</v>
       </c>
       <c r="D242" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E242" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F242" s="2"/>
       <c r="G242" s="2"/>
@@ -6890,10 +6893,10 @@
         <v>7</v>
       </c>
       <c r="D261" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E261" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F261" s="2"/>
       <c r="G261" s="2"/>
@@ -6911,10 +6914,10 @@
         <v>7</v>
       </c>
       <c r="D262" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E262" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F262" s="2"/>
       <c r="G262" s="2"/>
@@ -7058,10 +7061,10 @@
         <v>7</v>
       </c>
       <c r="D269" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E269" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F269" s="2"/>
       <c r="G269" s="2"/>
@@ -7079,10 +7082,10 @@
         <v>7</v>
       </c>
       <c r="D270" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E270" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F270" s="2"/>
       <c r="G270" s="2"/>
@@ -7139,7 +7142,7 @@
         <v>7</v>
       </c>
       <c r="C273" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D273" s="6" t="s">
         <v>15</v>
@@ -7220,16 +7223,16 @@
         <v>293</v>
       </c>
       <c r="B277" s="6" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="C277" s="6" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="D277" s="6" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="E277" s="6" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="F277" s="2"/>
       <c r="G277" s="2"/>
@@ -7237,11 +7240,21 @@
       <c r="I277" s="2"/>
     </row>
     <row r="278">
-      <c r="A278" s="16"/>
-      <c r="B278" s="17"/>
-      <c r="C278" s="17"/>
-      <c r="D278" s="17"/>
-      <c r="E278" s="17"/>
+      <c r="A278" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B278" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C278" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D278" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E278" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="F278" s="2"/>
       <c r="G278" s="2"/>
       <c r="H278" s="2"/>
@@ -15413,7 +15426,8 @@
     <hyperlink r:id="rId274" ref="A275"/>
     <hyperlink r:id="rId275" ref="A276"/>
     <hyperlink r:id="rId276" ref="A277"/>
+    <hyperlink r:id="rId277" ref="A278"/>
   </hyperlinks>
-  <drawing r:id="rId277"/>
+  <drawing r:id="rId278"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated page data files with new legal page
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="296">
   <si>
     <t>-PAGE-</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>https://heatlabs.net/legal/code-of-conduct</t>
+  </si>
+  <si>
+    <t>https://heatlabs.net/legal/player-content-policy</t>
   </si>
   <si>
     <t>https://heatlabs.net/legal/privacy-policy</t>
@@ -1412,7 +1415,7 @@
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
@@ -1516,7 +1519,7 @@
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -1620,7 +1623,7 @@
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1724,7 +1727,7 @@
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -3376,20 +3379,20 @@
       <c r="I93" s="2"/>
     </row>
     <row r="94">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="14" t="s">
         <v>110</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -3401,16 +3404,16 @@
         <v>111</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -3422,16 +3425,16 @@
         <v>112</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
@@ -3446,13 +3449,13 @@
         <v>7</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
@@ -3464,16 +3467,16 @@
         <v>114</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
@@ -3485,7 +3488,7 @@
         <v>115</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>7</v>
@@ -3512,10 +3515,10 @@
         <v>7</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -3533,10 +3536,10 @@
         <v>7</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
@@ -3548,16 +3551,16 @@
         <v>118</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
@@ -3569,7 +3572,7 @@
         <v>119</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>7</v>
@@ -3590,7 +3593,7 @@
         <v>120</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>7</v>
@@ -3611,10 +3614,10 @@
         <v>121</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>15</v>
@@ -3635,7 +3638,7 @@
         <v>7</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>15</v>
@@ -3698,7 +3701,7 @@
         <v>7</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>15</v>
@@ -3719,7 +3722,7 @@
         <v>7</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>15</v>
@@ -3971,7 +3974,7 @@
         <v>7</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>15</v>
@@ -3992,7 +3995,7 @@
         <v>7</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>15</v>
@@ -4052,7 +4055,7 @@
         <v>142</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>7</v>
@@ -4115,7 +4118,7 @@
         <v>145</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C129" s="6" t="s">
         <v>7</v>
@@ -4136,10 +4139,10 @@
         <v>146</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D130" s="6" t="s">
         <v>15</v>
@@ -4157,10 +4160,10 @@
         <v>147</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>15</v>
@@ -4223,7 +4226,7 @@
         <v>7</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D134" s="6" t="s">
         <v>15</v>
@@ -4244,7 +4247,7 @@
         <v>7</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>15</v>
@@ -4286,7 +4289,7 @@
         <v>7</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D137" s="6" t="s">
         <v>15</v>
@@ -4307,7 +4310,7 @@
         <v>7</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D138" s="6" t="s">
         <v>15</v>
@@ -4352,10 +4355,10 @@
         <v>7</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
@@ -4373,10 +4376,10 @@
         <v>7</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
@@ -4388,7 +4391,7 @@
         <v>158</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C142" s="6" t="s">
         <v>7</v>
@@ -4409,7 +4412,7 @@
         <v>159</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>7</v>
@@ -4517,7 +4520,7 @@
         <v>7</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D148" s="6" t="s">
         <v>15</v>
@@ -4538,7 +4541,7 @@
         <v>7</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>15</v>
@@ -4643,7 +4646,7 @@
         <v>7</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D154" s="6" t="s">
         <v>15</v>
@@ -4685,7 +4688,7 @@
         <v>7</v>
       </c>
       <c r="C156" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D156" s="6" t="s">
         <v>15</v>
@@ -4769,7 +4772,7 @@
         <v>7</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D160" s="6" t="s">
         <v>15</v>
@@ -4790,7 +4793,7 @@
         <v>7</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>15</v>
@@ -4916,7 +4919,7 @@
         <v>7</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D167" s="6" t="s">
         <v>15</v>
@@ -4937,7 +4940,7 @@
         <v>7</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>15</v>
@@ -5039,10 +5042,10 @@
         <v>189</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D173" s="6" t="s">
         <v>15</v>
@@ -5060,10 +5063,10 @@
         <v>190</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D174" s="6" t="s">
         <v>15</v>
@@ -5081,10 +5084,10 @@
         <v>191</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D175" s="6" t="s">
         <v>15</v>
@@ -5102,7 +5105,7 @@
         <v>192</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C176" s="6" t="s">
         <v>8</v>
@@ -5165,7 +5168,7 @@
         <v>195</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C179" s="6" t="s">
         <v>8</v>
@@ -5186,10 +5189,10 @@
         <v>196</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D180" s="6" t="s">
         <v>15</v>
@@ -5207,10 +5210,10 @@
         <v>197</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C181" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D181" s="6" t="s">
         <v>15</v>
@@ -5252,7 +5255,7 @@
         <v>8</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D183" s="6" t="s">
         <v>15</v>
@@ -5270,7 +5273,7 @@
         <v>200</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C184" s="6" t="s">
         <v>7</v>
@@ -5291,10 +5294,10 @@
         <v>201</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D185" s="6" t="s">
         <v>15</v>
@@ -5312,10 +5315,10 @@
         <v>202</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D186" s="6" t="s">
         <v>15</v>
@@ -5459,10 +5462,10 @@
         <v>209</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C193" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D193" s="6" t="s">
         <v>15</v>
@@ -5543,7 +5546,7 @@
         <v>213</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C197" s="6" t="s">
         <v>8</v>
@@ -5588,7 +5591,7 @@
         <v>7</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D199" s="6" t="s">
         <v>15</v>
@@ -5606,10 +5609,10 @@
         <v>216</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D200" s="6" t="s">
         <v>15</v>
@@ -5690,7 +5693,7 @@
         <v>220</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C204" s="6" t="s">
         <v>8</v>
@@ -5714,7 +5717,7 @@
         <v>7</v>
       </c>
       <c r="C205" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D205" s="6" t="s">
         <v>15</v>
@@ -5732,7 +5735,7 @@
         <v>222</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C206" s="6" t="s">
         <v>7</v>
@@ -5774,16 +5777,16 @@
         <v>224</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C208" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D208" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E208" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F208" s="2"/>
       <c r="G208" s="2"/>
@@ -5795,16 +5798,16 @@
         <v>225</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C209" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D209" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E209" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F209" s="2"/>
       <c r="G209" s="2"/>
@@ -5861,7 +5864,7 @@
         <v>8</v>
       </c>
       <c r="C212" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D212" s="6" t="s">
         <v>15</v>
@@ -5903,7 +5906,7 @@
         <v>8</v>
       </c>
       <c r="C214" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D214" s="6" t="s">
         <v>15</v>
@@ -5921,7 +5924,7 @@
         <v>231</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C215" s="6" t="s">
         <v>7</v>
@@ -5942,16 +5945,16 @@
         <v>232</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C216" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D216" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E216" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F216" s="2"/>
       <c r="G216" s="2"/>
@@ -5963,7 +5966,7 @@
         <v>233</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C217" s="6" t="s">
         <v>7</v>
@@ -5990,10 +5993,10 @@
         <v>7</v>
       </c>
       <c r="D218" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E218" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F218" s="2"/>
       <c r="G218" s="2"/>
@@ -6022,11 +6025,11 @@
       <c r="I219" s="2"/>
     </row>
     <row r="220">
-      <c r="A220" s="14" t="s">
+      <c r="A220" s="5" t="s">
         <v>236</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C220" s="6" t="s">
         <v>7</v>
@@ -6043,11 +6046,11 @@
       <c r="I220" s="2"/>
     </row>
     <row r="221">
-      <c r="A221" s="5" t="s">
+      <c r="A221" s="14" t="s">
         <v>237</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C221" s="6" t="s">
         <v>7</v>
@@ -6148,14 +6151,14 @@
       <c r="I225" s="2"/>
     </row>
     <row r="226">
-      <c r="A226" s="14" t="s">
+      <c r="A226" s="5" t="s">
         <v>242</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D226" s="6" t="s">
         <v>15</v>
@@ -6169,14 +6172,14 @@
       <c r="I226" s="2"/>
     </row>
     <row r="227">
-      <c r="A227" s="5" t="s">
+      <c r="A227" s="14" t="s">
         <v>243</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C227" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D227" s="6" t="s">
         <v>15</v>
@@ -6194,7 +6197,7 @@
         <v>244</v>
       </c>
       <c r="B228" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C228" s="6" t="s">
         <v>7</v>
@@ -6215,16 +6218,16 @@
         <v>245</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C229" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D229" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E229" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F229" s="2"/>
       <c r="G229" s="2"/>
@@ -6236,16 +6239,16 @@
         <v>246</v>
       </c>
       <c r="B230" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C230" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D230" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F230" s="2"/>
       <c r="G230" s="2"/>
@@ -6257,7 +6260,7 @@
         <v>247</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C231" s="6" t="s">
         <v>7</v>
@@ -6299,16 +6302,16 @@
         <v>249</v>
       </c>
       <c r="B233" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C233" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D233" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E233" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F233" s="2"/>
       <c r="G233" s="2"/>
@@ -6320,7 +6323,7 @@
         <v>250</v>
       </c>
       <c r="B234" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C234" s="6" t="s">
         <v>7</v>
@@ -6347,10 +6350,10 @@
         <v>7</v>
       </c>
       <c r="D235" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E235" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F235" s="2"/>
       <c r="G235" s="2"/>
@@ -6379,20 +6382,20 @@
       <c r="I236" s="2"/>
     </row>
     <row r="237">
-      <c r="A237" s="14" t="s">
+      <c r="A237" s="5" t="s">
         <v>253</v>
       </c>
       <c r="B237" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C237" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D237" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E237" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F237" s="2"/>
       <c r="G237" s="2"/>
@@ -6400,11 +6403,11 @@
       <c r="I237" s="2"/>
     </row>
     <row r="238">
-      <c r="A238" s="5" t="s">
+      <c r="A238" s="14" t="s">
         <v>254</v>
       </c>
       <c r="B238" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C238" s="6" t="s">
         <v>7</v>
@@ -6421,20 +6424,20 @@
       <c r="I238" s="2"/>
     </row>
     <row r="239">
-      <c r="A239" s="14" t="s">
+      <c r="A239" s="5" t="s">
         <v>255</v>
       </c>
       <c r="B239" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C239" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D239" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F239" s="2"/>
       <c r="G239" s="2"/>
@@ -6442,20 +6445,20 @@
       <c r="I239" s="2"/>
     </row>
     <row r="240">
-      <c r="A240" s="5" t="s">
+      <c r="A240" s="14" t="s">
         <v>256</v>
       </c>
       <c r="B240" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C240" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D240" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F240" s="2"/>
       <c r="G240" s="2"/>
@@ -6473,10 +6476,10 @@
         <v>7</v>
       </c>
       <c r="D241" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E241" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F241" s="2"/>
       <c r="G241" s="2"/>
@@ -6494,10 +6497,10 @@
         <v>7</v>
       </c>
       <c r="D242" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E242" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F242" s="2"/>
       <c r="G242" s="2"/>
@@ -6515,10 +6518,10 @@
         <v>7</v>
       </c>
       <c r="D243" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E243" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F243" s="2"/>
       <c r="G243" s="2"/>
@@ -6914,10 +6917,10 @@
         <v>7</v>
       </c>
       <c r="D262" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E262" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F262" s="2"/>
       <c r="G262" s="2"/>
@@ -6935,10 +6938,10 @@
         <v>7</v>
       </c>
       <c r="D263" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E263" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F263" s="2"/>
       <c r="G263" s="2"/>
@@ -7082,10 +7085,10 @@
         <v>7</v>
       </c>
       <c r="D270" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E270" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F270" s="2"/>
       <c r="G270" s="2"/>
@@ -7103,10 +7106,10 @@
         <v>7</v>
       </c>
       <c r="D271" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E271" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F271" s="2"/>
       <c r="G271" s="2"/>
@@ -7163,7 +7166,7 @@
         <v>7</v>
       </c>
       <c r="C274" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D274" s="6" t="s">
         <v>15</v>
@@ -7244,16 +7247,16 @@
         <v>294</v>
       </c>
       <c r="B278" s="6" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="C278" s="6" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="D278" s="6" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="E278" s="6" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="F278" s="2"/>
       <c r="G278" s="2"/>
@@ -7261,11 +7264,21 @@
       <c r="I278" s="2"/>
     </row>
     <row r="279">
-      <c r="A279" s="16"/>
-      <c r="B279" s="17"/>
-      <c r="C279" s="17"/>
-      <c r="D279" s="17"/>
-      <c r="E279" s="17"/>
+      <c r="A279" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B279" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C279" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D279" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E279" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="F279" s="2"/>
       <c r="G279" s="2"/>
       <c r="H279" s="2"/>
@@ -15427,7 +15440,8 @@
     <hyperlink r:id="rId275" ref="A276"/>
     <hyperlink r:id="rId276" ref="A277"/>
     <hyperlink r:id="rId277" ref="A278"/>
+    <hyperlink r:id="rId278" ref="A279"/>
   </hyperlinks>
-  <drawing r:id="rId278"/>
+  <drawing r:id="rId279"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated page data files with new easter egg friday 14 blog post
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -225,10 +225,10 @@
     <t>https://heatlabs.net/blog/easter-egg-friday-14</t>
   </si>
   <si>
+    <t>https://heatlabs.net/blog/easter-egg-friday-15</t>
+  </si>
+  <si>
     <t>NOT NEEDED</t>
-  </si>
-  <si>
-    <t>https://heatlabs.net/blog/easter-egg-friday-15</t>
   </si>
   <si>
     <t>https://heatlabs.net/blog/exploring-animation-and-movement-desync</t>
@@ -1415,7 +1415,7 @@
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
@@ -1519,7 +1519,7 @@
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -2543,10 +2543,10 @@
         <v>69</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>15</v>
@@ -2561,13 +2561,13 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="C55" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>15</v>
@@ -7268,16 +7268,16 @@
         <v>295</v>
       </c>
       <c r="B279" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C279" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D279" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E279" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F279" s="2"/>
       <c r="G279" s="2"/>

</xml_diff>

<commit_message>
updated page data files with new search subdomain
</commit_message>
<xml_diff>
--- a/page-data.xlsx
+++ b/page-data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="298">
   <si>
     <t>-PAGE-</t>
   </si>
@@ -132,6 +132,12 @@
     <t>https://heatlabs.net/agents/udarnik</t>
   </si>
   <si>
+    <t>https://heatlabs.net/ai</t>
+  </si>
+  <si>
+    <t>NOT NEEDED</t>
+  </si>
+  <si>
     <t>https://heatlabs.net/announcements/alpha-1-announcement-1</t>
   </si>
   <si>
@@ -888,6 +894,9 @@
     <t>https://mods.heatlabs.net</t>
   </si>
   <si>
+    <t>https://search.heatlabs.net</t>
+  </si>
+  <si>
     <t>https://social.heatlabs.net</t>
   </si>
   <si>
@@ -898,12 +907,6 @@
   </si>
   <si>
     <t>https://store.heatlabs.net</t>
-  </si>
-  <si>
-    <t>NOT NEEDED</t>
-  </si>
-  <si>
-    <t>https://heatlabs.net/ai</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1421,7 @@
       <c r="G3" s="10">
         <f>COUNTIF(B:B,"PENDING")
 </f>
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H3" s="10">
         <f>COUNTIF(B:B,"NOT INDEXED")
@@ -1522,7 +1525,7 @@
       <c r="G7" s="10">
         <f>COUNTIF(C:C,"PENDING")
 </f>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H7" s="10">
         <f>COUNTIF(C:C,"NOT INDEXED")
@@ -1626,7 +1629,7 @@
       <c r="G11" s="10">
         <f>COUNTIF(D:D,"UNKNOWN")
 </f>
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H11" s="10">
         <f>COUNTIF(D:D,"NOT HTTPS")
@@ -1730,7 +1733,7 @@
       <c r="G15" s="10">
         <f>COUNTIF(E:E,"UNKNOWN")
 </f>
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H15" s="10">
         <f>COUNTIF(E:E,"INVALID")
@@ -1916,16 +1919,16 @@
         <v>39</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1934,10 +1937,10 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>7</v>
@@ -1955,7 +1958,7 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>7</v>
@@ -1976,7 +1979,7 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>7</v>
@@ -1997,13 +2000,13 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>15</v>
@@ -2018,13 +2021,13 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>15</v>
@@ -2039,7 +2042,7 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>7</v>
@@ -2060,7 +2063,7 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>7</v>
@@ -2081,7 +2084,7 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>7</v>
@@ -2102,7 +2105,7 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>7</v>
@@ -2123,13 +2126,13 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>15</v>
@@ -2144,19 +2147,19 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2165,7 +2168,7 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>7</v>
@@ -2186,19 +2189,19 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -2207,7 +2210,7 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>8</v>
@@ -2228,7 +2231,7 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>8</v>
@@ -2249,13 +2252,13 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>15</v>
@@ -2269,11 +2272,11 @@
       <c r="I40" s="2"/>
     </row>
     <row r="41">
-      <c r="A41" s="14" t="s">
-        <v>56</v>
+      <c r="A41" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>7</v>
@@ -2290,8 +2293,8 @@
       <c r="I41" s="2"/>
     </row>
     <row r="42">
-      <c r="A42" s="5" t="s">
-        <v>57</v>
+      <c r="A42" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>7</v>
@@ -2312,13 +2315,13 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>15</v>
@@ -2333,13 +2336,13 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>15</v>
@@ -2354,7 +2357,7 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>8</v>
@@ -2375,7 +2378,7 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>8</v>
@@ -2384,10 +2387,10 @@
         <v>7</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -2396,19 +2399,19 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -2417,7 +2420,7 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>8</v>
@@ -2438,7 +2441,7 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>8</v>
@@ -2459,7 +2462,7 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>8</v>
@@ -2480,7 +2483,7 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>8</v>
@@ -2501,7 +2504,7 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>8</v>
@@ -2522,7 +2525,7 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>8</v>
@@ -2543,7 +2546,7 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>8</v>
@@ -2564,7 +2567,7 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>8</v>
@@ -2585,13 +2588,13 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>15</v>
@@ -2606,7 +2609,7 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>8</v>
@@ -2627,7 +2630,7 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>8</v>
@@ -2647,8 +2650,8 @@
       <c r="I58" s="2"/>
     </row>
     <row r="59">
-      <c r="A59" s="14" t="s">
-        <v>74</v>
+      <c r="A59" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>8</v>
@@ -2657,10 +2660,10 @@
         <v>7</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -2668,8 +2671,8 @@
       <c r="I59" s="2"/>
     </row>
     <row r="60">
-      <c r="A60" s="5" t="s">
-        <v>75</v>
+      <c r="A60" s="14" t="s">
+        <v>76</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>8</v>
@@ -2690,19 +2693,19 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -2710,8 +2713,8 @@
       <c r="I61" s="2"/>
     </row>
     <row r="62">
-      <c r="A62" s="14" t="s">
-        <v>77</v>
+      <c r="A62" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>8</v>
@@ -2731,8 +2734,8 @@
       <c r="I62" s="2"/>
     </row>
     <row r="63">
-      <c r="A63" s="5" t="s">
-        <v>78</v>
+      <c r="A63" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>8</v>
@@ -2753,7 +2756,7 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>8</v>
@@ -2774,13 +2777,13 @@
     </row>
     <row r="65">
       <c r="A65" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>15</v>
@@ -2795,19 +2798,19 @@
     </row>
     <row r="66">
       <c r="A66" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -2816,19 +2819,19 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -2837,10 +2840,10 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>7</v>
@@ -2858,7 +2861,7 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>8</v>
@@ -2879,13 +2882,13 @@
     </row>
     <row r="70">
       <c r="A70" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>15</v>
@@ -2900,7 +2903,7 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>8</v>
@@ -2921,13 +2924,13 @@
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>15</v>
@@ -2942,13 +2945,13 @@
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>15</v>
@@ -2963,13 +2966,13 @@
     </row>
     <row r="74">
       <c r="A74" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>15</v>
@@ -2984,13 +2987,13 @@
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>15</v>
@@ -3005,13 +3008,13 @@
     </row>
     <row r="76">
       <c r="A76" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>15</v>
@@ -3026,10 +3029,10 @@
     </row>
     <row r="77">
       <c r="A77" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>7</v>
@@ -3047,10 +3050,10 @@
     </row>
     <row r="78">
       <c r="A78" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>7</v>
@@ -3068,7 +3071,7 @@
     </row>
     <row r="79">
       <c r="A79" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>8</v>
@@ -3089,7 +3092,7 @@
     </row>
     <row r="80">
       <c r="A80" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>8</v>
@@ -3110,7 +3113,7 @@
     </row>
     <row r="81">
       <c r="A81" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>8</v>
@@ -3131,13 +3134,13 @@
     </row>
     <row r="82">
       <c r="A82" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>15</v>
@@ -3151,8 +3154,8 @@
       <c r="I82" s="2"/>
     </row>
     <row r="83">
-      <c r="A83" s="14" t="s">
-        <v>98</v>
+      <c r="A83" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>8</v>
@@ -3172,20 +3175,20 @@
       <c r="I83" s="2"/>
     </row>
     <row r="84">
-      <c r="A84" s="5" t="s">
-        <v>99</v>
+      <c r="A84" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
@@ -3194,7 +3197,7 @@
     </row>
     <row r="85">
       <c r="A85" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>7</v>
@@ -3215,7 +3218,7 @@
     </row>
     <row r="86">
       <c r="A86" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>7</v>
@@ -3236,7 +3239,7 @@
     </row>
     <row r="87">
       <c r="A87" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>7</v>
@@ -3245,10 +3248,10 @@
         <v>7</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -3257,7 +3260,7 @@
     </row>
     <row r="88">
       <c r="A88" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>7</v>
@@ -3278,7 +3281,7 @@
     </row>
     <row r="89">
       <c r="A89" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>7</v>
@@ -3299,7 +3302,7 @@
     </row>
     <row r="90">
       <c r="A90" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>7</v>
@@ -3320,7 +3323,7 @@
     </row>
     <row r="91">
       <c r="A91" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>7</v>
@@ -3341,7 +3344,7 @@
     </row>
     <row r="92">
       <c r="A92" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>7</v>
@@ -3350,10 +3353,10 @@
         <v>7</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
@@ -3362,7 +3365,7 @@
     </row>
     <row r="93">
       <c r="A93" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>7</v>
@@ -3371,10 +3374,10 @@
         <v>7</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
@@ -3382,14 +3385,14 @@
       <c r="I93" s="2"/>
     </row>
     <row r="94">
-      <c r="A94" s="14" t="s">
-        <v>109</v>
+      <c r="A94" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>15</v>
@@ -3403,20 +3406,20 @@
       <c r="I94" s="2"/>
     </row>
     <row r="95">
-      <c r="A95" s="5" t="s">
-        <v>110</v>
+      <c r="A95" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -3425,19 +3428,19 @@
     </row>
     <row r="96">
       <c r="A96" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
@@ -3446,19 +3449,19 @@
     </row>
     <row r="97">
       <c r="A97" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
@@ -3467,19 +3470,19 @@
     </row>
     <row r="98">
       <c r="A98" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
@@ -3488,19 +3491,19 @@
     </row>
     <row r="99">
       <c r="A99" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -3509,10 +3512,10 @@
     </row>
     <row r="100">
       <c r="A100" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>7</v>
@@ -3530,7 +3533,7 @@
     </row>
     <row r="101">
       <c r="A101" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>7</v>
@@ -3539,10 +3542,10 @@
         <v>7</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
@@ -3551,7 +3554,7 @@
     </row>
     <row r="102">
       <c r="A102" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>7</v>
@@ -3560,10 +3563,10 @@
         <v>7</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
@@ -3572,19 +3575,19 @@
     </row>
     <row r="103">
       <c r="A103" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
@@ -3593,10 +3596,10 @@
     </row>
     <row r="104">
       <c r="A104" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>7</v>
@@ -3614,10 +3617,10 @@
     </row>
     <row r="105">
       <c r="A105" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>7</v>
@@ -3635,13 +3638,13 @@
     </row>
     <row r="106">
       <c r="A106" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>15</v>
@@ -3656,13 +3659,13 @@
     </row>
     <row r="107">
       <c r="A107" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>15</v>
@@ -3677,7 +3680,7 @@
     </row>
     <row r="108">
       <c r="A108" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>7</v>
@@ -3698,7 +3701,7 @@
     </row>
     <row r="109">
       <c r="A109" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>7</v>
@@ -3719,13 +3722,13 @@
     </row>
     <row r="110">
       <c r="A110" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>15</v>
@@ -3740,13 +3743,13 @@
     </row>
     <row r="111">
       <c r="A111" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>15</v>
@@ -3761,7 +3764,7 @@
     </row>
     <row r="112">
       <c r="A112" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>7</v>
@@ -3782,7 +3785,7 @@
     </row>
     <row r="113">
       <c r="A113" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>7</v>
@@ -3803,7 +3806,7 @@
     </row>
     <row r="114">
       <c r="A114" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B114" s="6" t="s">
         <v>7</v>
@@ -3824,7 +3827,7 @@
     </row>
     <row r="115">
       <c r="A115" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>7</v>
@@ -3845,7 +3848,7 @@
     </row>
     <row r="116">
       <c r="A116" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>7</v>
@@ -3866,7 +3869,7 @@
     </row>
     <row r="117">
       <c r="A117" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>7</v>
@@ -3887,7 +3890,7 @@
     </row>
     <row r="118">
       <c r="A118" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>7</v>
@@ -3908,7 +3911,7 @@
     </row>
     <row r="119">
       <c r="A119" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B119" s="6" t="s">
         <v>7</v>
@@ -3929,7 +3932,7 @@
     </row>
     <row r="120">
       <c r="A120" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>7</v>
@@ -3950,7 +3953,7 @@
     </row>
     <row r="121">
       <c r="A121" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>7</v>
@@ -3971,7 +3974,7 @@
     </row>
     <row r="122">
       <c r="A122" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>7</v>
@@ -3992,7 +3995,7 @@
     </row>
     <row r="123">
       <c r="A123" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>7</v>
@@ -4013,7 +4016,7 @@
     </row>
     <row r="124">
       <c r="A124" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>7</v>
@@ -4034,7 +4037,7 @@
     </row>
     <row r="125">
       <c r="A125" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>7</v>
@@ -4055,7 +4058,7 @@
     </row>
     <row r="126">
       <c r="A126" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>7</v>
@@ -4076,10 +4079,10 @@
     </row>
     <row r="127">
       <c r="A127" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C127" s="6" t="s">
         <v>7</v>
@@ -4097,7 +4100,7 @@
     </row>
     <row r="128">
       <c r="A128" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>8</v>
@@ -4118,7 +4121,7 @@
     </row>
     <row r="129">
       <c r="A129" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>8</v>
@@ -4139,10 +4142,10 @@
     </row>
     <row r="130">
       <c r="A130" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C130" s="6" t="s">
         <v>7</v>
@@ -4160,10 +4163,10 @@
     </row>
     <row r="131">
       <c r="A131" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C131" s="6" t="s">
         <v>7</v>
@@ -4181,10 +4184,10 @@
     </row>
     <row r="132">
       <c r="A132" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C132" s="6" t="s">
         <v>7</v>
@@ -4202,7 +4205,7 @@
     </row>
     <row r="133">
       <c r="A133" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>7</v>
@@ -4223,7 +4226,7 @@
     </row>
     <row r="134">
       <c r="A134" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>7</v>
@@ -4244,13 +4247,13 @@
     </row>
     <row r="135">
       <c r="A135" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>15</v>
@@ -4265,13 +4268,13 @@
     </row>
     <row r="136">
       <c r="A136" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D136" s="6" t="s">
         <v>15</v>
@@ -4286,7 +4289,7 @@
     </row>
     <row r="137">
       <c r="A137" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>7</v>
@@ -4307,13 +4310,13 @@
     </row>
     <row r="138">
       <c r="A138" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D138" s="6" t="s">
         <v>15</v>
@@ -4328,13 +4331,13 @@
     </row>
     <row r="139">
       <c r="A139" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D139" s="6" t="s">
         <v>15</v>
@@ -4349,7 +4352,7 @@
     </row>
     <row r="140">
       <c r="A140" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>7</v>
@@ -4370,7 +4373,7 @@
     </row>
     <row r="141">
       <c r="A141" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B141" s="6" t="s">
         <v>7</v>
@@ -4379,10 +4382,10 @@
         <v>7</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
@@ -4391,7 +4394,7 @@
     </row>
     <row r="142">
       <c r="A142" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B142" s="6" t="s">
         <v>7</v>
@@ -4400,10 +4403,10 @@
         <v>7</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
@@ -4412,10 +4415,10 @@
     </row>
     <row r="143">
       <c r="A143" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>7</v>
@@ -4433,10 +4436,10 @@
     </row>
     <row r="144">
       <c r="A144" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C144" s="6" t="s">
         <v>7</v>
@@ -4454,7 +4457,7 @@
     </row>
     <row r="145">
       <c r="A145" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B145" s="6" t="s">
         <v>7</v>
@@ -4475,7 +4478,7 @@
     </row>
     <row r="146">
       <c r="A146" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B146" s="6" t="s">
         <v>7</v>
@@ -4496,7 +4499,7 @@
     </row>
     <row r="147">
       <c r="A147" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B147" s="6" t="s">
         <v>7</v>
@@ -4517,7 +4520,7 @@
     </row>
     <row r="148">
       <c r="A148" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B148" s="6" t="s">
         <v>7</v>
@@ -4538,13 +4541,13 @@
     </row>
     <row r="149">
       <c r="A149" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B149" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>15</v>
@@ -4559,13 +4562,13 @@
     </row>
     <row r="150">
       <c r="A150" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B150" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D150" s="6" t="s">
         <v>15</v>
@@ -4580,7 +4583,7 @@
     </row>
     <row r="151">
       <c r="A151" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B151" s="6" t="s">
         <v>7</v>
@@ -4601,7 +4604,7 @@
     </row>
     <row r="152">
       <c r="A152" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B152" s="6" t="s">
         <v>7</v>
@@ -4622,7 +4625,7 @@
     </row>
     <row r="153">
       <c r="A153" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B153" s="6" t="s">
         <v>7</v>
@@ -4643,7 +4646,7 @@
     </row>
     <row r="154">
       <c r="A154" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B154" s="6" t="s">
         <v>7</v>
@@ -4664,13 +4667,13 @@
     </row>
     <row r="155">
       <c r="A155" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B155" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D155" s="6" t="s">
         <v>15</v>
@@ -4685,7 +4688,7 @@
     </row>
     <row r="156">
       <c r="A156" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B156" s="6" t="s">
         <v>7</v>
@@ -4706,13 +4709,13 @@
     </row>
     <row r="157">
       <c r="A157" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B157" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D157" s="6" t="s">
         <v>15</v>
@@ -4727,7 +4730,7 @@
     </row>
     <row r="158">
       <c r="A158" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B158" s="6" t="s">
         <v>7</v>
@@ -4748,7 +4751,7 @@
     </row>
     <row r="159">
       <c r="A159" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B159" s="6" t="s">
         <v>7</v>
@@ -4769,7 +4772,7 @@
     </row>
     <row r="160">
       <c r="A160" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B160" s="6" t="s">
         <v>7</v>
@@ -4790,13 +4793,13 @@
     </row>
     <row r="161">
       <c r="A161" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B161" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>15</v>
@@ -4811,13 +4814,13 @@
     </row>
     <row r="162">
       <c r="A162" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B162" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D162" s="6" t="s">
         <v>15</v>
@@ -4832,7 +4835,7 @@
     </row>
     <row r="163">
       <c r="A163" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B163" s="6" t="s">
         <v>7</v>
@@ -4853,7 +4856,7 @@
     </row>
     <row r="164">
       <c r="A164" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B164" s="6" t="s">
         <v>7</v>
@@ -4874,7 +4877,7 @@
     </row>
     <row r="165">
       <c r="A165" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B165" s="6" t="s">
         <v>7</v>
@@ -4895,7 +4898,7 @@
     </row>
     <row r="166">
       <c r="A166" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B166" s="6" t="s">
         <v>7</v>
@@ -4916,7 +4919,7 @@
     </row>
     <row r="167">
       <c r="A167" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B167" s="6" t="s">
         <v>7</v>
@@ -4937,13 +4940,13 @@
     </row>
     <row r="168">
       <c r="A168" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B168" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D168" s="6" t="s">
         <v>15</v>
@@ -4958,13 +4961,13 @@
     </row>
     <row r="169">
       <c r="A169" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B169" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D169" s="6" t="s">
         <v>15</v>
@@ -4979,7 +4982,7 @@
     </row>
     <row r="170">
       <c r="A170" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B170" s="6" t="s">
         <v>7</v>
@@ -5000,7 +5003,7 @@
     </row>
     <row r="171">
       <c r="A171" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B171" s="6" t="s">
         <v>7</v>
@@ -5021,7 +5024,7 @@
     </row>
     <row r="172">
       <c r="A172" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B172" s="6" t="s">
         <v>7</v>
@@ -5042,7 +5045,7 @@
     </row>
     <row r="173">
       <c r="A173" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B173" s="6" t="s">
         <v>7</v>
@@ -5063,13 +5066,13 @@
     </row>
     <row r="174">
       <c r="A174" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D174" s="6" t="s">
         <v>15</v>
@@ -5084,13 +5087,13 @@
     </row>
     <row r="175">
       <c r="A175" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D175" s="6" t="s">
         <v>15</v>
@@ -5105,13 +5108,13 @@
     </row>
     <row r="176">
       <c r="A176" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D176" s="6" t="s">
         <v>15</v>
@@ -5126,10 +5129,10 @@
     </row>
     <row r="177">
       <c r="A177" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C177" s="6" t="s">
         <v>8</v>
@@ -5147,7 +5150,7 @@
     </row>
     <row r="178">
       <c r="A178" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B178" s="6" t="s">
         <v>7</v>
@@ -5168,7 +5171,7 @@
     </row>
     <row r="179">
       <c r="A179" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B179" s="6" t="s">
         <v>7</v>
@@ -5189,10 +5192,10 @@
     </row>
     <row r="180">
       <c r="A180" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C180" s="6" t="s">
         <v>8</v>
@@ -5210,13 +5213,13 @@
     </row>
     <row r="181">
       <c r="A181" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C181" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D181" s="6" t="s">
         <v>15</v>
@@ -5231,10 +5234,10 @@
     </row>
     <row r="182">
       <c r="A182" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C182" s="6" t="s">
         <v>7</v>
@@ -5252,13 +5255,13 @@
     </row>
     <row r="183">
       <c r="A183" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B183" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D183" s="6" t="s">
         <v>15</v>
@@ -5273,13 +5276,13 @@
     </row>
     <row r="184">
       <c r="A184" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B184" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C184" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D184" s="6" t="s">
         <v>15</v>
@@ -5294,10 +5297,10 @@
     </row>
     <row r="185">
       <c r="A185" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>7</v>
@@ -5315,13 +5318,13 @@
     </row>
     <row r="186">
       <c r="A186" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D186" s="6" t="s">
         <v>15</v>
@@ -5336,13 +5339,13 @@
     </row>
     <row r="187">
       <c r="A187" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C187" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D187" s="6" t="s">
         <v>15</v>
@@ -5357,7 +5360,7 @@
     </row>
     <row r="188">
       <c r="A188" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B188" s="6" t="s">
         <v>7</v>
@@ -5378,7 +5381,7 @@
     </row>
     <row r="189">
       <c r="A189" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B189" s="6" t="s">
         <v>7</v>
@@ -5399,7 +5402,7 @@
     </row>
     <row r="190">
       <c r="A190" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B190" s="6" t="s">
         <v>7</v>
@@ -5420,7 +5423,7 @@
     </row>
     <row r="191">
       <c r="A191" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B191" s="6" t="s">
         <v>7</v>
@@ -5441,7 +5444,7 @@
     </row>
     <row r="192">
       <c r="A192" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B192" s="6" t="s">
         <v>7</v>
@@ -5462,7 +5465,7 @@
     </row>
     <row r="193">
       <c r="A193" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B193" s="6" t="s">
         <v>7</v>
@@ -5483,13 +5486,13 @@
     </row>
     <row r="194">
       <c r="A194" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C194" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D194" s="6" t="s">
         <v>15</v>
@@ -5504,7 +5507,7 @@
     </row>
     <row r="195">
       <c r="A195" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B195" s="6" t="s">
         <v>8</v>
@@ -5525,7 +5528,7 @@
     </row>
     <row r="196">
       <c r="A196" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B196" s="6" t="s">
         <v>8</v>
@@ -5546,7 +5549,7 @@
     </row>
     <row r="197">
       <c r="A197" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B197" s="6" t="s">
         <v>8</v>
@@ -5567,10 +5570,10 @@
     </row>
     <row r="198">
       <c r="A198" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B198" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C198" s="6" t="s">
         <v>8</v>
@@ -5588,7 +5591,7 @@
     </row>
     <row r="199">
       <c r="A199" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B199" s="6" t="s">
         <v>7</v>
@@ -5609,13 +5612,13 @@
     </row>
     <row r="200">
       <c r="A200" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B200" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D200" s="6" t="s">
         <v>15</v>
@@ -5630,13 +5633,13 @@
     </row>
     <row r="201">
       <c r="A201" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C201" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D201" s="6" t="s">
         <v>15</v>
@@ -5651,7 +5654,7 @@
     </row>
     <row r="202">
       <c r="A202" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B202" s="6" t="s">
         <v>8</v>
@@ -5672,7 +5675,7 @@
     </row>
     <row r="203">
       <c r="A203" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B203" s="6" t="s">
         <v>8</v>
@@ -5693,7 +5696,7 @@
     </row>
     <row r="204">
       <c r="A204" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B204" s="6" t="s">
         <v>8</v>
@@ -5714,10 +5717,10 @@
     </row>
     <row r="205">
       <c r="A205" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C205" s="6" t="s">
         <v>8</v>
@@ -5735,13 +5738,13 @@
     </row>
     <row r="206">
       <c r="A206" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B206" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C206" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D206" s="6" t="s">
         <v>15</v>
@@ -5756,10 +5759,10 @@
     </row>
     <row r="207">
       <c r="A207" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C207" s="6" t="s">
         <v>7</v>
@@ -5777,7 +5780,7 @@
     </row>
     <row r="208">
       <c r="A208" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B208" s="6" t="s">
         <v>8</v>
@@ -5798,19 +5801,19 @@
     </row>
     <row r="209">
       <c r="A209" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C209" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D209" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E209" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F209" s="2"/>
       <c r="G209" s="2"/>
@@ -5819,19 +5822,19 @@
     </row>
     <row r="210">
       <c r="A210" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C210" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D210" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E210" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F210" s="2"/>
       <c r="G210" s="2"/>
@@ -5840,7 +5843,7 @@
     </row>
     <row r="211">
       <c r="A211" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B211" s="6" t="s">
         <v>8</v>
@@ -5861,7 +5864,7 @@
     </row>
     <row r="212">
       <c r="A212" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B212" s="6" t="s">
         <v>8</v>
@@ -5882,13 +5885,13 @@
     </row>
     <row r="213">
       <c r="A213" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B213" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C213" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D213" s="6" t="s">
         <v>15</v>
@@ -5903,7 +5906,7 @@
     </row>
     <row r="214">
       <c r="A214" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B214" s="6" t="s">
         <v>8</v>
@@ -5924,13 +5927,13 @@
     </row>
     <row r="215">
       <c r="A215" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B215" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C215" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D215" s="6" t="s">
         <v>15</v>
@@ -5945,10 +5948,10 @@
     </row>
     <row r="216">
       <c r="A216" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C216" s="6" t="s">
         <v>7</v>
@@ -5966,19 +5969,19 @@
     </row>
     <row r="217">
       <c r="A217" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C217" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D217" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E217" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F217" s="2"/>
       <c r="G217" s="2"/>
@@ -5987,10 +5990,10 @@
     </row>
     <row r="218">
       <c r="A218" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>7</v>
@@ -6008,7 +6011,7 @@
     </row>
     <row r="219">
       <c r="A219" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B219" s="6" t="s">
         <v>7</v>
@@ -6017,10 +6020,10 @@
         <v>7</v>
       </c>
       <c r="D219" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E219" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F219" s="2"/>
       <c r="G219" s="2"/>
@@ -6029,7 +6032,7 @@
     </row>
     <row r="220">
       <c r="A220" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B220" s="6" t="s">
         <v>7</v>
@@ -6049,11 +6052,11 @@
       <c r="I220" s="2"/>
     </row>
     <row r="221">
-      <c r="A221" s="14" t="s">
-        <v>236</v>
+      <c r="A221" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C221" s="6" t="s">
         <v>7</v>
@@ -6070,11 +6073,11 @@
       <c r="I221" s="2"/>
     </row>
     <row r="222">
-      <c r="A222" s="5" t="s">
-        <v>237</v>
+      <c r="A222" s="14" t="s">
+        <v>238</v>
       </c>
       <c r="B222" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C222" s="6" t="s">
         <v>7</v>
@@ -6092,7 +6095,7 @@
     </row>
     <row r="223">
       <c r="A223" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B223" s="6" t="s">
         <v>7</v>
@@ -6113,7 +6116,7 @@
     </row>
     <row r="224">
       <c r="A224" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B224" s="6" t="s">
         <v>7</v>
@@ -6134,7 +6137,7 @@
     </row>
     <row r="225">
       <c r="A225" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B225" s="6" t="s">
         <v>7</v>
@@ -6155,7 +6158,7 @@
     </row>
     <row r="226">
       <c r="A226" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B226" s="6" t="s">
         <v>7</v>
@@ -6175,14 +6178,14 @@
       <c r="I226" s="2"/>
     </row>
     <row r="227">
-      <c r="A227" s="14" t="s">
-        <v>242</v>
+      <c r="A227" s="5" t="s">
+        <v>243</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C227" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D227" s="6" t="s">
         <v>15</v>
@@ -6196,14 +6199,14 @@
       <c r="I227" s="2"/>
     </row>
     <row r="228">
-      <c r="A228" s="5" t="s">
-        <v>243</v>
+      <c r="A228" s="14" t="s">
+        <v>244</v>
       </c>
       <c r="B228" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D228" s="6" t="s">
         <v>15</v>
@@ -6218,10 +6221,10 @@
     </row>
     <row r="229">
       <c r="A229" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C229" s="6" t="s">
         <v>7</v>
@@ -6239,19 +6242,19 @@
     </row>
     <row r="230">
       <c r="A230" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B230" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C230" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D230" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F230" s="2"/>
       <c r="G230" s="2"/>
@@ -6260,19 +6263,19 @@
     </row>
     <row r="231">
       <c r="A231" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C231" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D231" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E231" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F231" s="2"/>
       <c r="G231" s="2"/>
@@ -6281,10 +6284,10 @@
     </row>
     <row r="232">
       <c r="A232" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B232" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C232" s="6" t="s">
         <v>7</v>
@@ -6302,7 +6305,7 @@
     </row>
     <row r="233">
       <c r="A233" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B233" s="6" t="s">
         <v>7</v>
@@ -6323,19 +6326,19 @@
     </row>
     <row r="234">
       <c r="A234" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B234" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C234" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D234" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F234" s="2"/>
       <c r="G234" s="2"/>
@@ -6344,10 +6347,10 @@
     </row>
     <row r="235">
       <c r="A235" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B235" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C235" s="6" t="s">
         <v>7</v>
@@ -6365,7 +6368,7 @@
     </row>
     <row r="236">
       <c r="A236" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B236" s="6" t="s">
         <v>7</v>
@@ -6374,10 +6377,10 @@
         <v>7</v>
       </c>
       <c r="D236" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E236" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F236" s="2"/>
       <c r="G236" s="2"/>
@@ -6386,7 +6389,7 @@
     </row>
     <row r="237">
       <c r="A237" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B237" s="6" t="s">
         <v>7</v>
@@ -6406,20 +6409,20 @@
       <c r="I237" s="2"/>
     </row>
     <row r="238">
-      <c r="A238" s="14" t="s">
-        <v>253</v>
+      <c r="A238" s="5" t="s">
+        <v>254</v>
       </c>
       <c r="B238" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C238" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D238" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E238" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F238" s="2"/>
       <c r="G238" s="2"/>
@@ -6427,11 +6430,11 @@
       <c r="I238" s="2"/>
     </row>
     <row r="239">
-      <c r="A239" s="5" t="s">
-        <v>254</v>
+      <c r="A239" s="14" t="s">
+        <v>255</v>
       </c>
       <c r="B239" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C239" s="6" t="s">
         <v>7</v>
@@ -6448,20 +6451,20 @@
       <c r="I239" s="2"/>
     </row>
     <row r="240">
-      <c r="A240" s="14" t="s">
-        <v>255</v>
+      <c r="A240" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="B240" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C240" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D240" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F240" s="2"/>
       <c r="G240" s="2"/>
@@ -6469,20 +6472,20 @@
       <c r="I240" s="2"/>
     </row>
     <row r="241">
-      <c r="A241" s="5" t="s">
-        <v>256</v>
+      <c r="A241" s="14" t="s">
+        <v>257</v>
       </c>
       <c r="B241" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C241" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D241" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E241" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F241" s="2"/>
       <c r="G241" s="2"/>
@@ -6491,7 +6494,7 @@
     </row>
     <row r="242">
       <c r="A242" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B242" s="6" t="s">
         <v>7</v>
@@ -6500,10 +6503,10 @@
         <v>7</v>
       </c>
       <c r="D242" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E242" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F242" s="2"/>
       <c r="G242" s="2"/>
@@ -6512,7 +6515,7 @@
     </row>
     <row r="243">
       <c r="A243" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B243" s="6" t="s">
         <v>7</v>
@@ -6521,10 +6524,10 @@
         <v>7</v>
       </c>
       <c r="D243" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E243" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F243" s="2"/>
       <c r="G243" s="2"/>
@@ -6533,7 +6536,7 @@
     </row>
     <row r="244">
       <c r="A244" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B244" s="6" t="s">
         <v>7</v>
@@ -6542,10 +6545,10 @@
         <v>7</v>
       </c>
       <c r="D244" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F244" s="2"/>
       <c r="G244" s="2"/>
@@ -6554,7 +6557,7 @@
     </row>
     <row r="245">
       <c r="A245" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B245" s="6" t="s">
         <v>7</v>
@@ -6575,7 +6578,7 @@
     </row>
     <row r="246">
       <c r="A246" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B246" s="6" t="s">
         <v>7</v>
@@ -6596,7 +6599,7 @@
     </row>
     <row r="247">
       <c r="A247" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B247" s="6" t="s">
         <v>7</v>
@@ -6617,7 +6620,7 @@
     </row>
     <row r="248">
       <c r="A248" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B248" s="6" t="s">
         <v>7</v>
@@ -6638,7 +6641,7 @@
     </row>
     <row r="249">
       <c r="A249" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B249" s="6" t="s">
         <v>7</v>
@@ -6659,7 +6662,7 @@
     </row>
     <row r="250">
       <c r="A250" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B250" s="6" t="s">
         <v>7</v>
@@ -6680,7 +6683,7 @@
     </row>
     <row r="251">
       <c r="A251" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B251" s="6" t="s">
         <v>7</v>
@@ -6701,7 +6704,7 @@
     </row>
     <row r="252">
       <c r="A252" s="15" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B252" s="6" t="s">
         <v>7</v>
@@ -6722,7 +6725,7 @@
     </row>
     <row r="253">
       <c r="A253" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B253" s="6" t="s">
         <v>7</v>
@@ -6743,7 +6746,7 @@
     </row>
     <row r="254">
       <c r="A254" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B254" s="6" t="s">
         <v>7</v>
@@ -6764,7 +6767,7 @@
     </row>
     <row r="255">
       <c r="A255" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B255" s="6" t="s">
         <v>7</v>
@@ -6785,7 +6788,7 @@
     </row>
     <row r="256">
       <c r="A256" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B256" s="6" t="s">
         <v>7</v>
@@ -6806,7 +6809,7 @@
     </row>
     <row r="257">
       <c r="A257" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B257" s="6" t="s">
         <v>7</v>
@@ -6827,7 +6830,7 @@
     </row>
     <row r="258">
       <c r="A258" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B258" s="6" t="s">
         <v>7</v>
@@ -6848,7 +6851,7 @@
     </row>
     <row r="259">
       <c r="A259" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B259" s="6" t="s">
         <v>7</v>
@@ -6869,7 +6872,7 @@
     </row>
     <row r="260">
       <c r="A260" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B260" s="6" t="s">
         <v>7</v>
@@ -6890,7 +6893,7 @@
     </row>
     <row r="261">
       <c r="A261" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B261" s="6" t="s">
         <v>7</v>
@@ -6911,7 +6914,7 @@
     </row>
     <row r="262">
       <c r="A262" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B262" s="6" t="s">
         <v>7</v>
@@ -6932,7 +6935,7 @@
     </row>
     <row r="263">
       <c r="A263" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B263" s="6" t="s">
         <v>7</v>
@@ -6941,10 +6944,10 @@
         <v>7</v>
       </c>
       <c r="D263" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E263" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F263" s="2"/>
       <c r="G263" s="2"/>
@@ -6953,7 +6956,7 @@
     </row>
     <row r="264">
       <c r="A264" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B264" s="6" t="s">
         <v>7</v>
@@ -6962,10 +6965,10 @@
         <v>7</v>
       </c>
       <c r="D264" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E264" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F264" s="2"/>
       <c r="G264" s="2"/>
@@ -6974,7 +6977,7 @@
     </row>
     <row r="265">
       <c r="A265" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B265" s="6" t="s">
         <v>7</v>
@@ -6995,7 +6998,7 @@
     </row>
     <row r="266">
       <c r="A266" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B266" s="6" t="s">
         <v>7</v>
@@ -7016,7 +7019,7 @@
     </row>
     <row r="267">
       <c r="A267" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B267" s="6" t="s">
         <v>7</v>
@@ -7037,7 +7040,7 @@
     </row>
     <row r="268">
       <c r="A268" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B268" s="6" t="s">
         <v>7</v>
@@ -7058,7 +7061,7 @@
     </row>
     <row r="269">
       <c r="A269" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B269" s="6" t="s">
         <v>7</v>
@@ -7079,7 +7082,7 @@
     </row>
     <row r="270">
       <c r="A270" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B270" s="6" t="s">
         <v>7</v>
@@ -7100,7 +7103,7 @@
     </row>
     <row r="271">
       <c r="A271" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B271" s="6" t="s">
         <v>7</v>
@@ -7109,10 +7112,10 @@
         <v>7</v>
       </c>
       <c r="D271" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E271" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F271" s="2"/>
       <c r="G271" s="2"/>
@@ -7121,7 +7124,7 @@
     </row>
     <row r="272">
       <c r="A272" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B272" s="6" t="s">
         <v>7</v>
@@ -7130,10 +7133,10 @@
         <v>7</v>
       </c>
       <c r="D272" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E272" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F272" s="2"/>
       <c r="G272" s="2"/>
@@ -7142,7 +7145,7 @@
     </row>
     <row r="273">
       <c r="A273" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B273" s="6" t="s">
         <v>7</v>
@@ -7163,7 +7166,7 @@
     </row>
     <row r="274">
       <c r="A274" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B274" s="6" t="s">
         <v>7</v>
@@ -7184,13 +7187,13 @@
     </row>
     <row r="275">
       <c r="A275" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B275" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C275" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D275" s="6" t="s">
         <v>15</v>
@@ -7205,7 +7208,7 @@
     </row>
     <row r="276">
       <c r="A276" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B276" s="6" t="s">
         <v>7</v>
@@ -7226,10 +7229,10 @@
     </row>
     <row r="277">
       <c r="A277" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B277" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C277" s="6" t="s">
         <v>8</v>
@@ -7247,7 +7250,7 @@
     </row>
     <row r="278">
       <c r="A278" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B278" s="6" t="s">
         <v>7</v>
@@ -7268,19 +7271,19 @@
     </row>
     <row r="279">
       <c r="A279" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B279" s="6" t="s">
-        <v>295</v>
+        <v>7</v>
       </c>
       <c r="C279" s="6" t="s">
-        <v>295</v>
+        <v>8</v>
       </c>
       <c r="D279" s="6" t="s">
-        <v>295</v>
+        <v>15</v>
       </c>
       <c r="E279" s="6" t="s">
-        <v>295</v>
+        <v>15</v>
       </c>
       <c r="F279" s="2"/>
       <c r="G279" s="2"/>
@@ -7292,16 +7295,16 @@
         <v>296</v>
       </c>
       <c r="B280" s="6" t="s">
-        <v>295</v>
+        <v>7</v>
       </c>
       <c r="C280" s="6" t="s">
-        <v>295</v>
+        <v>8</v>
       </c>
       <c r="D280" s="6" t="s">
-        <v>295</v>
+        <v>15</v>
       </c>
       <c r="E280" s="6" t="s">
-        <v>295</v>
+        <v>15</v>
       </c>
       <c r="F280" s="2"/>
       <c r="G280" s="2"/>
@@ -7309,11 +7312,21 @@
       <c r="I280" s="2"/>
     </row>
     <row r="281">
-      <c r="A281" s="16"/>
-      <c r="B281" s="17"/>
-      <c r="C281" s="17"/>
-      <c r="D281" s="17"/>
-      <c r="E281" s="17"/>
+      <c r="A281" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B281" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C281" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D281" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E281" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="F281" s="2"/>
       <c r="G281" s="2"/>
       <c r="H281" s="2"/>
@@ -15455,7 +15468,8 @@
     <hyperlink r:id="rId277" ref="A278"/>
     <hyperlink r:id="rId278" ref="A279"/>
     <hyperlink r:id="rId279" ref="A280"/>
+    <hyperlink r:id="rId280" ref="A281"/>
   </hyperlinks>
-  <drawing r:id="rId280"/>
+  <drawing r:id="rId281"/>
 </worksheet>
 </file>
</xml_diff>